<commit_message>
Update automatico via Actualizar 05-12-2020 08-20-33
</commit_message>
<xml_diff>
--- a/datacovidgt/Casos GT v1.xlsx
+++ b/datacovidgt/Casos GT v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID GT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="758" documentId="8_{9F1230D5-64C1-4EE0-9758-3A2331A06A47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DDF94715-FC45-4111-86BE-1B29A8B40045}"/>
+  <xr:revisionPtr revIDLastSave="771" documentId="8_{9F1230D5-64C1-4EE0-9758-3A2331A06A47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{688801C5-246C-413F-B4BA-9902C64FC30F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Nuevos " sheetId="6" r:id="rId1"/>
@@ -6970,8 +6970,8 @@
   </sheetPr>
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -7065,57 +7065,57 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="49">
-        <v>43958</v>
+        <v>43962</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
       </c>
       <c r="C13">
-        <v>638</v>
+        <v>679</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="49">
-        <v>43958</v>
+        <v>43962</v>
       </c>
       <c r="B14" t="s">
         <v>15</v>
       </c>
       <c r="C14">
-        <v>137</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="49">
-        <v>43958</v>
+        <v>43962</v>
       </c>
       <c r="B15" t="s">
         <v>16</v>
       </c>
       <c r="C15">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="49">
-        <v>43958</v>
+        <v>43962</v>
       </c>
       <c r="B16" t="s">
         <v>17</v>
       </c>
       <c r="C16">
-        <v>76</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="49">
-        <v>43958</v>
+        <v>43962</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
       </c>
       <c r="C17">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -57232,8 +57232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="B2:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-12-2020 17-21-46
</commit_message>
<xml_diff>
--- a/datacovidgt/Casos GT v1.xlsx
+++ b/datacovidgt/Casos GT v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22904"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22907"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID GT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="771" documentId="8_{9F1230D5-64C1-4EE0-9758-3A2331A06A47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{688801C5-246C-413F-B4BA-9902C64FC30F}"/>
+  <xr:revisionPtr revIDLastSave="1000" documentId="8_{9F1230D5-64C1-4EE0-9758-3A2331A06A47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FFC54259-E57A-457D-8230-461701B5DCA2}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Nuevos " sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5219" uniqueCount="910">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5355" uniqueCount="910">
   <si>
     <t>DIA</t>
   </si>
@@ -3504,18 +3504,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3529,6 +3517,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -3536,7 +3536,7 @@
     <cellStyle name="Millares" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="38">
+  <dxfs count="55">
     <dxf>
       <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
@@ -3803,6 +3803,57 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="21" formatCode="d\-mmm"/>
@@ -4140,38 +4191,158 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C7124E47-3D2D-419B-8945-4E2B1598725E}" name="NACIONAL" displayName="NACIONAL" ref="A1:K61" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36" headerRowBorderDxfId="34" tableBorderDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C7124E47-3D2D-419B-8945-4E2B1598725E}" name="NACIONAL" displayName="NACIONAL" ref="A1:K61" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53" headerRowBorderDxfId="51" tableBorderDxfId="52">
   <autoFilter ref="A1:K61" xr:uid="{33A3F7D7-6411-4CF7-BF16-EE442911A307}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{D8D5599C-26F8-4B96-A944-93A638641D17}" name="DIA" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{352161EA-93C1-4162-BA39-C8F655D430A1}" name="FECHA" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{2839CFBF-A305-42F2-88A4-C827A1D25679}" name="Casos Diarios" dataDxfId="31">
+    <tableColumn id="1" xr3:uid="{D8D5599C-26F8-4B96-A944-93A638641D17}" name="DIA" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{352161EA-93C1-4162-BA39-C8F655D430A1}" name="FECHA" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{2839CFBF-A305-42F2-88A4-C827A1D25679}" name="Casos Diarios" dataDxfId="48">
       <calculatedColumnFormula>+D2-D1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{746365E8-EF89-4CE5-9A68-ED14EB89C707}" name="CONFIRMADOS" dataDxfId="30"/>
-    <tableColumn id="5" xr3:uid="{1F35E502-3209-41A9-A716-55909FD4CE33}" name="ACTIVOS" dataDxfId="29"/>
-    <tableColumn id="6" xr3:uid="{E5532EE7-0A18-469F-BDF7-CAF333074AF6}" name="RECUPERADOS" dataDxfId="28"/>
-    <tableColumn id="7" xr3:uid="{62350318-0139-4403-A488-2B648C65EDDC}" name="FALLECIDOS" dataDxfId="27"/>
-    <tableColumn id="8" xr3:uid="{2FF37737-68C5-432E-8F2A-BCC30E017674}" name="Recuperados Dia" dataDxfId="26">
+    <tableColumn id="4" xr3:uid="{746365E8-EF89-4CE5-9A68-ED14EB89C707}" name="CONFIRMADOS" dataDxfId="47"/>
+    <tableColumn id="5" xr3:uid="{1F35E502-3209-41A9-A716-55909FD4CE33}" name="ACTIVOS" dataDxfId="46"/>
+    <tableColumn id="6" xr3:uid="{E5532EE7-0A18-469F-BDF7-CAF333074AF6}" name="RECUPERADOS" dataDxfId="45"/>
+    <tableColumn id="7" xr3:uid="{62350318-0139-4403-A488-2B648C65EDDC}" name="FALLECIDOS" dataDxfId="44"/>
+    <tableColumn id="8" xr3:uid="{2FF37737-68C5-432E-8F2A-BCC30E017674}" name="Recuperados Dia" dataDxfId="43">
       <calculatedColumnFormula>+F2-F1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{E0C7BDB2-997F-47C0-879C-AA731B03EFD8}" name="Muertes Dia" dataDxfId="25">
+    <tableColumn id="9" xr3:uid="{E0C7BDB2-997F-47C0-879C-AA731B03EFD8}" name="Muertes Dia" dataDxfId="42">
       <calculatedColumnFormula>+G2-G1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{2A7F7A4E-FC96-42F6-A103-85E6F20545FF}" name="Casos Activos" dataDxfId="24">
+    <tableColumn id="11" xr3:uid="{2A7F7A4E-FC96-42F6-A103-85E6F20545FF}" name="Casos Activos" dataDxfId="41">
       <calculatedColumnFormula>+NACIONAL[[#This Row],[CONFIRMADOS]]-NACIONAL[[#This Row],[FALLECIDOS]]-NACIONAL[[#This Row],[RECUPERADOS]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{3EE2EC84-A7FD-4AA3-9DDB-E9C4BEBF9399}" name="FALLECIDOS AJENOS A COVID19" dataDxfId="23"/>
+    <tableColumn id="10" xr3:uid="{3EE2EC84-A7FD-4AA3-9DDB-E9C4BEBF9399}" name="FALLECIDOS AJENOS A COVID19" dataDxfId="40"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D63A59D9-99C4-4678-B12B-D109AED59771}" name="Casos_Region3456111213" displayName="Casos_Region3456111213" ref="A44:C49" totalsRowShown="0">
+  <autoFilter ref="A44:C49" xr:uid="{2821B4F7-7666-491D-BB65-60EA7DF397FF}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{E5BC92B7-CDA0-4360-AABB-85F5E7236B58}" name="Fecha?" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{9F4AF9A7-4DF1-46DE-81AD-512F12EB5B1E}" name="Región"/>
+    <tableColumn id="3" xr3:uid="{9E06D87A-F7AB-4AF1-8737-F3418A3A4CA9}" name="Casos Confirmados"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{EF8BE795-CF3D-4CE2-93C8-9F34D23EF597}" name="Casos_Region345611121314" displayName="Casos_Region345611121314" ref="A51:C56" totalsRowShown="0">
+  <autoFilter ref="A51:C56" xr:uid="{10090E4A-87E5-42FE-A612-5937947AEC44}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{3C3B559E-8239-42EB-B604-6D47448C89F7}" name="Fecha?" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{2E216AC0-2816-468D-AD18-FC26410958F2}" name="Región"/>
+    <tableColumn id="3" xr3:uid="{D3F7CE52-048C-498F-B65F-16EE45F46EBC}" name="Casos Confirmados"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{55B1D945-2F63-4FF9-827F-1E77EDE96F2F}" name="Casos_Region34561112131415" displayName="Casos_Region34561112131415" ref="A58:C63" totalsRowShown="0">
+  <autoFilter ref="A58:C63" xr:uid="{5A0082E9-49BC-4396-9097-A6EE305DAFB1}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{7D0BA00C-DD29-46D6-B386-839779C94CA1}" name="Fecha?" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{5AF97B5D-5DF7-4648-B44F-6887B5DD7529}" name="Región"/>
+    <tableColumn id="3" xr3:uid="{8EA75C18-897B-4865-8233-7A9F67403C15}" name="Casos Confirmados"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{DCFC99A3-0B75-49DC-9A64-3DC2F452239E}" name="Casos_Region3456111213141516" displayName="Casos_Region3456111213141516" ref="A65:C70" totalsRowShown="0">
+  <autoFilter ref="A65:C70" xr:uid="{D3785D59-1878-4BBF-9C42-3C55B163CB7A}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{9D5DF5BA-28AA-4E89-AAD0-AB5F09889825}" name="Fecha?" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{41890EF8-844A-4A6F-9D17-1554F6E0C524}" name="Región"/>
+    <tableColumn id="3" xr3:uid="{B9310D47-D4A8-40C7-B107-C97B3600CFA1}" name="Casos Confirmados"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{CA77C4DA-2BD5-47AC-9EB5-366A697C859E}" name="Casos_Region345611121314151617" displayName="Casos_Region345611121314151617" ref="A72:C77" totalsRowShown="0">
+  <autoFilter ref="A72:C77" xr:uid="{D50C6FAC-5541-4C52-9628-56A2767DFEF6}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{99122905-BD28-4238-8386-A2C3003A8AFD}" name="Fecha?" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{0150ADA5-A0F6-4163-AE27-BEF4EE57482A}" name="Región"/>
+    <tableColumn id="3" xr3:uid="{8F070BFF-161C-44B1-B305-FF22900586A6}" name="Casos Confirmados"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{591C589D-A3F0-4B15-B7ED-13A2E5641B41}" name="Casos_Region34561112131415161718" displayName="Casos_Region34561112131415161718" ref="A79:C84" totalsRowShown="0">
+  <autoFilter ref="A79:C84" xr:uid="{0338D195-82A1-4119-A6B1-8C5547185915}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{C6413E56-66B7-4717-8AEC-829918482967}" name="Fecha?" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{AC432778-CE13-4119-8F19-68938971B9CB}" name="Región"/>
+    <tableColumn id="3" xr3:uid="{B27D73FC-C8FF-4F71-92A5-C43B9A6F6B27}" name="Casos Confirmados"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{23351F7B-5160-4487-879B-02B7F1F68AD3}" name="Casos_Region3456111213141516171819" displayName="Casos_Region3456111213141516171819" ref="A86:C91" totalsRowShown="0">
+  <autoFilter ref="A86:C91" xr:uid="{1825962C-1104-4A2C-953C-90AC56F30BBC}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{ED88267F-1CDF-4A7D-B391-1CB7667356A2}" name="Fecha?" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{ECF2074F-AF12-43CA-AC3D-EC67D28E35FA}" name="Región"/>
+    <tableColumn id="3" xr3:uid="{3F5B82D2-1E35-497D-8B6F-D070D190522E}" name="Casos Confirmados"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{3742891B-984C-41FC-82A1-655F98266DCD}" name="Casos_Region345611121314151617181920" displayName="Casos_Region345611121314151617181920" ref="A93:C98" totalsRowShown="0">
+  <autoFilter ref="A93:C98" xr:uid="{F630AF07-3F44-4D24-A1F0-CE36696EA01F}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{E72CFE8B-A540-4DB8-AE9D-038F35374AF0}" name="Fecha?" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{5CB01D4D-35B9-4AB8-9E24-D4CC9166970D}" name="Región"/>
+    <tableColumn id="3" xr3:uid="{C01B4E19-A03E-421E-90F1-D103DB48DB1D}" name="Casos Confirmados"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{5CABD000-1B38-4898-976A-55119E1FC4A0}" name="Casos_Region21" displayName="Casos_Region21" ref="A107:C112" totalsRowShown="0">
+  <autoFilter ref="A107:C112" xr:uid="{A281A194-639C-4C52-AF3B-7BDF4832D686}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{66797F5B-9BA2-460D-862F-418E22C94242}" name="Fecha?" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{03ED28EF-F694-4D10-B0C3-0FC76EE5038A}" name="Región"/>
+    <tableColumn id="3" xr3:uid="{8F25ABB3-9D5E-408F-9E00-78D61A8E3FA6}" name="Casos Confirmados"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{17E2B4B8-91A2-4645-8EAD-7238A95B7BF8}" name="Casos_Region2122" displayName="Casos_Region2122" ref="A114:C119" totalsRowShown="0">
+  <autoFilter ref="A114:C119" xr:uid="{EAC4B90F-6EFF-4396-B6BA-EFED235ADF4A}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{17CCFC76-BC17-430F-8A24-D8F0FA34FB13}" name="Fecha?" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{A573CD32-AFBC-4620-BB0A-A226E2D87308}" name="Región"/>
+    <tableColumn id="3" xr3:uid="{F0812C8E-5204-45F3-B338-633C228CA6F2}" name="Casos Confirmados"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D194683B-F380-4419-8481-EA84E67B22A1}" name="Casos_Region" displayName="Casos_Region" ref="A3:C8" totalsRowShown="0">
-  <autoFilter ref="A3:C8" xr:uid="{34E41DA0-9A9B-4F51-80FA-22E83F1973DA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D194683B-F380-4419-8481-EA84E67B22A1}" name="Casos_Region" displayName="Casos_Region" ref="A100:C105" totalsRowShown="0">
+  <autoFilter ref="A100:C105" xr:uid="{34E41DA0-9A9B-4F51-80FA-22E83F1973DA}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{734347CE-477D-41AD-B610-485A7ED9F808}" name="Fecha?" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{734347CE-477D-41AD-B610-485A7ED9F808}" name="Fecha?" dataDxfId="39"/>
     <tableColumn id="2" xr3:uid="{AEEA1AFD-C1EA-434A-B9D0-9FFA8A0FB2B1}" name="Región"/>
     <tableColumn id="3" xr3:uid="{6A14AD86-09F0-40EF-A380-7FD3103EB61A}" name="Casos Confirmados"/>
   </tableColumns>
@@ -4179,19 +4350,19 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{101D3457-3C6E-48E6-B12B-8EDD572B1235}" name="Casos_Region2" displayName="Casos_Region2" ref="A12:C17" totalsRowShown="0">
-  <autoFilter ref="A12:C17" xr:uid="{8BCBF50F-BA4A-4DDA-A2AD-ECAC246591F8}"/>
+<file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{B1A18652-A014-45B2-BA25-010CECB00FA0}" name="Casos_Region212223" displayName="Casos_Region212223" ref="A121:C126" totalsRowShown="0">
+  <autoFilter ref="A121:C126" xr:uid="{EAFF4425-E5A4-4DE5-899E-C29E27F5B240}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{948C823E-37CA-4DA7-8E85-2B07E220ADCC}" name="Fecha?" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{8775938F-957C-40AC-95F7-1B16C015A774}" name="Región"/>
-    <tableColumn id="3" xr3:uid="{9B0E7360-6C5A-4080-A874-F9525D68FA54}" name="Casos Confirmados"/>
+    <tableColumn id="1" xr3:uid="{68D0D495-5B3D-424B-8541-2FDA631AF853}" name="Fecha?" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{2689081A-CF6C-45BD-9AB5-CEC964810105}" name="Región"/>
+    <tableColumn id="3" xr3:uid="{B8765138-3C73-4DB1-A193-612328A2E76E}" name="Casos Confirmados"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{098B8ABD-39CC-481F-B5DD-8A1D47B5485B}" name="Detalle_Casos" displayName="Detalle_Casos" ref="A1:H1115" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" headerRowBorderDxfId="17" tableBorderDxfId="18">
   <autoFilter ref="A1:H1115" xr:uid="{D721CE67-7EB3-4B8C-BCC9-32CE3BEDA9AC}"/>
   <tableColumns count="8">
@@ -4212,7 +4383,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{EB010619-E8A6-4116-9C9C-D73284B3D1E1}" name="LOCALIZACION" displayName="LOCALIZACION" ref="A1:T342" totalsRowShown="0" headerRowDxfId="12">
   <autoFilter ref="A1:T342" xr:uid="{F755337D-02A3-4DAB-87BB-D016B95CC58B}"/>
   <tableColumns count="20">
@@ -4238,6 +4409,90 @@
     <tableColumn id="12" xr3:uid="{4599194D-BA8F-43C4-B068-8D03117965DB}" name="Población total" dataDxfId="2" dataCellStyle="Millares"/>
     <tableColumn id="20" xr3:uid="{4FFC72DD-11E2-400C-9FEE-91912B922BB8}" name="Sexo - Hombres" dataDxfId="1" dataCellStyle="Millares"/>
     <tableColumn id="21" xr3:uid="{E3D930E8-0241-4EF6-8308-70832F57DC80}" name="Sexo - Mujeres" dataDxfId="0" dataCellStyle="Millares"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{101D3457-3C6E-48E6-B12B-8EDD572B1235}" name="Casos_Region2" displayName="Casos_Region2" ref="A128:C133" totalsRowShown="0">
+  <autoFilter ref="A128:C133" xr:uid="{8BCBF50F-BA4A-4DDA-A2AD-ECAC246591F8}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{948C823E-37CA-4DA7-8E85-2B07E220ADCC}" name="Fecha?" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{8775938F-957C-40AC-95F7-1B16C015A774}" name="Región"/>
+    <tableColumn id="3" xr3:uid="{9B0E7360-6C5A-4080-A874-F9525D68FA54}" name="Casos Confirmados"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C2742386-4B94-4797-AF7D-79F889580DBB}" name="Casos_Region3" displayName="Casos_Region3" ref="A2:C7" totalsRowShown="0">
+  <autoFilter ref="A2:C7" xr:uid="{3748EFC6-3E6C-4AD5-BC4D-61D668B7DCC2}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{95DE0B55-2992-4D1F-9E73-CD885A43DBA7}" name="Fecha?" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{5B276D1F-061C-4DB2-A173-70FB0CD1A719}" name="Región"/>
+    <tableColumn id="3" xr3:uid="{B2B5C373-0D4A-4F09-98BA-3984D7537027}" name="Casos Confirmados"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B11B2113-BE52-43D4-91AC-2E344DEE2008}" name="Casos_Region34" displayName="Casos_Region34" ref="A9:C14" totalsRowShown="0">
+  <autoFilter ref="A9:C14" xr:uid="{3579FAFE-19E6-45BE-91C2-D67F3660A3A4}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{092B3FEF-7820-4008-B5B8-56E28C005877}" name="Fecha?" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{8997E4A4-1130-40B0-B909-5921A8D3B409}" name="Región"/>
+    <tableColumn id="3" xr3:uid="{83DA3FC0-965A-41F1-8F02-CE1BEE49BC3C}" name="Casos Confirmados"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6E385BE6-B3F7-49A9-8DB1-2BB33673335B}" name="Casos_Region345" displayName="Casos_Region345" ref="A16:C21" totalsRowShown="0">
+  <autoFilter ref="A16:C21" xr:uid="{301A1D02-60F4-4436-B755-1EA4E35BF270}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{F65EAAE7-10B3-4E46-B28A-8869F4D91A9B}" name="Fecha?" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{0A5F5FE6-9155-4D5C-841A-C2FC487797E5}" name="Región"/>
+    <tableColumn id="3" xr3:uid="{294D1AA7-92E8-471B-A857-E9FE3896A7B8}" name="Casos Confirmados"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{2F4BAAE9-401D-4BD5-B9B8-C010231167C5}" name="Casos_Region3456" displayName="Casos_Region3456" ref="A23:C28" totalsRowShown="0">
+  <autoFilter ref="A23:C28" xr:uid="{3E8B03E3-E399-4120-A5BE-924F83D217FC}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{AACA3BB1-363B-4FF3-9169-14076365DFC1}" name="Fecha?" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{0690CBC9-B25C-4611-8194-41A415625CF9}" name="Región"/>
+    <tableColumn id="3" xr3:uid="{2B3CB05D-DD88-4FCE-8C60-38389267B432}" name="Casos Confirmados"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{92926CD9-120D-4A4D-98AA-C2DE8ED2EDC2}" name="Casos_Region345611" displayName="Casos_Region345611" ref="A30:C35" totalsRowShown="0">
+  <autoFilter ref="A30:C35" xr:uid="{89779339-2441-456F-858B-2C999F7B54AB}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{D867A888-1301-4740-8695-D3685454F429}" name="Fecha?" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{1F225517-36A3-4804-B79A-76CE0324A681}" name="Región"/>
+    <tableColumn id="3" xr3:uid="{77F4EB90-A0BB-46F4-916F-BE11DB74D5AF}" name="Casos Confirmados"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{5B55B305-D1E1-4A61-9EA1-EA7B64227CCB}" name="Casos_Region34561112" displayName="Casos_Region34561112" ref="A37:C42" totalsRowShown="0">
+  <autoFilter ref="A37:C42" xr:uid="{FA91FE55-6400-444F-89A5-B0B9524EE310}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{39066C51-0F75-45D2-8CD3-C744A56AE8BA}" name="Fecha?" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{45A07C80-BC64-4F72-9B83-410FD6039488}" name="Región"/>
+    <tableColumn id="3" xr3:uid="{EAEFDAE5-CCDD-4B65-9B28-8899CFEF1CF9}" name="Casos Confirmados"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6890,7 +7145,7 @@
       <c r="A61" s="61">
         <v>60</v>
       </c>
-      <c r="B61" s="95">
+      <c r="B61" s="91">
         <v>43962</v>
       </c>
       <c r="C61" s="62">
@@ -6968,10 +7223,10 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A2:C133"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -6980,150 +7235,1334 @@
     <col min="3" max="3" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="C1">
-        <f>SUM(C4:C8)</f>
-        <v>1052</v>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>11</v>
+      <c r="A3" s="49">
+        <v>43944</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="C3">
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="49">
-        <v>43958</v>
+        <v>43944</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4">
-        <v>638</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="49">
-        <v>43958</v>
+        <v>43944</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5">
-        <v>137</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="49">
-        <v>43958</v>
+        <v>43944</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6">
-        <v>126</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="49">
-        <v>43958</v>
+        <v>43944</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7">
-        <v>76</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="49">
-        <v>43958</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8">
-        <v>75</v>
+      <c r="A8" s="49"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="49">
+        <v>43945</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="49">
+        <v>43945</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11">
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>11</v>
+      <c r="A12" s="49">
+        <v>43945</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="C12">
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="49">
-        <v>43962</v>
+        <v>43945</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C13">
-        <v>679</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="49">
-        <v>43962</v>
+        <v>43945</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C14">
-        <v>142</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="49">
-        <v>43962</v>
-      </c>
-      <c r="B15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15">
-        <v>128</v>
-      </c>
+      <c r="A15" s="49"/>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="49">
-        <v>43962</v>
+      <c r="A16" t="s">
+        <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16">
-        <v>87</v>
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="49">
+        <v>43946</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="49">
+        <v>43946</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="49">
+        <v>43946</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="49">
+        <v>43946</v>
+      </c>
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="49">
+        <v>43946</v>
+      </c>
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="49"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="49">
+        <v>43947</v>
+      </c>
+      <c r="B24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="49">
+        <v>43947</v>
+      </c>
+      <c r="B25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="49">
+        <v>43947</v>
+      </c>
+      <c r="B26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15" customHeight="1">
+      <c r="A27" s="49">
+        <v>43947</v>
+      </c>
+      <c r="B27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="49">
+        <v>43947</v>
+      </c>
+      <c r="B28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="49"/>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="49">
+        <v>43948</v>
+      </c>
+      <c r="B31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="49">
+        <v>43948</v>
+      </c>
+      <c r="B32" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="49">
+        <v>43948</v>
+      </c>
+      <c r="B33" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="49">
+        <v>43948</v>
+      </c>
+      <c r="B34" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="49">
+        <v>43948</v>
+      </c>
+      <c r="B35" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="49"/>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="49">
+        <v>43949</v>
+      </c>
+      <c r="B38" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="49">
+        <v>43949</v>
+      </c>
+      <c r="B39" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="49">
+        <v>43949</v>
+      </c>
+      <c r="B40" t="s">
+        <v>16</v>
+      </c>
+      <c r="C40">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="49">
+        <v>43949</v>
+      </c>
+      <c r="B41" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="49">
+        <v>43949</v>
+      </c>
+      <c r="B42" t="s">
+        <v>18</v>
+      </c>
+      <c r="C42">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="49"/>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>11</v>
+      </c>
+      <c r="B44" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="49">
+        <v>43950</v>
+      </c>
+      <c r="B45" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="49">
+        <v>43950</v>
+      </c>
+      <c r="B46" t="s">
+        <v>15</v>
+      </c>
+      <c r="C46">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="49">
+        <v>43950</v>
+      </c>
+      <c r="B47" t="s">
+        <v>16</v>
+      </c>
+      <c r="C47">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="49">
+        <v>43950</v>
+      </c>
+      <c r="B48" t="s">
+        <v>17</v>
+      </c>
+      <c r="C48">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="49">
+        <v>43950</v>
+      </c>
+      <c r="B49" t="s">
+        <v>18</v>
+      </c>
+      <c r="C49">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="49"/>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>11</v>
+      </c>
+      <c r="B51" t="s">
+        <v>12</v>
+      </c>
+      <c r="C51" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="49">
+        <v>43951</v>
+      </c>
+      <c r="B52" t="s">
+        <v>14</v>
+      </c>
+      <c r="C52">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="49">
+        <v>43951</v>
+      </c>
+      <c r="B53" t="s">
+        <v>15</v>
+      </c>
+      <c r="C53">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="49">
+        <v>43951</v>
+      </c>
+      <c r="B54" t="s">
+        <v>16</v>
+      </c>
+      <c r="C54">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="49">
+        <v>43951</v>
+      </c>
+      <c r="B55" t="s">
+        <v>17</v>
+      </c>
+      <c r="C55">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="49">
+        <v>43951</v>
+      </c>
+      <c r="B56" t="s">
+        <v>18</v>
+      </c>
+      <c r="C56">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="49"/>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>11</v>
+      </c>
+      <c r="B58" t="s">
+        <v>12</v>
+      </c>
+      <c r="C58" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="49">
+        <v>43952</v>
+      </c>
+      <c r="B59" t="s">
+        <v>14</v>
+      </c>
+      <c r="C59">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="49">
+        <v>43952</v>
+      </c>
+      <c r="B60" t="s">
+        <v>15</v>
+      </c>
+      <c r="C60">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="49">
+        <v>43952</v>
+      </c>
+      <c r="B61" t="s">
+        <v>16</v>
+      </c>
+      <c r="C61">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="49">
+        <v>43952</v>
+      </c>
+      <c r="B62" t="s">
+        <v>17</v>
+      </c>
+      <c r="C62">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="49">
+        <v>43952</v>
+      </c>
+      <c r="B63" t="s">
+        <v>18</v>
+      </c>
+      <c r="C63">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="49"/>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
+        <v>11</v>
+      </c>
+      <c r="B65" t="s">
+        <v>12</v>
+      </c>
+      <c r="C65" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="49">
+        <v>43953</v>
+      </c>
+      <c r="B66" t="s">
+        <v>14</v>
+      </c>
+      <c r="C66">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="49">
+        <v>43953</v>
+      </c>
+      <c r="B67" t="s">
+        <v>15</v>
+      </c>
+      <c r="C67">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="49">
+        <v>43953</v>
+      </c>
+      <c r="B68" t="s">
+        <v>16</v>
+      </c>
+      <c r="C68">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="49">
+        <v>43953</v>
+      </c>
+      <c r="B69" t="s">
+        <v>17</v>
+      </c>
+      <c r="C69">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="49">
+        <v>43953</v>
+      </c>
+      <c r="B70" t="s">
+        <v>18</v>
+      </c>
+      <c r="C70">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="49"/>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
+        <v>11</v>
+      </c>
+      <c r="B72" t="s">
+        <v>12</v>
+      </c>
+      <c r="C72" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="49">
+        <v>43954</v>
+      </c>
+      <c r="B73" t="s">
+        <v>14</v>
+      </c>
+      <c r="C73">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="49">
+        <v>43954</v>
+      </c>
+      <c r="B74" t="s">
+        <v>15</v>
+      </c>
+      <c r="C74">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="49">
+        <v>43954</v>
+      </c>
+      <c r="B75" t="s">
+        <v>16</v>
+      </c>
+      <c r="C75">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="49">
+        <v>43954</v>
+      </c>
+      <c r="B76" t="s">
+        <v>17</v>
+      </c>
+      <c r="C76">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="49">
+        <v>43954</v>
+      </c>
+      <c r="B77" t="s">
+        <v>18</v>
+      </c>
+      <c r="C77">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="49"/>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" t="s">
+        <v>11</v>
+      </c>
+      <c r="B79" t="s">
+        <v>12</v>
+      </c>
+      <c r="C79" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="49">
+        <v>43955</v>
+      </c>
+      <c r="B80" t="s">
+        <v>14</v>
+      </c>
+      <c r="C80">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="49">
+        <v>43955</v>
+      </c>
+      <c r="B81" t="s">
+        <v>15</v>
+      </c>
+      <c r="C81">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="49">
+        <v>43955</v>
+      </c>
+      <c r="B82" t="s">
+        <v>16</v>
+      </c>
+      <c r="C82">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" s="49">
+        <v>43955</v>
+      </c>
+      <c r="B83" t="s">
+        <v>17</v>
+      </c>
+      <c r="C83">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" s="49">
+        <v>43955</v>
+      </c>
+      <c r="B84" t="s">
+        <v>18</v>
+      </c>
+      <c r="C84">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="49"/>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" t="s">
+        <v>11</v>
+      </c>
+      <c r="B86" t="s">
+        <v>12</v>
+      </c>
+      <c r="C86" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="49">
+        <v>43956</v>
+      </c>
+      <c r="B87" t="s">
+        <v>14</v>
+      </c>
+      <c r="C87">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="49">
+        <v>43956</v>
+      </c>
+      <c r="B88" t="s">
+        <v>15</v>
+      </c>
+      <c r="C88">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" s="49">
+        <v>43956</v>
+      </c>
+      <c r="B89" t="s">
+        <v>16</v>
+      </c>
+      <c r="C89">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="49">
+        <v>43956</v>
+      </c>
+      <c r="B90" t="s">
+        <v>17</v>
+      </c>
+      <c r="C90">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" s="49">
+        <v>43956</v>
+      </c>
+      <c r="B91" t="s">
+        <v>18</v>
+      </c>
+      <c r="C91">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" s="49"/>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" t="s">
+        <v>11</v>
+      </c>
+      <c r="B93" t="s">
+        <v>12</v>
+      </c>
+      <c r="C93" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" s="49">
+        <v>43957</v>
+      </c>
+      <c r="B94" t="s">
+        <v>14</v>
+      </c>
+      <c r="C94">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" s="49">
+        <v>43957</v>
+      </c>
+      <c r="B95" t="s">
+        <v>15</v>
+      </c>
+      <c r="C95">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="49">
+        <v>43957</v>
+      </c>
+      <c r="B96" t="s">
+        <v>16</v>
+      </c>
+      <c r="C96">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" s="49">
+        <v>43957</v>
+      </c>
+      <c r="B97" t="s">
+        <v>17</v>
+      </c>
+      <c r="C97">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" s="49">
+        <v>43957</v>
+      </c>
+      <c r="B98" t="s">
+        <v>18</v>
+      </c>
+      <c r="C98">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" s="49"/>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" t="s">
+        <v>11</v>
+      </c>
+      <c r="B100" t="s">
+        <v>12</v>
+      </c>
+      <c r="C100" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" s="49">
+        <v>43958</v>
+      </c>
+      <c r="B101" t="s">
+        <v>14</v>
+      </c>
+      <c r="C101">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" s="49">
+        <v>43958</v>
+      </c>
+      <c r="B102" t="s">
+        <v>15</v>
+      </c>
+      <c r="C102">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" s="49">
+        <v>43958</v>
+      </c>
+      <c r="B103" t="s">
+        <v>16</v>
+      </c>
+      <c r="C103">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" s="49">
+        <v>43958</v>
+      </c>
+      <c r="B104" t="s">
+        <v>17</v>
+      </c>
+      <c r="C104">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" s="49">
+        <v>43958</v>
+      </c>
+      <c r="B105" t="s">
+        <v>18</v>
+      </c>
+      <c r="C105">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" s="49"/>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" t="s">
+        <v>11</v>
+      </c>
+      <c r="B107" t="s">
+        <v>12</v>
+      </c>
+      <c r="C107" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" s="49">
+        <v>43959</v>
+      </c>
+      <c r="B108" t="s">
+        <v>14</v>
+      </c>
+      <c r="C108">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" s="49">
+        <v>43959</v>
+      </c>
+      <c r="B109" t="s">
+        <v>15</v>
+      </c>
+      <c r="C109">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" s="49">
+        <v>43959</v>
+      </c>
+      <c r="B110" t="s">
+        <v>16</v>
+      </c>
+      <c r="C110">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" s="49">
+        <v>43959</v>
+      </c>
+      <c r="B111" t="s">
+        <v>17</v>
+      </c>
+      <c r="C111">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" s="49">
+        <v>43959</v>
+      </c>
+      <c r="B112" t="s">
+        <v>18</v>
+      </c>
+      <c r="C112">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" s="49"/>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" t="s">
+        <v>11</v>
+      </c>
+      <c r="B114" t="s">
+        <v>12</v>
+      </c>
+      <c r="C114" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" s="49">
+        <v>43960</v>
+      </c>
+      <c r="B115" t="s">
+        <v>14</v>
+      </c>
+      <c r="C115">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" s="49">
+        <v>43960</v>
+      </c>
+      <c r="B116" t="s">
+        <v>15</v>
+      </c>
+      <c r="C116">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" s="49">
+        <v>43960</v>
+      </c>
+      <c r="B117" t="s">
+        <v>16</v>
+      </c>
+      <c r="C117">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" s="49">
+        <v>43960</v>
+      </c>
+      <c r="B118" t="s">
+        <v>17</v>
+      </c>
+      <c r="C118">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" s="49">
+        <v>43960</v>
+      </c>
+      <c r="B119" t="s">
+        <v>18</v>
+      </c>
+      <c r="C119">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" s="49"/>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" t="s">
+        <v>11</v>
+      </c>
+      <c r="B121" t="s">
+        <v>12</v>
+      </c>
+      <c r="C121" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" s="49">
+        <v>43961</v>
+      </c>
+      <c r="B122" t="s">
+        <v>14</v>
+      </c>
+      <c r="C122">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" s="49">
+        <v>43961</v>
+      </c>
+      <c r="B123" t="s">
+        <v>15</v>
+      </c>
+      <c r="C123">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" s="49">
+        <v>43961</v>
+      </c>
+      <c r="B124" t="s">
+        <v>16</v>
+      </c>
+      <c r="C124">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125" s="49">
+        <v>43961</v>
+      </c>
+      <c r="B125" t="s">
+        <v>17</v>
+      </c>
+      <c r="C125">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126" s="49">
+        <v>43961</v>
+      </c>
+      <c r="B126" t="s">
+        <v>18</v>
+      </c>
+      <c r="C126">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" t="s">
+        <v>11</v>
+      </c>
+      <c r="B128" t="s">
+        <v>12</v>
+      </c>
+      <c r="C128" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="A129" s="49">
         <v>43962</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B129" t="s">
+        <v>14</v>
+      </c>
+      <c r="C129">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130" s="49">
+        <v>43962</v>
+      </c>
+      <c r="B130" t="s">
+        <v>15</v>
+      </c>
+      <c r="C130">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="A131" s="49">
+        <v>43962</v>
+      </c>
+      <c r="B131" t="s">
+        <v>16</v>
+      </c>
+      <c r="C131">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
+      <c r="A132" s="49">
+        <v>43962</v>
+      </c>
+      <c r="B132" t="s">
+        <v>17</v>
+      </c>
+      <c r="C132">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133" s="49">
+        <v>43962</v>
+      </c>
+      <c r="B133" t="s">
         <v>18</v>
       </c>
-      <c r="C17">
+      <c r="C133">
         <v>78</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="2">
+  <tableParts count="19">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId11"/>
+    <tablePart r:id="rId12"/>
+    <tablePart r:id="rId13"/>
+    <tablePart r:id="rId14"/>
+    <tablePart r:id="rId15"/>
+    <tablePart r:id="rId16"/>
+    <tablePart r:id="rId17"/>
+    <tablePart r:id="rId18"/>
+    <tablePart r:id="rId19"/>
   </tableParts>
 </worksheet>
 </file>
@@ -34209,7 +35648,7 @@
         <f>+IFERROR(VLOOKUP(B1052,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1052" s="96">
+      <c r="C1052" s="92">
         <v>44140</v>
       </c>
       <c r="D1052">
@@ -34232,7 +35671,7 @@
         <f>+IFERROR(VLOOKUP(B1053,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1053" s="96">
+      <c r="C1053" s="92">
         <v>44140</v>
       </c>
       <c r="D1053">
@@ -34255,7 +35694,7 @@
         <f>+IFERROR(VLOOKUP(B1054,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1054" s="96">
+      <c r="C1054" s="92">
         <v>44140</v>
       </c>
       <c r="D1054">
@@ -34278,7 +35717,7 @@
         <f>+IFERROR(VLOOKUP(B1055,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1055" s="96">
+      <c r="C1055" s="92">
         <v>44140</v>
       </c>
       <c r="D1055">
@@ -34301,7 +35740,7 @@
         <f>+IFERROR(VLOOKUP(B1056,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1056" s="96">
+      <c r="C1056" s="92">
         <v>44140</v>
       </c>
       <c r="D1056">
@@ -34324,7 +35763,7 @@
         <f>+IFERROR(VLOOKUP(B1057,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1057" s="96">
+      <c r="C1057" s="92">
         <v>44140</v>
       </c>
       <c r="D1057">
@@ -34347,7 +35786,7 @@
         <f>+IFERROR(VLOOKUP(B1058,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1058" s="96">
+      <c r="C1058" s="92">
         <v>44140</v>
       </c>
       <c r="D1058">
@@ -34370,7 +35809,7 @@
         <f>+IFERROR(VLOOKUP(B1059,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1059" s="96">
+      <c r="C1059" s="92">
         <v>44140</v>
       </c>
       <c r="D1059">
@@ -34393,7 +35832,7 @@
         <f>+IFERROR(VLOOKUP(B1060,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1060" s="96">
+      <c r="C1060" s="92">
         <v>44140</v>
       </c>
       <c r="D1060">
@@ -34416,7 +35855,7 @@
         <f>+IFERROR(VLOOKUP(B1061,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1061" s="96">
+      <c r="C1061" s="92">
         <v>44140</v>
       </c>
       <c r="D1061">
@@ -34439,7 +35878,7 @@
         <f>+IFERROR(VLOOKUP(B1062,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1062" s="96">
+      <c r="C1062" s="92">
         <v>44140</v>
       </c>
       <c r="D1062">
@@ -34462,7 +35901,7 @@
         <f>+IFERROR(VLOOKUP(B1063,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1063" s="96">
+      <c r="C1063" s="92">
         <v>44140</v>
       </c>
       <c r="D1063">
@@ -34485,7 +35924,7 @@
         <f>+IFERROR(VLOOKUP(B1064,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1064" s="96">
+      <c r="C1064" s="92">
         <v>44140</v>
       </c>
       <c r="D1064">
@@ -34508,7 +35947,7 @@
         <f>+IFERROR(VLOOKUP(B1065,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1065" s="96">
+      <c r="C1065" s="92">
         <v>44140</v>
       </c>
       <c r="D1065">
@@ -34531,7 +35970,7 @@
         <f>+IFERROR(VLOOKUP(B1066,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1066" s="96">
+      <c r="C1066" s="92">
         <v>44140</v>
       </c>
       <c r="D1066">
@@ -34554,7 +35993,7 @@
         <f>+IFERROR(VLOOKUP(B1067,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1067" s="96">
+      <c r="C1067" s="92">
         <v>44140</v>
       </c>
       <c r="D1067">
@@ -34577,7 +36016,7 @@
         <f>+IFERROR(VLOOKUP(B1068,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1068" s="96">
+      <c r="C1068" s="92">
         <v>44140</v>
       </c>
       <c r="D1068">
@@ -34600,7 +36039,7 @@
         <f>+IFERROR(VLOOKUP(B1069,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1069" s="96">
+      <c r="C1069" s="92">
         <v>44140</v>
       </c>
       <c r="D1069">
@@ -34623,7 +36062,7 @@
         <f>+IFERROR(VLOOKUP(B1070,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1070" s="96">
+      <c r="C1070" s="92">
         <v>44140</v>
       </c>
       <c r="D1070">
@@ -34646,7 +36085,7 @@
         <f>+IFERROR(VLOOKUP(B1071,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1071" s="96">
+      <c r="C1071" s="92">
         <v>44140</v>
       </c>
       <c r="D1071">
@@ -34669,7 +36108,7 @@
         <f>+IFERROR(VLOOKUP(B1072,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1072" s="96">
+      <c r="C1072" s="92">
         <v>44140</v>
       </c>
       <c r="D1072">
@@ -34692,7 +36131,7 @@
         <f>+IFERROR(VLOOKUP(B1073,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1073" s="96">
+      <c r="C1073" s="92">
         <v>44140</v>
       </c>
       <c r="D1073">
@@ -34715,7 +36154,7 @@
         <f>+IFERROR(VLOOKUP(B1074,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1074" s="96">
+      <c r="C1074" s="92">
         <v>44140</v>
       </c>
       <c r="D1074">
@@ -34738,7 +36177,7 @@
         <f>+IFERROR(VLOOKUP(B1075,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1075" s="96">
+      <c r="C1075" s="92">
         <v>44140</v>
       </c>
       <c r="D1075">
@@ -34761,7 +36200,7 @@
         <f>+IFERROR(VLOOKUP(B1076,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1076" s="96">
+      <c r="C1076" s="92">
         <v>44140</v>
       </c>
       <c r="D1076">
@@ -34784,7 +36223,7 @@
         <f>+IFERROR(VLOOKUP(B1077,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1077" s="96">
+      <c r="C1077" s="92">
         <v>44140</v>
       </c>
       <c r="D1077">
@@ -34807,7 +36246,7 @@
         <f>+IFERROR(VLOOKUP(B1078,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1078" s="96">
+      <c r="C1078" s="92">
         <v>44140</v>
       </c>
       <c r="D1078">
@@ -34830,7 +36269,7 @@
         <f>+IFERROR(VLOOKUP(B1079,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1079" s="96">
+      <c r="C1079" s="92">
         <v>44140</v>
       </c>
       <c r="D1079">
@@ -34853,7 +36292,7 @@
         <f>+IFERROR(VLOOKUP(B1080,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1080" s="96">
+      <c r="C1080" s="92">
         <v>44140</v>
       </c>
       <c r="D1080">
@@ -34876,7 +36315,7 @@
         <f>+IFERROR(VLOOKUP(B1081,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1081" s="96">
+      <c r="C1081" s="92">
         <v>44140</v>
       </c>
       <c r="D1081">
@@ -34899,7 +36338,7 @@
         <f>+IFERROR(VLOOKUP(B1082,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1082" s="96">
+      <c r="C1082" s="92">
         <v>44140</v>
       </c>
       <c r="D1082">
@@ -34922,7 +36361,7 @@
         <f>+IFERROR(VLOOKUP(B1083,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1083" s="96">
+      <c r="C1083" s="92">
         <v>44140</v>
       </c>
       <c r="D1083">
@@ -34945,7 +36384,7 @@
         <f>+IFERROR(VLOOKUP(B1084,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1084" s="96">
+      <c r="C1084" s="92">
         <v>44140</v>
       </c>
       <c r="D1084">
@@ -34968,7 +36407,7 @@
         <f>+IFERROR(VLOOKUP(B1085,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1085" s="96">
+      <c r="C1085" s="92">
         <v>44140</v>
       </c>
       <c r="D1085">
@@ -34991,7 +36430,7 @@
         <f>+IFERROR(VLOOKUP(B1086,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1086" s="96">
+      <c r="C1086" s="92">
         <v>44140</v>
       </c>
       <c r="D1086">
@@ -35014,7 +36453,7 @@
         <f>+IFERROR(VLOOKUP(B1087,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1087" s="96">
+      <c r="C1087" s="92">
         <v>44140</v>
       </c>
       <c r="D1087">
@@ -35037,7 +36476,7 @@
         <f>+IFERROR(VLOOKUP(B1088,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1088" s="96">
+      <c r="C1088" s="92">
         <v>44140</v>
       </c>
       <c r="D1088">
@@ -35060,7 +36499,7 @@
         <f>+IFERROR(VLOOKUP(B1089,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1089" s="96">
+      <c r="C1089" s="92">
         <v>44140</v>
       </c>
       <c r="D1089">
@@ -35083,7 +36522,7 @@
         <f>+IFERROR(VLOOKUP(B1090,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1090" s="96">
+      <c r="C1090" s="92">
         <v>44140</v>
       </c>
       <c r="D1090">
@@ -35106,7 +36545,7 @@
         <f>+IFERROR(VLOOKUP(B1091,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1091" s="96">
+      <c r="C1091" s="92">
         <v>44140</v>
       </c>
       <c r="D1091">
@@ -35129,7 +36568,7 @@
         <f>+IFERROR(VLOOKUP(B1092,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1092" s="96">
+      <c r="C1092" s="92">
         <v>44140</v>
       </c>
       <c r="D1092">
@@ -35152,7 +36591,7 @@
         <f>+IFERROR(VLOOKUP(B1093,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1093" s="96">
+      <c r="C1093" s="92">
         <v>44140</v>
       </c>
       <c r="D1093">
@@ -35175,7 +36614,7 @@
         <f>+IFERROR(VLOOKUP(B1094,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1094" s="96">
+      <c r="C1094" s="92">
         <v>44140</v>
       </c>
       <c r="D1094">
@@ -35198,7 +36637,7 @@
         <f>+IFERROR(VLOOKUP(B1095,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1095" s="96">
+      <c r="C1095" s="92">
         <v>44140</v>
       </c>
       <c r="D1095">
@@ -35221,7 +36660,7 @@
         <f>+IFERROR(VLOOKUP(B1096,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1096" s="96">
+      <c r="C1096" s="92">
         <v>44140</v>
       </c>
       <c r="D1096">
@@ -35244,7 +36683,7 @@
         <f>+IFERROR(VLOOKUP(B1097,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1097" s="96">
+      <c r="C1097" s="92">
         <v>44140</v>
       </c>
       <c r="D1097">
@@ -35267,7 +36706,7 @@
         <f>+IFERROR(VLOOKUP(B1098,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1098" s="96">
+      <c r="C1098" s="92">
         <v>44140</v>
       </c>
       <c r="D1098">
@@ -35290,7 +36729,7 @@
         <f>+IFERROR(VLOOKUP(B1099,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1099" s="96">
+      <c r="C1099" s="92">
         <v>44140</v>
       </c>
       <c r="D1099">
@@ -35313,7 +36752,7 @@
         <f>+IFERROR(VLOOKUP(B1100,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1100" s="96">
+      <c r="C1100" s="92">
         <v>44140</v>
       </c>
       <c r="D1100">
@@ -35336,7 +36775,7 @@
         <f>+IFERROR(VLOOKUP(B1101,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1101" s="96">
+      <c r="C1101" s="92">
         <v>44140</v>
       </c>
       <c r="D1101">
@@ -35359,7 +36798,7 @@
         <f>+IFERROR(VLOOKUP(B1102,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1102" s="96">
+      <c r="C1102" s="92">
         <v>44140</v>
       </c>
       <c r="D1102">
@@ -35382,7 +36821,7 @@
         <f>+IFERROR(VLOOKUP(B1103,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1103" s="96">
+      <c r="C1103" s="92">
         <v>44140</v>
       </c>
       <c r="D1103">
@@ -35405,7 +36844,7 @@
         <f>+IFERROR(VLOOKUP(B1104,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1104" s="96">
+      <c r="C1104" s="92">
         <v>44140</v>
       </c>
       <c r="D1104">
@@ -35428,7 +36867,7 @@
         <f>+IFERROR(VLOOKUP(B1105,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1105" s="96">
+      <c r="C1105" s="92">
         <v>44140</v>
       </c>
       <c r="D1105">
@@ -35451,7 +36890,7 @@
         <f>+IFERROR(VLOOKUP(B1106,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1106" s="96">
+      <c r="C1106" s="92">
         <v>44140</v>
       </c>
       <c r="D1106">
@@ -35474,7 +36913,7 @@
         <f>+IFERROR(VLOOKUP(B1107,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1107" s="96">
+      <c r="C1107" s="92">
         <v>44140</v>
       </c>
       <c r="D1107">
@@ -35497,7 +36936,7 @@
         <f>+IFERROR(VLOOKUP(B1108,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1108" s="96">
+      <c r="C1108" s="92">
         <v>44140</v>
       </c>
       <c r="D1108">
@@ -35520,7 +36959,7 @@
         <f>+IFERROR(VLOOKUP(B1109,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1109" s="96">
+      <c r="C1109" s="92">
         <v>44140</v>
       </c>
       <c r="D1109">
@@ -35543,7 +36982,7 @@
         <f>+IFERROR(VLOOKUP(B1110,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1110" s="96">
+      <c r="C1110" s="92">
         <v>44140</v>
       </c>
       <c r="D1110">
@@ -35566,7 +37005,7 @@
         <f>+IFERROR(VLOOKUP(B1111,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1111" s="96">
+      <c r="C1111" s="92">
         <v>44140</v>
       </c>
       <c r="D1111">
@@ -35589,7 +37028,7 @@
         <f>+IFERROR(VLOOKUP(B1112,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1112" s="96">
+      <c r="C1112" s="92">
         <v>44140</v>
       </c>
       <c r="D1112">
@@ -35612,7 +37051,7 @@
         <f>+IFERROR(VLOOKUP(B1113,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
       </c>
-      <c r="C1113" s="96">
+      <c r="C1113" s="92">
         <v>44140</v>
       </c>
       <c r="D1113">
@@ -35631,13 +37070,13 @@
       </c>
     </row>
     <row r="1114" spans="1:8" ht="15">
-      <c r="C1114" s="96"/>
+      <c r="C1114" s="92"/>
       <c r="E1114" s="53"/>
       <c r="F1114" s="53"/>
       <c r="G1114" s="53"/>
     </row>
     <row r="1115" spans="1:8" ht="15">
-      <c r="C1115" s="96"/>
+      <c r="C1115" s="92"/>
       <c r="E1115" s="53"/>
       <c r="F1115" s="53"/>
       <c r="G1115" s="53"/>
@@ -57438,7 +58877,7 @@
     </row>
     <row r="12" spans="2:8">
       <c r="B12" s="83"/>
-      <c r="C12" s="99"/>
+      <c r="C12" s="95"/>
       <c r="D12" s="61" t="s">
         <v>33</v>
       </c>
@@ -57448,7 +58887,7 @@
       <c r="F12" s="61" t="s">
         <v>888</v>
       </c>
-      <c r="G12" s="97" t="s">
+      <c r="G12" s="93" t="s">
         <v>886</v>
       </c>
       <c r="H12" s="84" t="s">
@@ -57467,7 +58906,7 @@
       <c r="F13" s="80" t="s">
         <v>885</v>
       </c>
-      <c r="G13" s="98" t="s">
+      <c r="G13" s="94" t="s">
         <v>890</v>
       </c>
       <c r="H13" s="81" t="s">
@@ -57486,7 +58925,7 @@
       <c r="F14" s="80" t="s">
         <v>885</v>
       </c>
-      <c r="G14" s="98" t="s">
+      <c r="G14" s="94" t="s">
         <v>890</v>
       </c>
       <c r="H14" s="81" t="s">
@@ -57507,7 +58946,7 @@
       <c r="F15" s="80" t="s">
         <v>894</v>
       </c>
-      <c r="G15" s="98">
+      <c r="G15" s="94">
         <v>43895</v>
       </c>
       <c r="H15" s="81" t="s">
@@ -57526,7 +58965,7 @@
       <c r="F16" s="80" t="s">
         <v>869</v>
       </c>
-      <c r="G16" s="98">
+      <c r="G16" s="94">
         <v>43895</v>
       </c>
       <c r="H16" s="81" t="s">
@@ -57547,7 +58986,7 @@
       <c r="F17" s="82" t="s">
         <v>899</v>
       </c>
-      <c r="G17" s="98">
+      <c r="G17" s="94">
         <v>44017</v>
       </c>
       <c r="H17" s="81" t="s">
@@ -57568,7 +59007,7 @@
       <c r="F18" s="80" t="s">
         <v>902</v>
       </c>
-      <c r="G18" s="98">
+      <c r="G18" s="94">
         <v>44140</v>
       </c>
       <c r="H18" s="81" t="s">
@@ -57624,7 +59063,7 @@
       <c r="B5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="91">
+      <c r="C5" s="96">
         <v>679</v>
       </c>
     </row>
@@ -57632,13 +59071,13 @@
       <c r="B6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="91"/>
+      <c r="C6" s="96"/>
     </row>
     <row r="7" spans="2:3" ht="15" thickBot="1">
       <c r="B7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="92"/>
+      <c r="C7" s="97"/>
     </row>
     <row r="10" spans="2:3">
       <c r="B10" s="85" t="s">
@@ -57656,7 +59095,7 @@
       <c r="B12" s="87" t="s">
         <v>96</v>
       </c>
-      <c r="C12" s="93">
+      <c r="C12" s="98">
         <v>142</v>
       </c>
     </row>
@@ -57664,19 +59103,19 @@
       <c r="B13" s="87" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="93"/>
+      <c r="C13" s="98"/>
     </row>
     <row r="14" spans="2:3">
       <c r="B14" s="87" t="s">
         <v>803</v>
       </c>
-      <c r="C14" s="93"/>
+      <c r="C14" s="98"/>
     </row>
     <row r="15" spans="2:3">
       <c r="B15" s="89" t="s">
         <v>745</v>
       </c>
-      <c r="C15" s="94"/>
+      <c r="C15" s="99"/>
     </row>
     <row r="17" spans="2:3">
       <c r="B17" s="85" t="s">
@@ -57690,7 +59129,7 @@
     </row>
     <row r="19" spans="2:3">
       <c r="B19" s="90"/>
-      <c r="C19" s="93">
+      <c r="C19" s="98">
         <v>128</v>
       </c>
     </row>
@@ -57698,25 +59137,25 @@
       <c r="B20" s="87" t="s">
         <v>506</v>
       </c>
-      <c r="C20" s="93"/>
+      <c r="C20" s="98"/>
     </row>
     <row r="21" spans="2:3">
       <c r="B21" s="87" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="93"/>
+      <c r="C21" s="98"/>
     </row>
     <row r="22" spans="2:3">
       <c r="B22" s="87" t="s">
         <v>449</v>
       </c>
-      <c r="C22" s="93"/>
+      <c r="C22" s="98"/>
     </row>
     <row r="23" spans="2:3">
       <c r="B23" s="89" t="s">
         <v>907</v>
       </c>
-      <c r="C23" s="94"/>
+      <c r="C23" s="99"/>
     </row>
     <row r="25" spans="2:3">
       <c r="B25" s="6" t="s">
@@ -57732,7 +59171,7 @@
       <c r="B27" s="3" t="s">
         <v>654</v>
       </c>
-      <c r="C27" s="91">
+      <c r="C27" s="96">
         <v>87</v>
       </c>
     </row>
@@ -57740,25 +59179,25 @@
       <c r="B28" s="3" t="s">
         <v>632</v>
       </c>
-      <c r="C28" s="91"/>
+      <c r="C28" s="96"/>
     </row>
     <row r="29" spans="2:3">
       <c r="B29" s="3" t="s">
         <v>700</v>
       </c>
-      <c r="C29" s="91"/>
+      <c r="C29" s="96"/>
     </row>
     <row r="30" spans="2:3">
       <c r="B30" s="3" t="s">
         <v>580</v>
       </c>
-      <c r="C30" s="91"/>
+      <c r="C30" s="96"/>
     </row>
     <row r="31" spans="2:3" ht="15" thickBot="1">
       <c r="B31" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="C31" s="92"/>
+      <c r="C31" s="97"/>
     </row>
     <row r="32" spans="2:3" ht="15" thickBot="1"/>
     <row r="33" spans="2:3">
@@ -57775,7 +59214,7 @@
       <c r="B35" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="C35" s="91">
+      <c r="C35" s="96">
         <v>78</v>
       </c>
     </row>
@@ -57783,25 +59222,25 @@
       <c r="B36" s="3" t="s">
         <v>819</v>
       </c>
-      <c r="C36" s="91"/>
+      <c r="C36" s="96"/>
     </row>
     <row r="37" spans="2:3">
       <c r="B37" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C37" s="91"/>
+      <c r="C37" s="96"/>
     </row>
     <row r="38" spans="2:3">
       <c r="B38" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C38" s="91"/>
+      <c r="C38" s="96"/>
     </row>
     <row r="39" spans="2:3" ht="15" thickBot="1">
       <c r="B39" s="5" t="s">
         <v>428</v>
       </c>
-      <c r="C39" s="92"/>
+      <c r="C39" s="97"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-13-2020 14-48-39
</commit_message>
<xml_diff>
--- a/datacovidgt/Casos GT v1.xlsx
+++ b/datacovidgt/Casos GT v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID GT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1084" documentId="8_{9F1230D5-64C1-4EE0-9758-3A2331A06A47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{09465DA5-C599-4FF3-8AEA-03AC7209A716}"/>
+  <xr:revisionPtr revIDLastSave="1222" documentId="8_{9F1230D5-64C1-4EE0-9758-3A2331A06A47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6DC1F214-4DCC-4460-9062-341B89CB8882}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Nuevos " sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5368" uniqueCount="910">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5540" uniqueCount="910">
   <si>
     <t>DIA</t>
   </si>
@@ -2774,11 +2774,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="d/m/yyyy"/>
   </numFmts>
   <fonts count="18">
     <font>
@@ -3321,7 +3322,7 @@
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -3519,6 +3520,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4141,8 +4145,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C7124E47-3D2D-419B-8945-4E2B1598725E}" name="NACIONAL" displayName="NACIONAL" ref="A1:K61" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35" headerRowBorderDxfId="33" tableBorderDxfId="34">
-  <autoFilter ref="A1:K61" xr:uid="{33A3F7D7-6411-4CF7-BF16-EE442911A307}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C7124E47-3D2D-419B-8945-4E2B1598725E}" name="NACIONAL" displayName="NACIONAL" ref="A1:K62" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35" headerRowBorderDxfId="33" tableBorderDxfId="34">
+  <autoFilter ref="A1:K62" xr:uid="{33A3F7D7-6411-4CF7-BF16-EE442911A307}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{D8D5599C-26F8-4B96-A944-93A638641D17}" name="DIA" dataDxfId="32"/>
     <tableColumn id="2" xr3:uid="{352161EA-93C1-4162-BA39-C8F655D430A1}" name="FECHA" dataDxfId="31"/>
@@ -4169,8 +4173,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C2742386-4B94-4797-AF7D-79F889580DBB}" name="Casos_Region3" displayName="Casos_Region3" ref="A2:C102" totalsRowShown="0">
-  <autoFilter ref="A2:C102" xr:uid="{3748EFC6-3E6C-4AD5-BC4D-61D668B7DCC2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C2742386-4B94-4797-AF7D-79F889580DBB}" name="Casos_Region3" displayName="Casos_Region3" ref="A2:C107" totalsRowShown="0">
+  <autoFilter ref="A2:C107" xr:uid="{3748EFC6-3E6C-4AD5-BC4D-61D668B7DCC2}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{95DE0B55-2992-4D1F-9E73-CD885A43DBA7}" name="Fecha?" dataDxfId="21"/>
     <tableColumn id="2" xr3:uid="{5B276D1F-061C-4DB2-A173-70FB0CD1A719}" name="Región"/>
@@ -4181,8 +4185,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{098B8ABD-39CC-481F-B5DD-8A1D47B5485B}" name="Detalle_Casos" displayName="Detalle_Casos" ref="A1:H1115" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" headerRowBorderDxfId="17" tableBorderDxfId="18">
-  <autoFilter ref="A1:H1115" xr:uid="{D721CE67-7EB3-4B8C-BCC9-32CE3BEDA9AC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{098B8ABD-39CC-481F-B5DD-8A1D47B5485B}" name="Detalle_Casos" displayName="Detalle_Casos" ref="A1:H1197" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" headerRowBorderDxfId="17" tableBorderDxfId="18">
+  <autoFilter ref="A1:H1197" xr:uid="{D721CE67-7EB3-4B8C-BCC9-32CE3BEDA9AC}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{65A687D5-CA23-4C97-A29B-DA50B325DBAE}" name="Región COVID">
       <calculatedColumnFormula>+IFERROR(VLOOKUP(B2,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</calculatedColumnFormula>
@@ -4534,8 +4538,8 @@
   </sheetPr>
   <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A36" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+    <sheetView showGridLines="0" topLeftCell="C42" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="J63" sqref="J63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -6913,8 +6917,43 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:12">
-      <c r="D62" s="11"/>
+    <row r="62" spans="1:12" ht="15">
+      <c r="A62" s="61">
+        <v>61</v>
+      </c>
+      <c r="B62" s="95">
+        <v>43963</v>
+      </c>
+      <c r="C62" s="62">
+        <v>85</v>
+      </c>
+      <c r="D62" s="63">
+        <v>1199</v>
+      </c>
+      <c r="E62" s="64">
+        <v>1050</v>
+      </c>
+      <c r="F62" s="65">
+        <v>120</v>
+      </c>
+      <c r="G62" s="66">
+        <v>27</v>
+      </c>
+      <c r="H62" s="62">
+        <f>+F62-F61</f>
+        <v>9</v>
+      </c>
+      <c r="I62" s="67">
+        <f>+G62-G61</f>
+        <v>1</v>
+      </c>
+      <c r="J62" s="68">
+        <f>+NACIONAL[[#This Row],[CONFIRMADOS]]-NACIONAL[[#This Row],[FALLECIDOS]]-NACIONAL[[#This Row],[RECUPERADOS]]</f>
+        <v>1052</v>
+      </c>
+      <c r="K62" s="69">
+        <v>2</v>
+      </c>
     </row>
     <row r="63" spans="1:12">
       <c r="D63" s="11"/>
@@ -6959,8 +6998,8 @@
   </sheetPr>
   <dimension ref="A2:C145"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="L106" sqref="L106"/>
+    <sheetView showGridLines="0" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="D107" sqref="D107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -8081,13 +8120,60 @@
       </c>
     </row>
     <row r="103" spans="1:3">
-      <c r="A103" s="49"/>
+      <c r="A103" s="49">
+        <v>43963</v>
+      </c>
+      <c r="B103" t="s">
+        <v>14</v>
+      </c>
+      <c r="C103">
+        <v>735</v>
+      </c>
     </row>
     <row r="104" spans="1:3">
-      <c r="A104" s="49"/>
-    </row>
-    <row r="106" spans="1:3" ht="15"/>
-    <row r="107" spans="1:3" ht="15"/>
+      <c r="A104" s="49">
+        <v>43963</v>
+      </c>
+      <c r="B104" t="s">
+        <v>15</v>
+      </c>
+      <c r="C104">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" s="49">
+        <v>43963</v>
+      </c>
+      <c r="B105" t="s">
+        <v>16</v>
+      </c>
+      <c r="C105">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="15">
+      <c r="A106" s="49">
+        <v>43963</v>
+      </c>
+      <c r="B106" t="s">
+        <v>17</v>
+      </c>
+      <c r="C106">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="15">
+      <c r="A107" s="49">
+        <v>43963</v>
+      </c>
+      <c r="B107" t="s">
+        <v>18</v>
+      </c>
+      <c r="C107">
+        <v>102</v>
+      </c>
+    </row>
     <row r="108" spans="1:3" ht="15"/>
     <row r="109" spans="1:3" ht="15"/>
     <row r="110" spans="1:3" ht="15"/>
@@ -8140,10 +8226,10 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:H1115"/>
+  <dimension ref="A1:H1197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1095" workbookViewId="0">
-      <selection activeCell="B1051" sqref="B1051:B1113"/>
+    <sheetView tabSelected="1" topLeftCell="A1112" workbookViewId="0">
+      <selection activeCell="H1114" sqref="H1114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -36824,16 +36910,2100 @@
       </c>
     </row>
     <row r="1114" spans="1:8">
-      <c r="C1114" s="90"/>
-      <c r="E1114" s="53"/>
+      <c r="A1114" t="str">
+        <f>+IFERROR(VLOOKUP(B1114,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1114" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1114" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1114">
+        <v>1115</v>
+      </c>
+      <c r="E1114" s="53">
+        <v>1</v>
+      </c>
       <c r="F1114" s="53"/>
-      <c r="G1114" s="53"/>
+      <c r="G1114" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1114">
+        <v>57</v>
+      </c>
     </row>
     <row r="1115" spans="1:8">
-      <c r="C1115" s="90"/>
-      <c r="E1115" s="53"/>
+      <c r="A1115" t="str">
+        <f>+IFERROR(VLOOKUP(B1115,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1115" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1115" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1115">
+        <v>1116</v>
+      </c>
+      <c r="E1115" s="53">
+        <v>1</v>
+      </c>
       <c r="F1115" s="53"/>
-      <c r="G1115" s="53"/>
+      <c r="G1115" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1115">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="1116" spans="1:8" ht="15">
+      <c r="A1116" t="str">
+        <f>+IFERROR(VLOOKUP(B1116,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1116" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1116" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1116">
+        <v>1117</v>
+      </c>
+      <c r="E1116" s="53"/>
+      <c r="F1116" s="53">
+        <v>1</v>
+      </c>
+      <c r="G1116" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1116">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1117" spans="1:8" ht="15">
+      <c r="A1117" t="str">
+        <f>+IFERROR(VLOOKUP(B1117,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1117" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1117" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1117">
+        <v>1118</v>
+      </c>
+      <c r="E1117" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1117" s="53"/>
+      <c r="G1117" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1117">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="1118" spans="1:8" ht="15">
+      <c r="A1118" t="str">
+        <f>+IFERROR(VLOOKUP(B1118,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1118" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1118" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1118">
+        <v>1119</v>
+      </c>
+      <c r="E1118" s="53"/>
+      <c r="F1118" s="53">
+        <v>1</v>
+      </c>
+      <c r="G1118" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1118">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="1119" spans="1:8" ht="15">
+      <c r="A1119" t="str">
+        <f>+IFERROR(VLOOKUP(B1119,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1119" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1119" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1119">
+        <v>1120</v>
+      </c>
+      <c r="E1119" s="53"/>
+      <c r="F1119" s="53">
+        <v>1</v>
+      </c>
+      <c r="G1119" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1119">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1120" spans="1:8" ht="15">
+      <c r="A1120" t="str">
+        <f>+IFERROR(VLOOKUP(B1120,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1120" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1120" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1120">
+        <v>1121</v>
+      </c>
+      <c r="E1120" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1120" s="53"/>
+      <c r="G1120" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1120">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="1121" spans="1:8" ht="15">
+      <c r="A1121" t="str">
+        <f>+IFERROR(VLOOKUP(B1121,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1121" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1121" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1121">
+        <v>1122</v>
+      </c>
+      <c r="E1121" s="53"/>
+      <c r="F1121" s="53">
+        <v>1</v>
+      </c>
+      <c r="G1121" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1121">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1122" spans="1:8" ht="15">
+      <c r="A1122" t="str">
+        <f>+IFERROR(VLOOKUP(B1122,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1122" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1122" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1122">
+        <v>1123</v>
+      </c>
+      <c r="E1122" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1122" s="53"/>
+      <c r="G1122" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1122">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="1123" spans="1:8" ht="15">
+      <c r="A1123" t="str">
+        <f>+IFERROR(VLOOKUP(B1123,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1123" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1123" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1123">
+        <v>1124</v>
+      </c>
+      <c r="E1123" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1123" s="53"/>
+      <c r="G1123" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1124" spans="1:8" ht="15">
+      <c r="A1124" t="str">
+        <f>+IFERROR(VLOOKUP(B1124,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1124" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1124" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1124">
+        <v>1125</v>
+      </c>
+      <c r="E1124" s="53"/>
+      <c r="F1124" s="53">
+        <v>1</v>
+      </c>
+      <c r="G1124" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1124">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="1125" spans="1:8" ht="15">
+      <c r="A1125" t="str">
+        <f>+IFERROR(VLOOKUP(B1125,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1125" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1125" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1125">
+        <v>1126</v>
+      </c>
+      <c r="E1125" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1125" s="53"/>
+      <c r="G1125" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1125">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="1126" spans="1:8" ht="15">
+      <c r="A1126" t="str">
+        <f>+IFERROR(VLOOKUP(B1126,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1126" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1126" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1126">
+        <v>1127</v>
+      </c>
+      <c r="E1126" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1126" s="53"/>
+      <c r="G1126" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1126">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="1127" spans="1:8" ht="15">
+      <c r="A1127" t="str">
+        <f>+IFERROR(VLOOKUP(B1127,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1127" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1127" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1127">
+        <v>1128</v>
+      </c>
+      <c r="E1127" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1127" s="53"/>
+      <c r="G1127" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1127">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1128" spans="1:8" ht="15">
+      <c r="A1128" t="str">
+        <f>+IFERROR(VLOOKUP(B1128,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1128" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1128" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1128">
+        <v>1129</v>
+      </c>
+      <c r="E1128" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1128" s="53"/>
+      <c r="G1128" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1128">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="1129" spans="1:8" ht="15">
+      <c r="A1129" t="str">
+        <f>+IFERROR(VLOOKUP(B1129,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1129" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1129" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1129">
+        <v>1130</v>
+      </c>
+      <c r="E1129" s="53"/>
+      <c r="F1129" s="53">
+        <v>1</v>
+      </c>
+      <c r="G1129" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1129">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="1130" spans="1:8" ht="15">
+      <c r="A1130" t="str">
+        <f>+IFERROR(VLOOKUP(B1130,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1130" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1130" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1130">
+        <v>1131</v>
+      </c>
+      <c r="E1130" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1130" s="53"/>
+      <c r="G1130" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1130">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1131" spans="1:8" ht="15">
+      <c r="A1131" t="str">
+        <f>+IFERROR(VLOOKUP(B1131,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1131" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1131" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1131">
+        <v>1132</v>
+      </c>
+      <c r="E1131" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1131" s="53"/>
+      <c r="G1131" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1131">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="1132" spans="1:8" ht="15">
+      <c r="A1132" t="str">
+        <f>+IFERROR(VLOOKUP(B1132,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1132" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1132" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1132">
+        <v>1133</v>
+      </c>
+      <c r="E1132" s="53"/>
+      <c r="F1132" s="53"/>
+      <c r="G1132" s="53"/>
+      <c r="H1132">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1133" spans="1:8" ht="15">
+      <c r="A1133" t="str">
+        <f>+IFERROR(VLOOKUP(B1133,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1133" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1133" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1133">
+        <v>1134</v>
+      </c>
+      <c r="E1133" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1133" s="53"/>
+      <c r="G1133" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1133">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="1134" spans="1:8" ht="15">
+      <c r="A1134" t="str">
+        <f>+IFERROR(VLOOKUP(B1134,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1134" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1134" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1134">
+        <v>1135</v>
+      </c>
+      <c r="E1134" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1134" s="53"/>
+      <c r="G1134" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1134">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="1135" spans="1:8" ht="15">
+      <c r="A1135" t="str">
+        <f>+IFERROR(VLOOKUP(B1135,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1135" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1135" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1135">
+        <v>1136</v>
+      </c>
+      <c r="E1135" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1135" s="53"/>
+      <c r="G1135" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1135">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1136" spans="1:8" ht="15">
+      <c r="A1136" t="str">
+        <f>+IFERROR(VLOOKUP(B1136,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1136" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1136" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1136">
+        <v>1137</v>
+      </c>
+      <c r="E1136" s="53"/>
+      <c r="F1136" s="53">
+        <v>1</v>
+      </c>
+      <c r="G1136" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1136">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1137" spans="1:8" ht="15">
+      <c r="A1137" t="str">
+        <f>+IFERROR(VLOOKUP(B1137,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1137" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1137" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1137">
+        <v>1138</v>
+      </c>
+      <c r="E1137" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1137" s="53"/>
+      <c r="G1137" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1137">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="1138" spans="1:8" ht="15">
+      <c r="A1138" t="str">
+        <f>+IFERROR(VLOOKUP(B1138,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1138" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1138" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1138">
+        <v>1139</v>
+      </c>
+      <c r="E1138" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1138" s="53"/>
+      <c r="G1138" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1138">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="1139" spans="1:8" ht="15">
+      <c r="A1139" t="str">
+        <f>+IFERROR(VLOOKUP(B1139,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1139" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1139" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1139">
+        <v>1140</v>
+      </c>
+      <c r="E1139" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1139" s="53"/>
+      <c r="G1139" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1139">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1140" spans="1:8" ht="15">
+      <c r="A1140" t="str">
+        <f>+IFERROR(VLOOKUP(B1140,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1140" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1140" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1140">
+        <v>1141</v>
+      </c>
+      <c r="E1140" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1140" s="53"/>
+      <c r="G1140" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1140">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="1141" spans="1:8" ht="15">
+      <c r="A1141" t="str">
+        <f>+IFERROR(VLOOKUP(B1141,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1141" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1141" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1141">
+        <v>1142</v>
+      </c>
+      <c r="E1141" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1141" s="53"/>
+      <c r="G1141" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1141">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1142" spans="1:8" ht="15">
+      <c r="A1142" t="str">
+        <f>+IFERROR(VLOOKUP(B1142,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1142" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1142" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1142">
+        <v>1143</v>
+      </c>
+      <c r="E1142" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1142" s="53"/>
+      <c r="G1142" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1142">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="1143" spans="1:8" ht="15">
+      <c r="A1143" t="str">
+        <f>+IFERROR(VLOOKUP(B1143,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1143" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1143" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1143">
+        <v>1144</v>
+      </c>
+      <c r="E1143" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1143" s="53"/>
+      <c r="G1143" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1143">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="1144" spans="1:8" ht="15">
+      <c r="A1144" t="str">
+        <f>+IFERROR(VLOOKUP(B1144,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1144" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1144" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1144">
+        <v>1145</v>
+      </c>
+      <c r="E1144" s="53"/>
+      <c r="F1144" s="53">
+        <v>1</v>
+      </c>
+      <c r="G1144" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1144">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1145" spans="1:8" ht="15">
+      <c r="A1145" t="str">
+        <f>+IFERROR(VLOOKUP(B1145,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1145" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1145" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1145">
+        <v>1146</v>
+      </c>
+      <c r="E1145" s="53"/>
+      <c r="F1145" s="53">
+        <v>1</v>
+      </c>
+      <c r="G1145" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1145">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1146" spans="1:8" ht="15">
+      <c r="A1146" t="str">
+        <f>+IFERROR(VLOOKUP(B1146,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1146" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1146" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1146">
+        <v>1147</v>
+      </c>
+      <c r="E1146" s="53"/>
+      <c r="F1146" s="53">
+        <v>1</v>
+      </c>
+      <c r="G1146" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1146">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="1147" spans="1:8" ht="15">
+      <c r="A1147" t="str">
+        <f>+IFERROR(VLOOKUP(B1147,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1147" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1147" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1147">
+        <v>1148</v>
+      </c>
+      <c r="E1147" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1147" s="53"/>
+      <c r="G1147" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1147">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="1148" spans="1:8" ht="15">
+      <c r="A1148" t="str">
+        <f>+IFERROR(VLOOKUP(B1148,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1148" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1148" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1148">
+        <v>1149</v>
+      </c>
+      <c r="E1148" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1148" s="53"/>
+      <c r="G1148" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1148">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="1149" spans="1:8" ht="15">
+      <c r="A1149" t="str">
+        <f>+IFERROR(VLOOKUP(B1149,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1149" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1149" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1149">
+        <v>1150</v>
+      </c>
+      <c r="E1149" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1149" s="53"/>
+      <c r="G1149" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1149">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="1150" spans="1:8" ht="15">
+      <c r="A1150" t="str">
+        <f>+IFERROR(VLOOKUP(B1150,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1150" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1150" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1150">
+        <v>1151</v>
+      </c>
+      <c r="E1150" s="53"/>
+      <c r="F1150" s="53">
+        <v>1</v>
+      </c>
+      <c r="G1150" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1150">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="1151" spans="1:8" ht="15">
+      <c r="A1151" t="str">
+        <f>+IFERROR(VLOOKUP(B1151,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1151" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1151" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1151">
+        <v>1152</v>
+      </c>
+      <c r="E1151" s="53"/>
+      <c r="F1151" s="53">
+        <v>1</v>
+      </c>
+      <c r="G1151" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1151">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1152" spans="1:8" ht="15">
+      <c r="A1152" t="str">
+        <f>+IFERROR(VLOOKUP(B1152,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1152" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1152" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1152">
+        <v>1153</v>
+      </c>
+      <c r="E1152" s="53"/>
+      <c r="F1152" s="53">
+        <v>1</v>
+      </c>
+      <c r="G1152" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1152">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="1153" spans="1:8" ht="15">
+      <c r="A1153" t="str">
+        <f>+IFERROR(VLOOKUP(B1153,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1153" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1153" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1153">
+        <v>1154</v>
+      </c>
+      <c r="E1153" s="53"/>
+      <c r="F1153" s="53">
+        <v>1</v>
+      </c>
+      <c r="G1153" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1153">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="1154" spans="1:8" ht="15">
+      <c r="A1154" t="str">
+        <f>+IFERROR(VLOOKUP(B1154,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1154" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1154" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1154">
+        <v>1155</v>
+      </c>
+      <c r="E1154" s="53"/>
+      <c r="F1154" s="53">
+        <v>1</v>
+      </c>
+      <c r="G1154" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1154">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1155" spans="1:8" ht="15">
+      <c r="A1155" t="str">
+        <f>+IFERROR(VLOOKUP(B1155,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1155" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1155" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1155">
+        <v>1156</v>
+      </c>
+      <c r="E1155" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1155" s="53"/>
+      <c r="G1155" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1155">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="1156" spans="1:8" ht="15">
+      <c r="A1156" t="str">
+        <f>+IFERROR(VLOOKUP(B1156,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1156" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1156" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1156">
+        <v>1157</v>
+      </c>
+      <c r="E1156" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1156" s="53"/>
+      <c r="G1156" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1156">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1157" spans="1:8" ht="15">
+      <c r="A1157" t="str">
+        <f>+IFERROR(VLOOKUP(B1157,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1157" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1157" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1157">
+        <v>1158</v>
+      </c>
+      <c r="E1157" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1157" s="53"/>
+      <c r="G1157" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1157">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1158" spans="1:8" ht="15">
+      <c r="A1158" t="str">
+        <f>+IFERROR(VLOOKUP(B1158,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1158" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1158" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1158">
+        <v>1159</v>
+      </c>
+      <c r="E1158" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1158" s="53"/>
+      <c r="G1158" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1158">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="1159" spans="1:8" ht="15">
+      <c r="A1159" t="str">
+        <f>+IFERROR(VLOOKUP(B1159,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1159" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1159" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1159">
+        <v>1160</v>
+      </c>
+      <c r="E1159" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1159" s="53"/>
+      <c r="G1159" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1159">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1160" spans="1:8" ht="15">
+      <c r="A1160" t="str">
+        <f>+IFERROR(VLOOKUP(B1160,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1160" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1160" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1160">
+        <v>1161</v>
+      </c>
+      <c r="E1160" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1160" s="53"/>
+      <c r="G1160" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1160">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1161" spans="1:8" ht="15">
+      <c r="A1161" t="str">
+        <f>+IFERROR(VLOOKUP(B1161,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1161" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1161" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1161">
+        <v>1162</v>
+      </c>
+      <c r="E1161" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1161" s="53"/>
+      <c r="G1161" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1161">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1162" spans="1:8" ht="15">
+      <c r="A1162" t="str">
+        <f>+IFERROR(VLOOKUP(B1162,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1162" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1162" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1162">
+        <v>1164</v>
+      </c>
+      <c r="E1162" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1162" s="53"/>
+      <c r="G1162" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1162">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="1163" spans="1:8" ht="15">
+      <c r="A1163" t="str">
+        <f>+IFERROR(VLOOKUP(B1163,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1163" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1163" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1163">
+        <v>1165</v>
+      </c>
+      <c r="E1163" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1163" s="53"/>
+      <c r="G1163" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1163">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="1164" spans="1:8" ht="15">
+      <c r="A1164" t="str">
+        <f>+IFERROR(VLOOKUP(B1164,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1164" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1164" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1164">
+        <v>1166</v>
+      </c>
+      <c r="E1164" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1164" s="53"/>
+      <c r="G1164" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1164">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="1165" spans="1:8" ht="15">
+      <c r="A1165" t="str">
+        <f>+IFERROR(VLOOKUP(B1165,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1165" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1165" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1165">
+        <v>1167</v>
+      </c>
+      <c r="E1165" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1165" s="53"/>
+      <c r="G1165" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1165">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="1166" spans="1:8" ht="15">
+      <c r="A1166" t="str">
+        <f>+IFERROR(VLOOKUP(B1166,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1166" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1166" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1166">
+        <v>1168</v>
+      </c>
+      <c r="E1166" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1166" s="53"/>
+      <c r="G1166" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1166">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="1167" spans="1:8" ht="15">
+      <c r="A1167" t="str">
+        <f>+IFERROR(VLOOKUP(B1167,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1167" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1167" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1167">
+        <v>1169</v>
+      </c>
+      <c r="E1167" s="53"/>
+      <c r="F1167" s="53">
+        <v>1</v>
+      </c>
+      <c r="G1167" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1167">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1168" spans="1:8" ht="15">
+      <c r="A1168" t="str">
+        <f>+IFERROR(VLOOKUP(B1168,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1168" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1168" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1168">
+        <v>1170</v>
+      </c>
+      <c r="E1168" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1168" s="53"/>
+      <c r="G1168" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1168">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="1169" spans="1:8" ht="15">
+      <c r="A1169" t="str">
+        <f>+IFERROR(VLOOKUP(B1169,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1169" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1169" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1169">
+        <v>1171</v>
+      </c>
+      <c r="E1169" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1169" s="53"/>
+      <c r="G1169" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1169">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1170" spans="1:8" ht="15">
+      <c r="A1170" t="str">
+        <f>+IFERROR(VLOOKUP(B1170,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1170" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1170" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1170">
+        <v>1172</v>
+      </c>
+      <c r="E1170" s="53"/>
+      <c r="F1170" s="53">
+        <v>1</v>
+      </c>
+      <c r="G1170" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1170">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="1171" spans="1:8" ht="15">
+      <c r="A1171" t="str">
+        <f>+IFERROR(VLOOKUP(B1171,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1171" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1171" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1171">
+        <v>1173</v>
+      </c>
+      <c r="E1171" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1171" s="53"/>
+      <c r="G1171" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1171">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1172" spans="1:8" ht="15">
+      <c r="A1172" t="str">
+        <f>+IFERROR(VLOOKUP(B1172,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1172" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1172" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1172">
+        <v>1174</v>
+      </c>
+      <c r="E1172" s="53"/>
+      <c r="F1172" s="53">
+        <v>1</v>
+      </c>
+      <c r="G1172" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1172">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1173" spans="1:8" ht="15">
+      <c r="A1173" t="str">
+        <f>+IFERROR(VLOOKUP(B1173,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1173" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1173" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1173">
+        <v>1175</v>
+      </c>
+      <c r="E1173" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1173" s="53"/>
+      <c r="G1173" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1173">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="1174" spans="1:8" ht="15">
+      <c r="A1174" t="str">
+        <f>+IFERROR(VLOOKUP(B1174,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1174" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1174" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1174">
+        <v>1176</v>
+      </c>
+      <c r="E1174" s="53"/>
+      <c r="F1174" s="53">
+        <v>1</v>
+      </c>
+      <c r="G1174" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1174">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="1175" spans="1:8" ht="15">
+      <c r="A1175" t="str">
+        <f>+IFERROR(VLOOKUP(B1175,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1175" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1175" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1175">
+        <v>1177</v>
+      </c>
+      <c r="E1175" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1175" s="53"/>
+      <c r="G1175" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1175">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="1176" spans="1:8" ht="15">
+      <c r="A1176" t="str">
+        <f>+IFERROR(VLOOKUP(B1176,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1176" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1176" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1176">
+        <v>1178</v>
+      </c>
+      <c r="E1176" s="53"/>
+      <c r="F1176" s="53">
+        <v>1</v>
+      </c>
+      <c r="G1176" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1176">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="1177" spans="1:8" ht="15">
+      <c r="A1177" t="str">
+        <f>+IFERROR(VLOOKUP(B1177,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1177" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1177" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1177">
+        <v>1179</v>
+      </c>
+      <c r="E1177" s="53"/>
+      <c r="F1177" s="53">
+        <v>1</v>
+      </c>
+      <c r="G1177" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1177">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="1178" spans="1:8" ht="15">
+      <c r="A1178" t="str">
+        <f>+IFERROR(VLOOKUP(B1178,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1178" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1178" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1178">
+        <v>1180</v>
+      </c>
+      <c r="E1178" s="53"/>
+      <c r="F1178" s="53">
+        <v>1</v>
+      </c>
+      <c r="G1178" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1178">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="1179" spans="1:8" ht="15">
+      <c r="A1179" t="str">
+        <f>+IFERROR(VLOOKUP(B1179,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1179" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1179" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1179">
+        <v>1181</v>
+      </c>
+      <c r="E1179" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1179" s="53"/>
+      <c r="G1179" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1179">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="1180" spans="1:8" ht="15">
+      <c r="A1180" t="str">
+        <f>+IFERROR(VLOOKUP(B1180,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1180" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1180" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1180">
+        <v>1182</v>
+      </c>
+      <c r="E1180" s="53"/>
+      <c r="F1180" s="53">
+        <v>1</v>
+      </c>
+      <c r="G1180" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1180">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="1181" spans="1:8" ht="15">
+      <c r="A1181" t="str">
+        <f>+IFERROR(VLOOKUP(B1181,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1181" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1181" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1181">
+        <v>1183</v>
+      </c>
+      <c r="E1181" s="53"/>
+      <c r="F1181" s="53">
+        <v>1</v>
+      </c>
+      <c r="G1181" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1181">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1182" spans="1:8" ht="15">
+      <c r="A1182" t="str">
+        <f>+IFERROR(VLOOKUP(B1182,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1182" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1182" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1182">
+        <v>1184</v>
+      </c>
+      <c r="E1182" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1182" s="53"/>
+      <c r="G1182" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1182">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1183" spans="1:8" ht="15">
+      <c r="A1183" t="str">
+        <f>+IFERROR(VLOOKUP(B1183,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1183" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1183" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1183">
+        <v>1185</v>
+      </c>
+      <c r="E1183" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1183" s="53"/>
+      <c r="G1183" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1183">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="1184" spans="1:8" ht="15">
+      <c r="A1184" t="str">
+        <f>+IFERROR(VLOOKUP(B1184,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1184" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1184" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1184">
+        <v>1186</v>
+      </c>
+      <c r="E1184" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1184" s="53"/>
+      <c r="G1184" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1184">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="1185" spans="1:8" ht="15">
+      <c r="A1185" t="str">
+        <f>+IFERROR(VLOOKUP(B1185,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1185" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1185" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1185">
+        <v>1187</v>
+      </c>
+      <c r="E1185" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1185" s="53"/>
+      <c r="G1185" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1185">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="1186" spans="1:8" ht="15">
+      <c r="A1186" t="str">
+        <f>+IFERROR(VLOOKUP(B1186,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1186" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1186" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1186">
+        <v>1188</v>
+      </c>
+      <c r="E1186" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1186" s="53"/>
+      <c r="G1186" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1186">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="1187" spans="1:8" ht="15">
+      <c r="A1187" t="str">
+        <f>+IFERROR(VLOOKUP(B1187,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1187" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1187" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1187">
+        <v>1189</v>
+      </c>
+      <c r="E1187" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1187" s="53"/>
+      <c r="G1187" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1187">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="1188" spans="1:8" ht="15">
+      <c r="A1188" t="str">
+        <f>+IFERROR(VLOOKUP(B1188,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1188" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1188" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1188">
+        <v>1190</v>
+      </c>
+      <c r="E1188" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1188" s="53"/>
+      <c r="G1188" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1188">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="1189" spans="1:8" ht="15">
+      <c r="A1189" t="str">
+        <f>+IFERROR(VLOOKUP(B1189,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1189" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1189" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1189">
+        <v>1191</v>
+      </c>
+      <c r="E1189" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1189" s="53"/>
+      <c r="G1189" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1189">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1190" spans="1:8" ht="15">
+      <c r="A1190" t="str">
+        <f>+IFERROR(VLOOKUP(B1190,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1190" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1190" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1190">
+        <v>1192</v>
+      </c>
+      <c r="E1190" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1190" s="53"/>
+      <c r="G1190" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1190">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1191" spans="1:8" ht="15">
+      <c r="A1191" t="str">
+        <f>+IFERROR(VLOOKUP(B1191,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1191" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1191" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1191">
+        <v>1193</v>
+      </c>
+      <c r="E1191" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1191" s="53"/>
+      <c r="G1191" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1191">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1192" spans="1:8" ht="15">
+      <c r="A1192" t="str">
+        <f>+IFERROR(VLOOKUP(B1192,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1192" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1192" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1192">
+        <v>1194</v>
+      </c>
+      <c r="E1192" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1192" s="53"/>
+      <c r="G1192" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1192">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="1193" spans="1:8" ht="15">
+      <c r="A1193" t="str">
+        <f>+IFERROR(VLOOKUP(B1193,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1193" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1193" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1193">
+        <v>1195</v>
+      </c>
+      <c r="E1193" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1193" s="53"/>
+      <c r="G1193" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1193">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="1194" spans="1:8" ht="15">
+      <c r="A1194" t="str">
+        <f>+IFERROR(VLOOKUP(B1194,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1194" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1194" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1194">
+        <v>1196</v>
+      </c>
+      <c r="E1194" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1194" s="53"/>
+      <c r="G1194" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1194">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1195" spans="1:8" ht="15">
+      <c r="A1195" t="str">
+        <f>+IFERROR(VLOOKUP(B1195,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1195" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1195" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1195">
+        <v>1197</v>
+      </c>
+      <c r="E1195" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1195" s="53"/>
+      <c r="G1195" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1195">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="1196" spans="1:8" ht="15">
+      <c r="A1196" t="str">
+        <f>+IFERROR(VLOOKUP(B1196,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1196" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1196" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1196">
+        <v>1198</v>
+      </c>
+      <c r="E1196" s="53">
+        <v>1</v>
+      </c>
+      <c r="F1196" s="53"/>
+      <c r="G1196" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1196">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="1197" spans="1:8" ht="15">
+      <c r="A1197" t="str">
+        <f>+IFERROR(VLOOKUP(B1197,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1197" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1197" s="90">
+        <v>44170</v>
+      </c>
+      <c r="D1197">
+        <v>1199</v>
+      </c>
+      <c r="E1197" s="53"/>
+      <c r="F1197" s="53">
+        <v>1</v>
+      </c>
+      <c r="G1197" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1197">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -58816,7 +60986,7 @@
       <c r="B5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="95">
+      <c r="C5" s="96">
         <v>679</v>
       </c>
     </row>
@@ -58824,13 +60994,13 @@
       <c r="B6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="95"/>
+      <c r="C6" s="96"/>
     </row>
     <row r="7" spans="2:3" ht="15" thickBot="1">
       <c r="B7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="96"/>
+      <c r="C7" s="97"/>
     </row>
     <row r="10" spans="2:3">
       <c r="B10" s="83" t="s">
@@ -58848,7 +61018,7 @@
       <c r="B12" s="85" t="s">
         <v>96</v>
       </c>
-      <c r="C12" s="97">
+      <c r="C12" s="98">
         <v>142</v>
       </c>
     </row>
@@ -58856,19 +61026,19 @@
       <c r="B13" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="97"/>
+      <c r="C13" s="98"/>
     </row>
     <row r="14" spans="2:3">
       <c r="B14" s="85" t="s">
         <v>803</v>
       </c>
-      <c r="C14" s="97"/>
+      <c r="C14" s="98"/>
     </row>
     <row r="15" spans="2:3">
       <c r="B15" s="87" t="s">
         <v>745</v>
       </c>
-      <c r="C15" s="98"/>
+      <c r="C15" s="99"/>
     </row>
     <row r="17" spans="2:3">
       <c r="B17" s="83" t="s">
@@ -58882,7 +61052,7 @@
     </row>
     <row r="19" spans="2:3">
       <c r="B19" s="88"/>
-      <c r="C19" s="97">
+      <c r="C19" s="98">
         <v>128</v>
       </c>
     </row>
@@ -58890,25 +61060,25 @@
       <c r="B20" s="85" t="s">
         <v>506</v>
       </c>
-      <c r="C20" s="97"/>
+      <c r="C20" s="98"/>
     </row>
     <row r="21" spans="2:3">
       <c r="B21" s="85" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="97"/>
+      <c r="C21" s="98"/>
     </row>
     <row r="22" spans="2:3">
       <c r="B22" s="85" t="s">
         <v>449</v>
       </c>
-      <c r="C22" s="97"/>
+      <c r="C22" s="98"/>
     </row>
     <row r="23" spans="2:3">
       <c r="B23" s="87" t="s">
         <v>907</v>
       </c>
-      <c r="C23" s="98"/>
+      <c r="C23" s="99"/>
     </row>
     <row r="25" spans="2:3">
       <c r="B25" s="6" t="s">
@@ -58924,7 +61094,7 @@
       <c r="B27" s="3" t="s">
         <v>654</v>
       </c>
-      <c r="C27" s="95">
+      <c r="C27" s="96">
         <v>87</v>
       </c>
     </row>
@@ -58932,25 +61102,25 @@
       <c r="B28" s="3" t="s">
         <v>632</v>
       </c>
-      <c r="C28" s="95"/>
+      <c r="C28" s="96"/>
     </row>
     <row r="29" spans="2:3">
       <c r="B29" s="3" t="s">
         <v>700</v>
       </c>
-      <c r="C29" s="95"/>
+      <c r="C29" s="96"/>
     </row>
     <row r="30" spans="2:3">
       <c r="B30" s="3" t="s">
         <v>580</v>
       </c>
-      <c r="C30" s="95"/>
+      <c r="C30" s="96"/>
     </row>
     <row r="31" spans="2:3" ht="15" thickBot="1">
       <c r="B31" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="C31" s="96"/>
+      <c r="C31" s="97"/>
     </row>
     <row r="32" spans="2:3" ht="15" thickBot="1"/>
     <row r="33" spans="2:3">
@@ -58967,7 +61137,7 @@
       <c r="B35" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="C35" s="95">
+      <c r="C35" s="96">
         <v>78</v>
       </c>
     </row>
@@ -58975,25 +61145,25 @@
       <c r="B36" s="3" t="s">
         <v>819</v>
       </c>
-      <c r="C36" s="95"/>
+      <c r="C36" s="96"/>
     </row>
     <row r="37" spans="2:3">
       <c r="B37" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C37" s="95"/>
+      <c r="C37" s="96"/>
     </row>
     <row r="38" spans="2:3">
       <c r="B38" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C38" s="95"/>
+      <c r="C38" s="96"/>
     </row>
     <row r="39" spans="2:3" ht="15" thickBot="1">
       <c r="B39" s="5" t="s">
         <v>428</v>
       </c>
-      <c r="C39" s="96"/>
+      <c r="C39" s="97"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-13-2020 19-00-58
</commit_message>
<xml_diff>
--- a/datacovidgt/Casos GT v1.xlsx
+++ b/datacovidgt/Casos GT v1.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1222" documentId="8_{9F1230D5-64C1-4EE0-9758-3A2331A06A47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6DC1F214-4DCC-4460-9062-341B89CB8882}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Nuevos " sheetId="6" r:id="rId1"/>
@@ -4539,7 +4539,7 @@
   <dimension ref="A1:L71"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="C42" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="J63" sqref="J63"/>
+      <selection activeCell="J71" sqref="J71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -6998,8 +6998,8 @@
   </sheetPr>
   <dimension ref="A2:C145"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="D107" sqref="D107"/>
+    <sheetView showGridLines="0" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="A112" sqref="A112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -8228,8 +8228,8 @@
   </sheetPr>
   <dimension ref="A1:H1197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1112" workbookViewId="0">
-      <selection activeCell="H1114" sqref="H1114"/>
+    <sheetView topLeftCell="A1171" workbookViewId="0">
+      <selection activeCell="H1204" sqref="H1204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -39020,8 +39020,8 @@
   </sheetPr>
   <dimension ref="A1:T342"/>
   <sheetViews>
-    <sheetView topLeftCell="E9" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="E9" workbookViewId="0">
+      <selection activeCell="R43" sqref="R43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-14-2020 07-02-25
</commit_message>
<xml_diff>
--- a/datacovidgt/Casos GT v1.xlsx
+++ b/datacovidgt/Casos GT v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID GT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1227" documentId="8_{9F1230D5-64C1-4EE0-9758-3A2331A06A47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{689AE752-7C63-4DDF-8DB0-E83058F6D952}"/>
+  <xr:revisionPtr revIDLastSave="1331" documentId="8_{9F1230D5-64C1-4EE0-9758-3A2331A06A47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{98F4AFDF-ED92-411A-B16E-A096CD9B9646}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Nuevos " sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5541" uniqueCount="910">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5689" uniqueCount="910">
   <si>
     <t>DIA</t>
   </si>
@@ -4169,8 +4169,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C2742386-4B94-4797-AF7D-79F889580DBB}" name="Casos_Region3" displayName="Casos_Region3" ref="A2:C107" totalsRowShown="0">
-  <autoFilter ref="A2:C107" xr:uid="{3748EFC6-3E6C-4AD5-BC4D-61D668B7DCC2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C2742386-4B94-4797-AF7D-79F889580DBB}" name="Casos_Region3" displayName="Casos_Region3" ref="A2:C112" totalsRowShown="0">
+  <autoFilter ref="A2:C112" xr:uid="{3748EFC6-3E6C-4AD5-BC4D-61D668B7DCC2}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{95DE0B55-2992-4D1F-9E73-CD885A43DBA7}" name="Fecha?" dataDxfId="21"/>
     <tableColumn id="2" xr3:uid="{5B276D1F-061C-4DB2-A173-70FB0CD1A719}" name="Región"/>
@@ -4181,8 +4181,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{098B8ABD-39CC-481F-B5DD-8A1D47B5485B}" name="Detalle_Casos" displayName="Detalle_Casos" ref="A1:H1197" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" headerRowBorderDxfId="17" tableBorderDxfId="18">
-  <autoFilter ref="A1:H1197" xr:uid="{D721CE67-7EB3-4B8C-BCC9-32CE3BEDA9AC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{098B8ABD-39CC-481F-B5DD-8A1D47B5485B}" name="Detalle_Casos" displayName="Detalle_Casos" ref="A1:H1340" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" headerRowBorderDxfId="17" tableBorderDxfId="18">
+  <autoFilter ref="A1:H1340" xr:uid="{D721CE67-7EB3-4B8C-BCC9-32CE3BEDA9AC}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{65A687D5-CA23-4C97-A29B-DA50B325DBAE}" name="Región COVID">
       <calculatedColumnFormula>+IFERROR(VLOOKUP(B2,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</calculatedColumnFormula>
@@ -4534,8 +4534,8 @@
   </sheetPr>
   <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A42" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView showGridLines="0" topLeftCell="A47" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="K66" sqref="K66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -6955,25 +6955,39 @@
       <c r="A63" s="61">
         <v>62</v>
       </c>
-      <c r="B63" s="94"/>
-      <c r="C63" s="62"/>
-      <c r="D63" s="63"/>
-      <c r="E63" s="64"/>
-      <c r="F63" s="65"/>
-      <c r="G63" s="66"/>
+      <c r="B63" s="94">
+        <v>43964</v>
+      </c>
+      <c r="C63" s="62">
+        <v>143</v>
+      </c>
+      <c r="D63" s="63">
+        <v>1342</v>
+      </c>
+      <c r="E63" s="64">
+        <v>1190</v>
+      </c>
+      <c r="F63" s="65">
+        <v>121</v>
+      </c>
+      <c r="G63" s="66">
+        <v>29</v>
+      </c>
       <c r="H63" s="62">
         <f>+F63-F62</f>
-        <v>-120</v>
+        <v>1</v>
       </c>
       <c r="I63" s="67">
         <f>+G63-G62</f>
-        <v>-27</v>
+        <v>2</v>
       </c>
       <c r="J63" s="68">
         <f>+NACIONAL[[#This Row],[CONFIRMADOS]]-NACIONAL[[#This Row],[FALLECIDOS]]-NACIONAL[[#This Row],[RECUPERADOS]]</f>
-        <v>0</v>
-      </c>
-      <c r="K63" s="69"/>
+        <v>1192</v>
+      </c>
+      <c r="K63" s="69">
+        <v>2</v>
+      </c>
     </row>
     <row r="64" spans="1:12">
       <c r="D64" s="11"/>
@@ -7015,8 +7029,8 @@
   </sheetPr>
   <dimension ref="A2:C145"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="A112" sqref="A112"/>
+    <sheetView showGridLines="0" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="A113" sqref="A113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -8191,11 +8205,61 @@
         <v>102</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="15"/>
-    <row r="109" spans="1:3" ht="15"/>
-    <row r="110" spans="1:3" ht="15"/>
-    <row r="111" spans="1:3" ht="15"/>
-    <row r="112" spans="1:3" ht="15" customHeight="1"/>
+    <row r="108" spans="1:3" ht="15">
+      <c r="A108" s="49">
+        <v>43964</v>
+      </c>
+      <c r="B108" t="s">
+        <v>14</v>
+      </c>
+      <c r="C108">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="15">
+      <c r="A109" s="49">
+        <v>43964</v>
+      </c>
+      <c r="B109" t="s">
+        <v>15</v>
+      </c>
+      <c r="C109">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="15">
+      <c r="A110" s="49">
+        <v>43964</v>
+      </c>
+      <c r="B110" t="s">
+        <v>16</v>
+      </c>
+      <c r="C110">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="15">
+      <c r="A111" s="49">
+        <v>43964</v>
+      </c>
+      <c r="B111" t="s">
+        <v>17</v>
+      </c>
+      <c r="C111">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="15" customHeight="1">
+      <c r="A112" s="49">
+        <v>43964</v>
+      </c>
+      <c r="B112" t="s">
+        <v>18</v>
+      </c>
+      <c r="C112">
+        <v>124</v>
+      </c>
+    </row>
     <row r="113" ht="15"/>
     <row r="114" ht="15"/>
     <row r="115" ht="15"/>
@@ -8243,10 +8307,10 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:H1197"/>
+  <dimension ref="A1:H1340"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1119" workbookViewId="0">
-      <selection activeCell="H1132" sqref="H1132"/>
+    <sheetView topLeftCell="A1329" workbookViewId="0">
+      <selection activeCell="D1341" sqref="D1341"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -35323,7 +35387,7 @@
         <v>34</v>
       </c>
       <c r="C1052" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1052">
         <v>1053</v>
@@ -35349,7 +35413,7 @@
         <v>34</v>
       </c>
       <c r="C1053" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1053">
         <v>1054</v>
@@ -35375,7 +35439,7 @@
         <v>34</v>
       </c>
       <c r="C1054" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1054">
         <v>1055</v>
@@ -35401,7 +35465,7 @@
         <v>34</v>
       </c>
       <c r="C1055" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1055">
         <v>1056</v>
@@ -35427,7 +35491,7 @@
         <v>34</v>
       </c>
       <c r="C1056" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1056">
         <v>1057</v>
@@ -35453,7 +35517,7 @@
         <v>34</v>
       </c>
       <c r="C1057" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1057">
         <v>1058</v>
@@ -35479,7 +35543,7 @@
         <v>34</v>
       </c>
       <c r="C1058" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1058">
         <v>1059</v>
@@ -35505,7 +35569,7 @@
         <v>34</v>
       </c>
       <c r="C1059" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1059">
         <v>1060</v>
@@ -35531,7 +35595,7 @@
         <v>34</v>
       </c>
       <c r="C1060" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1060">
         <v>1061</v>
@@ -35557,7 +35621,7 @@
         <v>34</v>
       </c>
       <c r="C1061" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1061">
         <v>1062</v>
@@ -35583,7 +35647,7 @@
         <v>34</v>
       </c>
       <c r="C1062" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1062">
         <v>1063</v>
@@ -35609,7 +35673,7 @@
         <v>34</v>
       </c>
       <c r="C1063" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1063">
         <v>1064</v>
@@ -35635,7 +35699,7 @@
         <v>34</v>
       </c>
       <c r="C1064" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1064">
         <v>1065</v>
@@ -35661,7 +35725,7 @@
         <v>34</v>
       </c>
       <c r="C1065" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1065">
         <v>1066</v>
@@ -35687,7 +35751,7 @@
         <v>34</v>
       </c>
       <c r="C1066" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1066">
         <v>1067</v>
@@ -35713,7 +35777,7 @@
         <v>34</v>
       </c>
       <c r="C1067" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1067">
         <v>1068</v>
@@ -35739,7 +35803,7 @@
         <v>34</v>
       </c>
       <c r="C1068" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1068">
         <v>1069</v>
@@ -35765,7 +35829,7 @@
         <v>34</v>
       </c>
       <c r="C1069" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1069">
         <v>1070</v>
@@ -35791,7 +35855,7 @@
         <v>34</v>
       </c>
       <c r="C1070" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1070">
         <v>1071</v>
@@ -35817,7 +35881,7 @@
         <v>34</v>
       </c>
       <c r="C1071" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1071">
         <v>1072</v>
@@ -35843,7 +35907,7 @@
         <v>34</v>
       </c>
       <c r="C1072" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1072">
         <v>1073</v>
@@ -35869,7 +35933,7 @@
         <v>34</v>
       </c>
       <c r="C1073" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1073">
         <v>1074</v>
@@ -35895,7 +35959,7 @@
         <v>34</v>
       </c>
       <c r="C1074" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1074">
         <v>1075</v>
@@ -35921,7 +35985,7 @@
         <v>34</v>
       </c>
       <c r="C1075" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1075">
         <v>1076</v>
@@ -35947,7 +36011,7 @@
         <v>34</v>
       </c>
       <c r="C1076" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1076">
         <v>1077</v>
@@ -35973,7 +36037,7 @@
         <v>34</v>
       </c>
       <c r="C1077" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1077">
         <v>1078</v>
@@ -35999,7 +36063,7 @@
         <v>34</v>
       </c>
       <c r="C1078" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1078">
         <v>1079</v>
@@ -36025,7 +36089,7 @@
         <v>34</v>
       </c>
       <c r="C1079" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1079">
         <v>1080</v>
@@ -36051,7 +36115,7 @@
         <v>34</v>
       </c>
       <c r="C1080" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1080">
         <v>1081</v>
@@ -36077,7 +36141,7 @@
         <v>34</v>
       </c>
       <c r="C1081" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1081">
         <v>1082</v>
@@ -36103,7 +36167,7 @@
         <v>34</v>
       </c>
       <c r="C1082" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1082">
         <v>1083</v>
@@ -36129,7 +36193,7 @@
         <v>34</v>
       </c>
       <c r="C1083" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1083">
         <v>1084</v>
@@ -36155,7 +36219,7 @@
         <v>34</v>
       </c>
       <c r="C1084" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1084">
         <v>1085</v>
@@ -36181,7 +36245,7 @@
         <v>34</v>
       </c>
       <c r="C1085" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1085">
         <v>1086</v>
@@ -36207,7 +36271,7 @@
         <v>34</v>
       </c>
       <c r="C1086" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1086">
         <v>1087</v>
@@ -36233,7 +36297,7 @@
         <v>34</v>
       </c>
       <c r="C1087" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1087">
         <v>1088</v>
@@ -36259,7 +36323,7 @@
         <v>34</v>
       </c>
       <c r="C1088" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1088">
         <v>1089</v>
@@ -36285,7 +36349,7 @@
         <v>34</v>
       </c>
       <c r="C1089" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1089">
         <v>1090</v>
@@ -36311,7 +36375,7 @@
         <v>34</v>
       </c>
       <c r="C1090" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1090">
         <v>1091</v>
@@ -36337,7 +36401,7 @@
         <v>34</v>
       </c>
       <c r="C1091" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1091">
         <v>1092</v>
@@ -36363,7 +36427,7 @@
         <v>34</v>
       </c>
       <c r="C1092" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1092">
         <v>1093</v>
@@ -36389,7 +36453,7 @@
         <v>34</v>
       </c>
       <c r="C1093" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1093">
         <v>1094</v>
@@ -36415,7 +36479,7 @@
         <v>34</v>
       </c>
       <c r="C1094" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1094">
         <v>1095</v>
@@ -36441,7 +36505,7 @@
         <v>34</v>
       </c>
       <c r="C1095" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1095">
         <v>1096</v>
@@ -36467,7 +36531,7 @@
         <v>34</v>
       </c>
       <c r="C1096" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1096">
         <v>1097</v>
@@ -36493,7 +36557,7 @@
         <v>34</v>
       </c>
       <c r="C1097" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1097">
         <v>1098</v>
@@ -36519,7 +36583,7 @@
         <v>34</v>
       </c>
       <c r="C1098" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1098">
         <v>1099</v>
@@ -36545,7 +36609,7 @@
         <v>34</v>
       </c>
       <c r="C1099" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1099">
         <v>1100</v>
@@ -36571,7 +36635,7 @@
         <v>34</v>
       </c>
       <c r="C1100" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1100">
         <v>1101</v>
@@ -36597,7 +36661,7 @@
         <v>34</v>
       </c>
       <c r="C1101" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1101">
         <v>1102</v>
@@ -36623,7 +36687,7 @@
         <v>34</v>
       </c>
       <c r="C1102" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1102">
         <v>1103</v>
@@ -36649,7 +36713,7 @@
         <v>34</v>
       </c>
       <c r="C1103" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1103">
         <v>1104</v>
@@ -36675,7 +36739,7 @@
         <v>34</v>
       </c>
       <c r="C1104" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1104">
         <v>1105</v>
@@ -36701,7 +36765,7 @@
         <v>34</v>
       </c>
       <c r="C1105" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1105">
         <v>1106</v>
@@ -36727,7 +36791,7 @@
         <v>34</v>
       </c>
       <c r="C1106" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1106">
         <v>1107</v>
@@ -36753,7 +36817,7 @@
         <v>34</v>
       </c>
       <c r="C1107" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1107">
         <v>1108</v>
@@ -36779,7 +36843,7 @@
         <v>34</v>
       </c>
       <c r="C1108" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1108">
         <v>1109</v>
@@ -36805,7 +36869,7 @@
         <v>34</v>
       </c>
       <c r="C1109" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1109">
         <v>1110</v>
@@ -36831,7 +36895,7 @@
         <v>34</v>
       </c>
       <c r="C1110" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1110">
         <v>1111</v>
@@ -36857,7 +36921,7 @@
         <v>34</v>
       </c>
       <c r="C1111" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1111">
         <v>1112</v>
@@ -36883,7 +36947,7 @@
         <v>34</v>
       </c>
       <c r="C1112" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1112">
         <v>1113</v>
@@ -36909,7 +36973,7 @@
         <v>34</v>
       </c>
       <c r="C1113" s="89">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="D1113">
         <v>1114</v>
@@ -36935,7 +36999,7 @@
         <v>34</v>
       </c>
       <c r="C1114" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1114">
         <v>1115</v>
@@ -36960,7 +37024,7 @@
         <v>34</v>
       </c>
       <c r="C1115" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1115">
         <v>1116</v>
@@ -36985,7 +37049,7 @@
         <v>34</v>
       </c>
       <c r="C1116" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1116">
         <v>1117</v>
@@ -37010,7 +37074,7 @@
         <v>34</v>
       </c>
       <c r="C1117" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1117">
         <v>1118</v>
@@ -37035,7 +37099,7 @@
         <v>34</v>
       </c>
       <c r="C1118" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1118">
         <v>1119</v>
@@ -37060,7 +37124,7 @@
         <v>34</v>
       </c>
       <c r="C1119" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1119">
         <v>1120</v>
@@ -37085,7 +37149,7 @@
         <v>34</v>
       </c>
       <c r="C1120" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1120">
         <v>1121</v>
@@ -37110,7 +37174,7 @@
         <v>34</v>
       </c>
       <c r="C1121" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1121">
         <v>1122</v>
@@ -37135,7 +37199,7 @@
         <v>34</v>
       </c>
       <c r="C1122" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1122">
         <v>1123</v>
@@ -37160,7 +37224,7 @@
         <v>34</v>
       </c>
       <c r="C1123" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1123">
         <v>1124</v>
@@ -37185,7 +37249,7 @@
         <v>34</v>
       </c>
       <c r="C1124" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1124">
         <v>1125</v>
@@ -37210,7 +37274,7 @@
         <v>34</v>
       </c>
       <c r="C1125" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1125">
         <v>1126</v>
@@ -37235,7 +37299,7 @@
         <v>34</v>
       </c>
       <c r="C1126" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1126">
         <v>1127</v>
@@ -37260,7 +37324,7 @@
         <v>34</v>
       </c>
       <c r="C1127" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1127">
         <v>1128</v>
@@ -37285,7 +37349,7 @@
         <v>34</v>
       </c>
       <c r="C1128" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1128">
         <v>1129</v>
@@ -37310,7 +37374,7 @@
         <v>34</v>
       </c>
       <c r="C1129" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1129">
         <v>1130</v>
@@ -37335,7 +37399,7 @@
         <v>34</v>
       </c>
       <c r="C1130" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1130">
         <v>1131</v>
@@ -37360,7 +37424,7 @@
         <v>34</v>
       </c>
       <c r="C1131" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1131">
         <v>1132</v>
@@ -37385,7 +37449,7 @@
         <v>34</v>
       </c>
       <c r="C1132" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1132">
         <v>1133</v>
@@ -37410,7 +37474,7 @@
         <v>34</v>
       </c>
       <c r="C1133" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1133">
         <v>1134</v>
@@ -37435,7 +37499,7 @@
         <v>34</v>
       </c>
       <c r="C1134" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1134">
         <v>1135</v>
@@ -37460,7 +37524,7 @@
         <v>34</v>
       </c>
       <c r="C1135" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1135">
         <v>1136</v>
@@ -37485,7 +37549,7 @@
         <v>34</v>
       </c>
       <c r="C1136" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1136">
         <v>1137</v>
@@ -37510,7 +37574,7 @@
         <v>34</v>
       </c>
       <c r="C1137" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1137">
         <v>1138</v>
@@ -37535,7 +37599,7 @@
         <v>34</v>
       </c>
       <c r="C1138" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1138">
         <v>1139</v>
@@ -37560,7 +37624,7 @@
         <v>34</v>
       </c>
       <c r="C1139" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1139">
         <v>1140</v>
@@ -37585,7 +37649,7 @@
         <v>34</v>
       </c>
       <c r="C1140" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1140">
         <v>1141</v>
@@ -37610,7 +37674,7 @@
         <v>34</v>
       </c>
       <c r="C1141" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1141">
         <v>1142</v>
@@ -37635,7 +37699,7 @@
         <v>34</v>
       </c>
       <c r="C1142" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1142">
         <v>1143</v>
@@ -37660,7 +37724,7 @@
         <v>34</v>
       </c>
       <c r="C1143" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1143">
         <v>1144</v>
@@ -37685,7 +37749,7 @@
         <v>34</v>
       </c>
       <c r="C1144" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1144">
         <v>1145</v>
@@ -37710,7 +37774,7 @@
         <v>34</v>
       </c>
       <c r="C1145" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1145">
         <v>1146</v>
@@ -37735,7 +37799,7 @@
         <v>34</v>
       </c>
       <c r="C1146" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1146">
         <v>1147</v>
@@ -37760,7 +37824,7 @@
         <v>34</v>
       </c>
       <c r="C1147" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1147">
         <v>1148</v>
@@ -37785,7 +37849,7 @@
         <v>34</v>
       </c>
       <c r="C1148" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1148">
         <v>1149</v>
@@ -37810,7 +37874,7 @@
         <v>34</v>
       </c>
       <c r="C1149" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1149">
         <v>1150</v>
@@ -37835,7 +37899,7 @@
         <v>34</v>
       </c>
       <c r="C1150" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1150">
         <v>1151</v>
@@ -37860,7 +37924,7 @@
         <v>34</v>
       </c>
       <c r="C1151" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1151">
         <v>1152</v>
@@ -37885,7 +37949,7 @@
         <v>34</v>
       </c>
       <c r="C1152" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1152">
         <v>1153</v>
@@ -37910,7 +37974,7 @@
         <v>34</v>
       </c>
       <c r="C1153" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1153">
         <v>1154</v>
@@ -37935,7 +37999,7 @@
         <v>34</v>
       </c>
       <c r="C1154" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1154">
         <v>1155</v>
@@ -37960,7 +38024,7 @@
         <v>34</v>
       </c>
       <c r="C1155" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1155">
         <v>1156</v>
@@ -37985,7 +38049,7 @@
         <v>34</v>
       </c>
       <c r="C1156" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1156">
         <v>1157</v>
@@ -38010,7 +38074,7 @@
         <v>34</v>
       </c>
       <c r="C1157" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1157">
         <v>1158</v>
@@ -38035,7 +38099,7 @@
         <v>34</v>
       </c>
       <c r="C1158" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1158">
         <v>1159</v>
@@ -38060,7 +38124,7 @@
         <v>34</v>
       </c>
       <c r="C1159" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1159">
         <v>1160</v>
@@ -38085,7 +38149,7 @@
         <v>34</v>
       </c>
       <c r="C1160" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1160">
         <v>1161</v>
@@ -38110,7 +38174,7 @@
         <v>34</v>
       </c>
       <c r="C1161" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1161">
         <v>1162</v>
@@ -38135,7 +38199,7 @@
         <v>34</v>
       </c>
       <c r="C1162" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1162">
         <v>1164</v>
@@ -38160,7 +38224,7 @@
         <v>34</v>
       </c>
       <c r="C1163" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1163">
         <v>1165</v>
@@ -38185,7 +38249,7 @@
         <v>34</v>
       </c>
       <c r="C1164" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1164">
         <v>1166</v>
@@ -38210,7 +38274,7 @@
         <v>34</v>
       </c>
       <c r="C1165" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1165">
         <v>1167</v>
@@ -38235,7 +38299,7 @@
         <v>34</v>
       </c>
       <c r="C1166" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1166">
         <v>1168</v>
@@ -38260,7 +38324,7 @@
         <v>34</v>
       </c>
       <c r="C1167" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1167">
         <v>1169</v>
@@ -38285,7 +38349,7 @@
         <v>34</v>
       </c>
       <c r="C1168" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1168">
         <v>1170</v>
@@ -38310,7 +38374,7 @@
         <v>34</v>
       </c>
       <c r="C1169" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1169">
         <v>1171</v>
@@ -38335,7 +38399,7 @@
         <v>34</v>
       </c>
       <c r="C1170" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1170">
         <v>1172</v>
@@ -38360,7 +38424,7 @@
         <v>34</v>
       </c>
       <c r="C1171" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1171">
         <v>1173</v>
@@ -38385,7 +38449,7 @@
         <v>34</v>
       </c>
       <c r="C1172" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1172">
         <v>1174</v>
@@ -38410,7 +38474,7 @@
         <v>34</v>
       </c>
       <c r="C1173" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1173">
         <v>1175</v>
@@ -38435,7 +38499,7 @@
         <v>34</v>
       </c>
       <c r="C1174" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1174">
         <v>1176</v>
@@ -38460,7 +38524,7 @@
         <v>34</v>
       </c>
       <c r="C1175" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1175">
         <v>1177</v>
@@ -38485,7 +38549,7 @@
         <v>34</v>
       </c>
       <c r="C1176" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1176">
         <v>1178</v>
@@ -38510,7 +38574,7 @@
         <v>34</v>
       </c>
       <c r="C1177" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1177">
         <v>1179</v>
@@ -38535,7 +38599,7 @@
         <v>34</v>
       </c>
       <c r="C1178" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1178">
         <v>1180</v>
@@ -38560,7 +38624,7 @@
         <v>34</v>
       </c>
       <c r="C1179" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1179">
         <v>1181</v>
@@ -38585,7 +38649,7 @@
         <v>34</v>
       </c>
       <c r="C1180" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1180">
         <v>1182</v>
@@ -38610,7 +38674,7 @@
         <v>34</v>
       </c>
       <c r="C1181" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1181">
         <v>1183</v>
@@ -38635,7 +38699,7 @@
         <v>34</v>
       </c>
       <c r="C1182" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1182">
         <v>1184</v>
@@ -38660,7 +38724,7 @@
         <v>34</v>
       </c>
       <c r="C1183" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1183">
         <v>1185</v>
@@ -38685,7 +38749,7 @@
         <v>34</v>
       </c>
       <c r="C1184" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1184">
         <v>1186</v>
@@ -38710,7 +38774,7 @@
         <v>34</v>
       </c>
       <c r="C1185" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1185">
         <v>1187</v>
@@ -38735,7 +38799,7 @@
         <v>34</v>
       </c>
       <c r="C1186" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1186">
         <v>1188</v>
@@ -38760,7 +38824,7 @@
         <v>34</v>
       </c>
       <c r="C1187" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1187">
         <v>1189</v>
@@ -38785,7 +38849,7 @@
         <v>34</v>
       </c>
       <c r="C1188" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1188">
         <v>1190</v>
@@ -38810,7 +38874,7 @@
         <v>34</v>
       </c>
       <c r="C1189" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1189">
         <v>1191</v>
@@ -38835,7 +38899,7 @@
         <v>34</v>
       </c>
       <c r="C1190" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1190">
         <v>1192</v>
@@ -38860,7 +38924,7 @@
         <v>34</v>
       </c>
       <c r="C1191" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1191">
         <v>1193</v>
@@ -38885,7 +38949,7 @@
         <v>34</v>
       </c>
       <c r="C1192" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1192">
         <v>1194</v>
@@ -38910,7 +38974,7 @@
         <v>34</v>
       </c>
       <c r="C1193" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1193">
         <v>1195</v>
@@ -38935,7 +38999,7 @@
         <v>34</v>
       </c>
       <c r="C1194" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1194">
         <v>1196</v>
@@ -38960,7 +39024,7 @@
         <v>34</v>
       </c>
       <c r="C1195" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1195">
         <v>1197</v>
@@ -38985,7 +39049,7 @@
         <v>34</v>
       </c>
       <c r="C1196" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1196">
         <v>1198</v>
@@ -39010,7 +39074,7 @@
         <v>34</v>
       </c>
       <c r="C1197" s="89">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="D1197">
         <v>1199</v>
@@ -39024,6 +39088,3009 @@
       </c>
       <c r="H1197">
         <v>38</v>
+      </c>
+    </row>
+    <row r="1198" spans="1:8" ht="15">
+      <c r="A1198" t="str">
+        <f>+IFERROR(VLOOKUP(B1198,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1198" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1198" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1198">
+        <v>1200</v>
+      </c>
+      <c r="E1198" s="53"/>
+      <c r="F1198" s="53"/>
+      <c r="G1198" s="53" t="str">
+        <f t="shared" ref="G1198:G1229" si="20">+IF(E1198=1,"Masculino","Femenino")</f>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1199" spans="1:8" ht="15">
+      <c r="A1199" t="str">
+        <f>+IFERROR(VLOOKUP(B1199,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1199" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1199" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1199">
+        <v>1201</v>
+      </c>
+      <c r="E1199" s="53"/>
+      <c r="F1199" s="53"/>
+      <c r="G1199" s="53" t="str">
+        <f t="shared" si="20"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1200" spans="1:8" ht="15">
+      <c r="A1200" t="str">
+        <f>+IFERROR(VLOOKUP(B1200,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1200" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1200" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1200">
+        <v>1202</v>
+      </c>
+      <c r="E1200" s="53"/>
+      <c r="F1200" s="53"/>
+      <c r="G1200" s="53" t="str">
+        <f t="shared" si="20"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1201" spans="1:7" ht="15">
+      <c r="A1201" t="str">
+        <f>+IFERROR(VLOOKUP(B1201,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1201" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1201" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1201">
+        <v>1203</v>
+      </c>
+      <c r="E1201" s="53"/>
+      <c r="F1201" s="53"/>
+      <c r="G1201" s="53" t="str">
+        <f t="shared" si="20"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1202" spans="1:7" ht="15">
+      <c r="A1202" t="str">
+        <f>+IFERROR(VLOOKUP(B1202,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1202" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1202" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1202">
+        <v>1204</v>
+      </c>
+      <c r="E1202" s="53"/>
+      <c r="F1202" s="53"/>
+      <c r="G1202" s="53" t="str">
+        <f t="shared" si="20"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1203" spans="1:7" ht="15">
+      <c r="A1203" t="str">
+        <f>+IFERROR(VLOOKUP(B1203,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1203" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1203" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1203">
+        <v>1205</v>
+      </c>
+      <c r="E1203" s="53"/>
+      <c r="F1203" s="53"/>
+      <c r="G1203" s="53" t="str">
+        <f t="shared" si="20"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1204" spans="1:7" ht="15">
+      <c r="A1204" t="str">
+        <f>+IFERROR(VLOOKUP(B1204,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1204" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1204" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1204">
+        <v>1206</v>
+      </c>
+      <c r="E1204" s="53"/>
+      <c r="F1204" s="53"/>
+      <c r="G1204" s="53" t="str">
+        <f t="shared" si="20"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1205" spans="1:7" ht="15">
+      <c r="A1205" t="str">
+        <f>+IFERROR(VLOOKUP(B1205,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1205" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1205" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1205">
+        <v>1207</v>
+      </c>
+      <c r="E1205" s="53"/>
+      <c r="F1205" s="53"/>
+      <c r="G1205" s="53" t="str">
+        <f t="shared" si="20"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1206" spans="1:7" ht="15">
+      <c r="A1206" t="str">
+        <f>+IFERROR(VLOOKUP(B1206,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1206" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1206" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1206">
+        <v>1208</v>
+      </c>
+      <c r="E1206" s="53"/>
+      <c r="F1206" s="53"/>
+      <c r="G1206" s="53" t="str">
+        <f t="shared" si="20"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1207" spans="1:7" ht="15">
+      <c r="A1207" t="str">
+        <f>+IFERROR(VLOOKUP(B1207,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1207" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1207" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1207">
+        <v>1209</v>
+      </c>
+      <c r="E1207" s="53"/>
+      <c r="F1207" s="53"/>
+      <c r="G1207" s="53" t="str">
+        <f t="shared" si="20"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1208" spans="1:7" ht="15">
+      <c r="A1208" t="str">
+        <f>+IFERROR(VLOOKUP(B1208,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1208" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1208" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1208">
+        <v>1210</v>
+      </c>
+      <c r="E1208" s="53"/>
+      <c r="F1208" s="53"/>
+      <c r="G1208" s="53" t="str">
+        <f t="shared" si="20"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1209" spans="1:7" ht="15">
+      <c r="A1209" t="str">
+        <f>+IFERROR(VLOOKUP(B1209,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1209" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1209" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1209">
+        <v>1211</v>
+      </c>
+      <c r="E1209" s="53"/>
+      <c r="F1209" s="53"/>
+      <c r="G1209" s="53" t="str">
+        <f t="shared" si="20"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1210" spans="1:7" ht="15">
+      <c r="A1210" t="str">
+        <f>+IFERROR(VLOOKUP(B1210,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1210" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1210" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1210">
+        <v>1212</v>
+      </c>
+      <c r="E1210" s="53"/>
+      <c r="F1210" s="53"/>
+      <c r="G1210" s="53" t="str">
+        <f t="shared" si="20"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1211" spans="1:7" ht="15">
+      <c r="A1211" t="str">
+        <f>+IFERROR(VLOOKUP(B1211,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1211" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1211" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1211">
+        <v>1213</v>
+      </c>
+      <c r="E1211" s="53"/>
+      <c r="F1211" s="53"/>
+      <c r="G1211" s="53" t="str">
+        <f t="shared" si="20"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1212" spans="1:7" ht="15">
+      <c r="A1212" t="str">
+        <f>+IFERROR(VLOOKUP(B1212,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1212" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1212" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1212">
+        <v>1214</v>
+      </c>
+      <c r="E1212" s="53"/>
+      <c r="F1212" s="53"/>
+      <c r="G1212" s="53" t="str">
+        <f t="shared" si="20"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1213" spans="1:7" ht="15">
+      <c r="A1213" t="str">
+        <f>+IFERROR(VLOOKUP(B1213,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1213" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1213" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1213">
+        <v>1215</v>
+      </c>
+      <c r="E1213" s="53"/>
+      <c r="F1213" s="53"/>
+      <c r="G1213" s="53" t="str">
+        <f t="shared" si="20"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1214" spans="1:7" ht="15">
+      <c r="A1214" t="str">
+        <f>+IFERROR(VLOOKUP(B1214,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1214" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1214" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1214">
+        <v>1216</v>
+      </c>
+      <c r="E1214" s="53"/>
+      <c r="F1214" s="53"/>
+      <c r="G1214" s="53" t="str">
+        <f t="shared" si="20"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1215" spans="1:7" ht="15">
+      <c r="A1215" t="str">
+        <f>+IFERROR(VLOOKUP(B1215,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1215" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1215" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1215">
+        <v>1217</v>
+      </c>
+      <c r="E1215" s="53"/>
+      <c r="F1215" s="53"/>
+      <c r="G1215" s="53" t="str">
+        <f t="shared" si="20"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1216" spans="1:7" ht="15">
+      <c r="A1216" t="str">
+        <f>+IFERROR(VLOOKUP(B1216,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1216" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1216" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1216">
+        <v>1218</v>
+      </c>
+      <c r="E1216" s="53"/>
+      <c r="F1216" s="53"/>
+      <c r="G1216" s="53" t="str">
+        <f t="shared" si="20"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1217" spans="1:7" ht="15">
+      <c r="A1217" t="str">
+        <f>+IFERROR(VLOOKUP(B1217,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1217" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1217" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1217">
+        <v>1219</v>
+      </c>
+      <c r="E1217" s="53"/>
+      <c r="F1217" s="53"/>
+      <c r="G1217" s="53" t="str">
+        <f t="shared" si="20"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1218" spans="1:7" ht="15">
+      <c r="A1218" t="str">
+        <f>+IFERROR(VLOOKUP(B1218,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1218" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1218" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1218">
+        <v>1220</v>
+      </c>
+      <c r="E1218" s="53"/>
+      <c r="F1218" s="53"/>
+      <c r="G1218" s="53" t="str">
+        <f t="shared" si="20"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1219" spans="1:7" ht="15">
+      <c r="A1219" t="str">
+        <f>+IFERROR(VLOOKUP(B1219,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1219" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1219" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1219">
+        <v>1221</v>
+      </c>
+      <c r="E1219" s="53"/>
+      <c r="F1219" s="53"/>
+      <c r="G1219" s="53" t="str">
+        <f t="shared" si="20"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1220" spans="1:7" ht="15">
+      <c r="A1220" t="str">
+        <f>+IFERROR(VLOOKUP(B1220,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1220" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1220" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1220">
+        <v>1222</v>
+      </c>
+      <c r="E1220" s="53"/>
+      <c r="F1220" s="53"/>
+      <c r="G1220" s="53" t="str">
+        <f t="shared" si="20"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1221" spans="1:7" ht="15">
+      <c r="A1221" t="str">
+        <f>+IFERROR(VLOOKUP(B1221,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1221" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1221" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1221">
+        <v>1223</v>
+      </c>
+      <c r="E1221" s="53"/>
+      <c r="F1221" s="53"/>
+      <c r="G1221" s="53" t="str">
+        <f t="shared" si="20"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1222" spans="1:7" ht="15">
+      <c r="A1222" t="str">
+        <f>+IFERROR(VLOOKUP(B1222,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1222" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1222" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1222">
+        <v>1224</v>
+      </c>
+      <c r="E1222" s="53"/>
+      <c r="F1222" s="53"/>
+      <c r="G1222" s="53" t="str">
+        <f t="shared" si="20"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1223" spans="1:7" ht="15">
+      <c r="A1223" t="str">
+        <f>+IFERROR(VLOOKUP(B1223,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1223" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1223" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1223">
+        <v>1225</v>
+      </c>
+      <c r="E1223" s="53"/>
+      <c r="F1223" s="53"/>
+      <c r="G1223" s="53" t="str">
+        <f t="shared" si="20"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1224" spans="1:7" ht="15">
+      <c r="A1224" t="str">
+        <f>+IFERROR(VLOOKUP(B1224,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1224" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1224" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1224">
+        <v>1226</v>
+      </c>
+      <c r="E1224" s="53"/>
+      <c r="F1224" s="53"/>
+      <c r="G1224" s="53" t="str">
+        <f t="shared" si="20"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1225" spans="1:7" ht="15">
+      <c r="A1225" t="str">
+        <f>+IFERROR(VLOOKUP(B1225,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1225" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1225" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1225">
+        <v>1227</v>
+      </c>
+      <c r="E1225" s="53"/>
+      <c r="F1225" s="53"/>
+      <c r="G1225" s="53" t="str">
+        <f t="shared" si="20"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1226" spans="1:7" ht="15">
+      <c r="A1226" t="str">
+        <f>+IFERROR(VLOOKUP(B1226,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1226" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1226" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1226">
+        <v>1228</v>
+      </c>
+      <c r="E1226" s="53"/>
+      <c r="F1226" s="53"/>
+      <c r="G1226" s="53" t="str">
+        <f t="shared" si="20"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1227" spans="1:7" ht="15">
+      <c r="A1227" t="str">
+        <f>+IFERROR(VLOOKUP(B1227,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1227" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1227" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1227">
+        <v>1229</v>
+      </c>
+      <c r="E1227" s="53"/>
+      <c r="F1227" s="53"/>
+      <c r="G1227" s="53" t="str">
+        <f t="shared" si="20"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1228" spans="1:7" ht="15">
+      <c r="A1228" t="str">
+        <f>+IFERROR(VLOOKUP(B1228,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1228" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1228" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1228">
+        <v>1230</v>
+      </c>
+      <c r="E1228" s="53"/>
+      <c r="F1228" s="53"/>
+      <c r="G1228" s="53" t="str">
+        <f t="shared" si="20"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1229" spans="1:7" ht="15">
+      <c r="A1229" t="str">
+        <f>+IFERROR(VLOOKUP(B1229,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1229" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1229" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1229">
+        <v>1231</v>
+      </c>
+      <c r="E1229" s="53"/>
+      <c r="F1229" s="53"/>
+      <c r="G1229" s="53" t="str">
+        <f t="shared" si="20"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1230" spans="1:7" ht="15">
+      <c r="A1230" t="str">
+        <f>+IFERROR(VLOOKUP(B1230,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1230" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1230" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1230">
+        <v>1232</v>
+      </c>
+      <c r="E1230" s="53"/>
+      <c r="F1230" s="53"/>
+      <c r="G1230" s="53" t="str">
+        <f t="shared" ref="G1230:G1261" si="21">+IF(E1230=1,"Masculino","Femenino")</f>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1231" spans="1:7" ht="15">
+      <c r="A1231" t="str">
+        <f>+IFERROR(VLOOKUP(B1231,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1231" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1231" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1231">
+        <v>1233</v>
+      </c>
+      <c r="E1231" s="53"/>
+      <c r="F1231" s="53"/>
+      <c r="G1231" s="53" t="str">
+        <f t="shared" si="21"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1232" spans="1:7" ht="15">
+      <c r="A1232" t="str">
+        <f>+IFERROR(VLOOKUP(B1232,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1232" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1232" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1232">
+        <v>1234</v>
+      </c>
+      <c r="E1232" s="53"/>
+      <c r="F1232" s="53"/>
+      <c r="G1232" s="53" t="str">
+        <f t="shared" si="21"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1233" spans="1:7" ht="15">
+      <c r="A1233" t="str">
+        <f>+IFERROR(VLOOKUP(B1233,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1233" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1233" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1233">
+        <v>1235</v>
+      </c>
+      <c r="E1233" s="53"/>
+      <c r="F1233" s="53"/>
+      <c r="G1233" s="53" t="str">
+        <f t="shared" si="21"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1234" spans="1:7" ht="15">
+      <c r="A1234" t="str">
+        <f>+IFERROR(VLOOKUP(B1234,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1234" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1234" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1234">
+        <v>1236</v>
+      </c>
+      <c r="E1234" s="53"/>
+      <c r="F1234" s="53"/>
+      <c r="G1234" s="53" t="str">
+        <f t="shared" si="21"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1235" spans="1:7" ht="15">
+      <c r="A1235" t="str">
+        <f>+IFERROR(VLOOKUP(B1235,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1235" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1235" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1235">
+        <v>1237</v>
+      </c>
+      <c r="E1235" s="53"/>
+      <c r="F1235" s="53"/>
+      <c r="G1235" s="53" t="str">
+        <f t="shared" si="21"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1236" spans="1:7" ht="15">
+      <c r="A1236" t="str">
+        <f>+IFERROR(VLOOKUP(B1236,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1236" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1236" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1236">
+        <v>1238</v>
+      </c>
+      <c r="E1236" s="53"/>
+      <c r="F1236" s="53"/>
+      <c r="G1236" s="53" t="str">
+        <f t="shared" si="21"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1237" spans="1:7" ht="15">
+      <c r="A1237" t="str">
+        <f>+IFERROR(VLOOKUP(B1237,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1237" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1237" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1237">
+        <v>1239</v>
+      </c>
+      <c r="E1237" s="53"/>
+      <c r="F1237" s="53"/>
+      <c r="G1237" s="53" t="str">
+        <f t="shared" si="21"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1238" spans="1:7" ht="15">
+      <c r="A1238" t="str">
+        <f>+IFERROR(VLOOKUP(B1238,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1238" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1238" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1238">
+        <v>1240</v>
+      </c>
+      <c r="E1238" s="53"/>
+      <c r="F1238" s="53"/>
+      <c r="G1238" s="53" t="str">
+        <f t="shared" si="21"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1239" spans="1:7" ht="15">
+      <c r="A1239" t="str">
+        <f>+IFERROR(VLOOKUP(B1239,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1239" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1239" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1239">
+        <v>1241</v>
+      </c>
+      <c r="E1239" s="53"/>
+      <c r="F1239" s="53"/>
+      <c r="G1239" s="53" t="str">
+        <f t="shared" si="21"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1240" spans="1:7" ht="15">
+      <c r="A1240" t="str">
+        <f>+IFERROR(VLOOKUP(B1240,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1240" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1240" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1240">
+        <v>1242</v>
+      </c>
+      <c r="E1240" s="53"/>
+      <c r="F1240" s="53"/>
+      <c r="G1240" s="53" t="str">
+        <f t="shared" si="21"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1241" spans="1:7" ht="15">
+      <c r="A1241" t="str">
+        <f>+IFERROR(VLOOKUP(B1241,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1241" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1241" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1241">
+        <v>1243</v>
+      </c>
+      <c r="E1241" s="53"/>
+      <c r="F1241" s="53"/>
+      <c r="G1241" s="53" t="str">
+        <f t="shared" si="21"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1242" spans="1:7" ht="15">
+      <c r="A1242" t="str">
+        <f>+IFERROR(VLOOKUP(B1242,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1242" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1242" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1242">
+        <v>1244</v>
+      </c>
+      <c r="E1242" s="53"/>
+      <c r="F1242" s="53"/>
+      <c r="G1242" s="53" t="str">
+        <f t="shared" si="21"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1243" spans="1:7" ht="15">
+      <c r="A1243" t="str">
+        <f>+IFERROR(VLOOKUP(B1243,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1243" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1243" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1243">
+        <v>1245</v>
+      </c>
+      <c r="E1243" s="53"/>
+      <c r="F1243" s="53"/>
+      <c r="G1243" s="53" t="str">
+        <f t="shared" si="21"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1244" spans="1:7" ht="15">
+      <c r="A1244" t="str">
+        <f>+IFERROR(VLOOKUP(B1244,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1244" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1244" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1244">
+        <v>1246</v>
+      </c>
+      <c r="E1244" s="53"/>
+      <c r="F1244" s="53"/>
+      <c r="G1244" s="53" t="str">
+        <f t="shared" si="21"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1245" spans="1:7" ht="15">
+      <c r="A1245" t="str">
+        <f>+IFERROR(VLOOKUP(B1245,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1245" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1245" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1245">
+        <v>1247</v>
+      </c>
+      <c r="E1245" s="53"/>
+      <c r="F1245" s="53"/>
+      <c r="G1245" s="53" t="str">
+        <f t="shared" si="21"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1246" spans="1:7" ht="15">
+      <c r="A1246" t="str">
+        <f>+IFERROR(VLOOKUP(B1246,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1246" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1246" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1246">
+        <v>1248</v>
+      </c>
+      <c r="E1246" s="53"/>
+      <c r="F1246" s="53"/>
+      <c r="G1246" s="53" t="str">
+        <f t="shared" si="21"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1247" spans="1:7" ht="15">
+      <c r="A1247" t="str">
+        <f>+IFERROR(VLOOKUP(B1247,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1247" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1247" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1247">
+        <v>1249</v>
+      </c>
+      <c r="E1247" s="53"/>
+      <c r="F1247" s="53"/>
+      <c r="G1247" s="53" t="str">
+        <f t="shared" si="21"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1248" spans="1:7" ht="15">
+      <c r="A1248" t="str">
+        <f>+IFERROR(VLOOKUP(B1248,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1248" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1248" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1248">
+        <v>1250</v>
+      </c>
+      <c r="E1248" s="53"/>
+      <c r="F1248" s="53"/>
+      <c r="G1248" s="53" t="str">
+        <f t="shared" si="21"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1249" spans="1:7" ht="15">
+      <c r="A1249" t="str">
+        <f>+IFERROR(VLOOKUP(B1249,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1249" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1249" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1249">
+        <v>1251</v>
+      </c>
+      <c r="E1249" s="53"/>
+      <c r="F1249" s="53"/>
+      <c r="G1249" s="53" t="str">
+        <f t="shared" si="21"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1250" spans="1:7" ht="15">
+      <c r="A1250" t="str">
+        <f>+IFERROR(VLOOKUP(B1250,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1250" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1250" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1250">
+        <v>1252</v>
+      </c>
+      <c r="E1250" s="53"/>
+      <c r="F1250" s="53"/>
+      <c r="G1250" s="53" t="str">
+        <f t="shared" si="21"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1251" spans="1:7" ht="15">
+      <c r="A1251" t="str">
+        <f>+IFERROR(VLOOKUP(B1251,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1251" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1251" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1251">
+        <v>1253</v>
+      </c>
+      <c r="E1251" s="53"/>
+      <c r="F1251" s="53"/>
+      <c r="G1251" s="53" t="str">
+        <f t="shared" si="21"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1252" spans="1:7" ht="15">
+      <c r="A1252" t="str">
+        <f>+IFERROR(VLOOKUP(B1252,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1252" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1252" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1252">
+        <v>1254</v>
+      </c>
+      <c r="E1252" s="53"/>
+      <c r="F1252" s="53"/>
+      <c r="G1252" s="53" t="str">
+        <f t="shared" si="21"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1253" spans="1:7" ht="15">
+      <c r="A1253" t="str">
+        <f>+IFERROR(VLOOKUP(B1253,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1253" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1253" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1253">
+        <v>1255</v>
+      </c>
+      <c r="E1253" s="53"/>
+      <c r="F1253" s="53"/>
+      <c r="G1253" s="53" t="str">
+        <f t="shared" si="21"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1254" spans="1:7" ht="15">
+      <c r="A1254" t="str">
+        <f>+IFERROR(VLOOKUP(B1254,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1254" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1254" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1254">
+        <v>1256</v>
+      </c>
+      <c r="E1254" s="53"/>
+      <c r="F1254" s="53"/>
+      <c r="G1254" s="53" t="str">
+        <f t="shared" si="21"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1255" spans="1:7" ht="15">
+      <c r="A1255" t="str">
+        <f>+IFERROR(VLOOKUP(B1255,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1255" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1255" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1255">
+        <v>1257</v>
+      </c>
+      <c r="E1255" s="53"/>
+      <c r="F1255" s="53"/>
+      <c r="G1255" s="53" t="str">
+        <f t="shared" si="21"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1256" spans="1:7" ht="15">
+      <c r="A1256" t="str">
+        <f>+IFERROR(VLOOKUP(B1256,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1256" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1256" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1256">
+        <v>1258</v>
+      </c>
+      <c r="E1256" s="53"/>
+      <c r="F1256" s="53"/>
+      <c r="G1256" s="53" t="str">
+        <f t="shared" si="21"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1257" spans="1:7" ht="15">
+      <c r="A1257" t="str">
+        <f>+IFERROR(VLOOKUP(B1257,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1257" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1257" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1257">
+        <v>1259</v>
+      </c>
+      <c r="E1257" s="53"/>
+      <c r="F1257" s="53"/>
+      <c r="G1257" s="53" t="str">
+        <f t="shared" si="21"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1258" spans="1:7" ht="15">
+      <c r="A1258" t="str">
+        <f>+IFERROR(VLOOKUP(B1258,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1258" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1258" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1258">
+        <v>1260</v>
+      </c>
+      <c r="E1258" s="53"/>
+      <c r="F1258" s="53"/>
+      <c r="G1258" s="53" t="str">
+        <f t="shared" si="21"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1259" spans="1:7" ht="15">
+      <c r="A1259" t="str">
+        <f>+IFERROR(VLOOKUP(B1259,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1259" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1259" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1259">
+        <v>1261</v>
+      </c>
+      <c r="E1259" s="53"/>
+      <c r="F1259" s="53"/>
+      <c r="G1259" s="53" t="str">
+        <f t="shared" si="21"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1260" spans="1:7" ht="15">
+      <c r="A1260" t="str">
+        <f>+IFERROR(VLOOKUP(B1260,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1260" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1260" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1260">
+        <v>1262</v>
+      </c>
+      <c r="E1260" s="53"/>
+      <c r="F1260" s="53"/>
+      <c r="G1260" s="53" t="str">
+        <f t="shared" si="21"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1261" spans="1:7" ht="15">
+      <c r="A1261" t="str">
+        <f>+IFERROR(VLOOKUP(B1261,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1261" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1261" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1261">
+        <v>1263</v>
+      </c>
+      <c r="E1261" s="53"/>
+      <c r="F1261" s="53"/>
+      <c r="G1261" s="53" t="str">
+        <f t="shared" si="21"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1262" spans="1:7" ht="15">
+      <c r="A1262" t="str">
+        <f>+IFERROR(VLOOKUP(B1262,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1262" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1262" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1262">
+        <v>1264</v>
+      </c>
+      <c r="E1262" s="53"/>
+      <c r="F1262" s="53"/>
+      <c r="G1262" s="53" t="str">
+        <f t="shared" ref="G1262:G1293" si="22">+IF(E1262=1,"Masculino","Femenino")</f>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1263" spans="1:7" ht="15">
+      <c r="A1263" t="str">
+        <f>+IFERROR(VLOOKUP(B1263,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1263" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1263" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1263">
+        <v>1265</v>
+      </c>
+      <c r="E1263" s="53"/>
+      <c r="F1263" s="53"/>
+      <c r="G1263" s="53" t="str">
+        <f t="shared" si="22"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1264" spans="1:7" ht="15">
+      <c r="A1264" t="str">
+        <f>+IFERROR(VLOOKUP(B1264,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1264" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1264" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1264">
+        <v>1266</v>
+      </c>
+      <c r="E1264" s="53"/>
+      <c r="F1264" s="53"/>
+      <c r="G1264" s="53" t="str">
+        <f t="shared" si="22"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1265" spans="1:7" ht="15">
+      <c r="A1265" t="str">
+        <f>+IFERROR(VLOOKUP(B1265,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1265" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1265" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1265">
+        <v>1267</v>
+      </c>
+      <c r="E1265" s="53"/>
+      <c r="F1265" s="53"/>
+      <c r="G1265" s="53" t="str">
+        <f t="shared" si="22"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1266" spans="1:7" ht="15">
+      <c r="A1266" t="str">
+        <f>+IFERROR(VLOOKUP(B1266,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1266" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1266" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1266">
+        <v>1268</v>
+      </c>
+      <c r="E1266" s="53"/>
+      <c r="F1266" s="53"/>
+      <c r="G1266" s="53" t="str">
+        <f t="shared" si="22"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1267" spans="1:7" ht="15">
+      <c r="A1267" t="str">
+        <f>+IFERROR(VLOOKUP(B1267,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1267" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1267" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1267">
+        <v>1269</v>
+      </c>
+      <c r="E1267" s="53"/>
+      <c r="F1267" s="53"/>
+      <c r="G1267" s="53" t="str">
+        <f t="shared" si="22"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1268" spans="1:7" ht="15">
+      <c r="A1268" t="str">
+        <f>+IFERROR(VLOOKUP(B1268,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1268" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1268" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1268">
+        <v>1270</v>
+      </c>
+      <c r="E1268" s="53"/>
+      <c r="F1268" s="53"/>
+      <c r="G1268" s="53" t="str">
+        <f t="shared" si="22"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1269" spans="1:7" ht="15">
+      <c r="A1269" t="str">
+        <f>+IFERROR(VLOOKUP(B1269,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1269" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1269" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1269">
+        <v>1271</v>
+      </c>
+      <c r="E1269" s="53"/>
+      <c r="F1269" s="53"/>
+      <c r="G1269" s="53" t="str">
+        <f t="shared" si="22"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1270" spans="1:7" ht="15">
+      <c r="A1270" t="str">
+        <f>+IFERROR(VLOOKUP(B1270,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1270" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1270" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1270">
+        <v>1272</v>
+      </c>
+      <c r="E1270" s="53"/>
+      <c r="F1270" s="53"/>
+      <c r="G1270" s="53" t="str">
+        <f t="shared" si="22"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1271" spans="1:7" ht="15">
+      <c r="A1271" t="str">
+        <f>+IFERROR(VLOOKUP(B1271,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1271" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1271" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1271">
+        <v>1273</v>
+      </c>
+      <c r="E1271" s="53"/>
+      <c r="F1271" s="53"/>
+      <c r="G1271" s="53" t="str">
+        <f t="shared" si="22"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1272" spans="1:7" ht="15">
+      <c r="A1272" t="str">
+        <f>+IFERROR(VLOOKUP(B1272,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1272" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1272" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1272">
+        <v>1274</v>
+      </c>
+      <c r="E1272" s="53"/>
+      <c r="F1272" s="53"/>
+      <c r="G1272" s="53" t="str">
+        <f t="shared" si="22"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1273" spans="1:7" ht="15">
+      <c r="A1273" t="str">
+        <f>+IFERROR(VLOOKUP(B1273,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1273" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1273" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1273">
+        <v>1275</v>
+      </c>
+      <c r="E1273" s="53"/>
+      <c r="F1273" s="53"/>
+      <c r="G1273" s="53" t="str">
+        <f t="shared" si="22"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1274" spans="1:7" ht="15">
+      <c r="A1274" t="str">
+        <f>+IFERROR(VLOOKUP(B1274,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1274" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1274" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1274">
+        <v>1276</v>
+      </c>
+      <c r="E1274" s="53"/>
+      <c r="F1274" s="53"/>
+      <c r="G1274" s="53" t="str">
+        <f t="shared" si="22"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1275" spans="1:7" ht="15">
+      <c r="A1275" t="str">
+        <f>+IFERROR(VLOOKUP(B1275,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1275" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1275" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1275">
+        <v>1277</v>
+      </c>
+      <c r="E1275" s="53"/>
+      <c r="F1275" s="53"/>
+      <c r="G1275" s="53" t="str">
+        <f t="shared" si="22"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1276" spans="1:7" ht="15">
+      <c r="A1276" t="str">
+        <f>+IFERROR(VLOOKUP(B1276,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1276" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1276" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1276">
+        <v>1278</v>
+      </c>
+      <c r="E1276" s="53"/>
+      <c r="F1276" s="53"/>
+      <c r="G1276" s="53" t="str">
+        <f t="shared" si="22"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1277" spans="1:7" ht="15">
+      <c r="A1277" t="str">
+        <f>+IFERROR(VLOOKUP(B1277,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1277" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1277" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1277">
+        <v>1279</v>
+      </c>
+      <c r="E1277" s="53"/>
+      <c r="F1277" s="53"/>
+      <c r="G1277" s="53" t="str">
+        <f t="shared" si="22"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1278" spans="1:7" ht="15">
+      <c r="A1278" t="str">
+        <f>+IFERROR(VLOOKUP(B1278,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1278" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1278" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1278">
+        <v>1280</v>
+      </c>
+      <c r="E1278" s="53"/>
+      <c r="F1278" s="53"/>
+      <c r="G1278" s="53" t="str">
+        <f t="shared" si="22"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1279" spans="1:7" ht="15">
+      <c r="A1279" t="str">
+        <f>+IFERROR(VLOOKUP(B1279,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1279" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1279" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1279">
+        <v>1281</v>
+      </c>
+      <c r="E1279" s="53"/>
+      <c r="F1279" s="53"/>
+      <c r="G1279" s="53" t="str">
+        <f t="shared" si="22"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1280" spans="1:7" ht="15">
+      <c r="A1280" t="str">
+        <f>+IFERROR(VLOOKUP(B1280,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1280" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1280" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1280">
+        <v>1282</v>
+      </c>
+      <c r="E1280" s="53"/>
+      <c r="F1280" s="53"/>
+      <c r="G1280" s="53" t="str">
+        <f t="shared" si="22"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1281" spans="1:7" ht="15">
+      <c r="A1281" t="str">
+        <f>+IFERROR(VLOOKUP(B1281,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1281" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1281" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1281">
+        <v>1283</v>
+      </c>
+      <c r="E1281" s="53"/>
+      <c r="F1281" s="53"/>
+      <c r="G1281" s="53" t="str">
+        <f t="shared" si="22"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1282" spans="1:7" ht="15">
+      <c r="A1282" t="str">
+        <f>+IFERROR(VLOOKUP(B1282,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1282" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1282" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1282">
+        <v>1284</v>
+      </c>
+      <c r="E1282" s="53"/>
+      <c r="F1282" s="53"/>
+      <c r="G1282" s="53" t="str">
+        <f t="shared" si="22"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1283" spans="1:7" ht="15">
+      <c r="A1283" t="str">
+        <f>+IFERROR(VLOOKUP(B1283,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1283" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1283" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1283">
+        <v>1285</v>
+      </c>
+      <c r="E1283" s="53"/>
+      <c r="F1283" s="53"/>
+      <c r="G1283" s="53" t="str">
+        <f t="shared" si="22"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1284" spans="1:7" ht="15">
+      <c r="A1284" t="str">
+        <f>+IFERROR(VLOOKUP(B1284,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1284" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1284" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1284">
+        <v>1286</v>
+      </c>
+      <c r="E1284" s="53"/>
+      <c r="F1284" s="53"/>
+      <c r="G1284" s="53" t="str">
+        <f t="shared" si="22"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1285" spans="1:7" ht="15">
+      <c r="A1285" t="str">
+        <f>+IFERROR(VLOOKUP(B1285,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1285" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1285" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1285">
+        <v>1287</v>
+      </c>
+      <c r="E1285" s="53"/>
+      <c r="F1285" s="53"/>
+      <c r="G1285" s="53" t="str">
+        <f t="shared" si="22"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1286" spans="1:7" ht="15">
+      <c r="A1286" t="str">
+        <f>+IFERROR(VLOOKUP(B1286,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1286" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1286" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1286">
+        <v>1288</v>
+      </c>
+      <c r="E1286" s="53"/>
+      <c r="F1286" s="53"/>
+      <c r="G1286" s="53" t="str">
+        <f t="shared" si="22"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1287" spans="1:7" ht="15">
+      <c r="A1287" t="str">
+        <f>+IFERROR(VLOOKUP(B1287,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1287" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1287" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1287">
+        <v>1289</v>
+      </c>
+      <c r="E1287" s="53"/>
+      <c r="F1287" s="53"/>
+      <c r="G1287" s="53" t="str">
+        <f t="shared" si="22"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1288" spans="1:7" ht="15">
+      <c r="A1288" t="str">
+        <f>+IFERROR(VLOOKUP(B1288,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1288" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1288" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1288">
+        <v>1290</v>
+      </c>
+      <c r="E1288" s="53"/>
+      <c r="F1288" s="53"/>
+      <c r="G1288" s="53" t="str">
+        <f t="shared" si="22"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1289" spans="1:7" ht="15">
+      <c r="A1289" t="str">
+        <f>+IFERROR(VLOOKUP(B1289,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1289" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1289" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1289">
+        <v>1291</v>
+      </c>
+      <c r="E1289" s="53"/>
+      <c r="F1289" s="53"/>
+      <c r="G1289" s="53" t="str">
+        <f t="shared" si="22"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1290" spans="1:7" ht="15">
+      <c r="A1290" t="str">
+        <f>+IFERROR(VLOOKUP(B1290,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1290" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1290" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1290">
+        <v>1292</v>
+      </c>
+      <c r="E1290" s="53"/>
+      <c r="F1290" s="53"/>
+      <c r="G1290" s="53" t="str">
+        <f t="shared" si="22"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1291" spans="1:7" ht="15">
+      <c r="A1291" t="str">
+        <f>+IFERROR(VLOOKUP(B1291,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1291" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1291" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1291">
+        <v>1293</v>
+      </c>
+      <c r="E1291" s="53"/>
+      <c r="F1291" s="53"/>
+      <c r="G1291" s="53" t="str">
+        <f t="shared" si="22"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1292" spans="1:7" ht="15">
+      <c r="A1292" t="str">
+        <f>+IFERROR(VLOOKUP(B1292,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1292" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1292" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1292">
+        <v>1294</v>
+      </c>
+      <c r="E1292" s="53"/>
+      <c r="F1292" s="53"/>
+      <c r="G1292" s="53" t="str">
+        <f t="shared" si="22"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1293" spans="1:7" ht="15">
+      <c r="A1293" t="str">
+        <f>+IFERROR(VLOOKUP(B1293,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1293" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1293" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1293">
+        <v>1295</v>
+      </c>
+      <c r="E1293" s="53"/>
+      <c r="F1293" s="53"/>
+      <c r="G1293" s="53" t="str">
+        <f t="shared" si="22"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1294" spans="1:7" ht="15">
+      <c r="A1294" t="str">
+        <f>+IFERROR(VLOOKUP(B1294,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1294" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1294" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1294">
+        <v>1296</v>
+      </c>
+      <c r="E1294" s="53"/>
+      <c r="F1294" s="53"/>
+      <c r="G1294" s="53" t="str">
+        <f t="shared" ref="G1294:G1325" si="23">+IF(E1294=1,"Masculino","Femenino")</f>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1295" spans="1:7" ht="15">
+      <c r="A1295" t="str">
+        <f>+IFERROR(VLOOKUP(B1295,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1295" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1295" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1295">
+        <v>1297</v>
+      </c>
+      <c r="E1295" s="53"/>
+      <c r="F1295" s="53"/>
+      <c r="G1295" s="53" t="str">
+        <f t="shared" si="23"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1296" spans="1:7" ht="15">
+      <c r="A1296" t="str">
+        <f>+IFERROR(VLOOKUP(B1296,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1296" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1296" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1296">
+        <v>1298</v>
+      </c>
+      <c r="E1296" s="53"/>
+      <c r="F1296" s="53"/>
+      <c r="G1296" s="53" t="str">
+        <f t="shared" si="23"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1297" spans="1:7" ht="15">
+      <c r="A1297" t="str">
+        <f>+IFERROR(VLOOKUP(B1297,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1297" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1297" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1297">
+        <v>1299</v>
+      </c>
+      <c r="E1297" s="53"/>
+      <c r="F1297" s="53"/>
+      <c r="G1297" s="53" t="str">
+        <f t="shared" si="23"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1298" spans="1:7" ht="15">
+      <c r="A1298" t="str">
+        <f>+IFERROR(VLOOKUP(B1298,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1298" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1298" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1298">
+        <v>1300</v>
+      </c>
+      <c r="E1298" s="53"/>
+      <c r="F1298" s="53"/>
+      <c r="G1298" s="53" t="str">
+        <f t="shared" si="23"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1299" spans="1:7" ht="15">
+      <c r="A1299" t="str">
+        <f>+IFERROR(VLOOKUP(B1299,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1299" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1299" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1299">
+        <v>1301</v>
+      </c>
+      <c r="E1299" s="53"/>
+      <c r="F1299" s="53"/>
+      <c r="G1299" s="53" t="str">
+        <f t="shared" si="23"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1300" spans="1:7" ht="15">
+      <c r="A1300" t="str">
+        <f>+IFERROR(VLOOKUP(B1300,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1300" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1300" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1300">
+        <v>1302</v>
+      </c>
+      <c r="E1300" s="53"/>
+      <c r="F1300" s="53"/>
+      <c r="G1300" s="53" t="str">
+        <f t="shared" si="23"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1301" spans="1:7" ht="15">
+      <c r="A1301" t="str">
+        <f>+IFERROR(VLOOKUP(B1301,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1301" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1301" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1301">
+        <v>1303</v>
+      </c>
+      <c r="E1301" s="53"/>
+      <c r="F1301" s="53"/>
+      <c r="G1301" s="53" t="str">
+        <f t="shared" si="23"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1302" spans="1:7" ht="15">
+      <c r="A1302" t="str">
+        <f>+IFERROR(VLOOKUP(B1302,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1302" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1302" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1302">
+        <v>1304</v>
+      </c>
+      <c r="E1302" s="53"/>
+      <c r="F1302" s="53"/>
+      <c r="G1302" s="53" t="str">
+        <f t="shared" si="23"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1303" spans="1:7" ht="15">
+      <c r="A1303" t="str">
+        <f>+IFERROR(VLOOKUP(B1303,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1303" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1303" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1303">
+        <v>1305</v>
+      </c>
+      <c r="E1303" s="53"/>
+      <c r="F1303" s="53"/>
+      <c r="G1303" s="53" t="str">
+        <f t="shared" si="23"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1304" spans="1:7" ht="15">
+      <c r="A1304" t="str">
+        <f>+IFERROR(VLOOKUP(B1304,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1304" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1304" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1304">
+        <v>1306</v>
+      </c>
+      <c r="E1304" s="53"/>
+      <c r="F1304" s="53"/>
+      <c r="G1304" s="53" t="str">
+        <f t="shared" si="23"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1305" spans="1:7" ht="15">
+      <c r="A1305" t="str">
+        <f>+IFERROR(VLOOKUP(B1305,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1305" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1305" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1305">
+        <v>1307</v>
+      </c>
+      <c r="E1305" s="53"/>
+      <c r="F1305" s="53"/>
+      <c r="G1305" s="53" t="str">
+        <f t="shared" si="23"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1306" spans="1:7" ht="15">
+      <c r="A1306" t="str">
+        <f>+IFERROR(VLOOKUP(B1306,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1306" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1306" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1306">
+        <v>1308</v>
+      </c>
+      <c r="E1306" s="53"/>
+      <c r="F1306" s="53"/>
+      <c r="G1306" s="53" t="str">
+        <f t="shared" si="23"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1307" spans="1:7" ht="15">
+      <c r="A1307" t="str">
+        <f>+IFERROR(VLOOKUP(B1307,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1307" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1307" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1307">
+        <v>1309</v>
+      </c>
+      <c r="E1307" s="53"/>
+      <c r="F1307" s="53"/>
+      <c r="G1307" s="53" t="str">
+        <f t="shared" si="23"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1308" spans="1:7" ht="15">
+      <c r="A1308" t="str">
+        <f>+IFERROR(VLOOKUP(B1308,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1308" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1308" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1308">
+        <v>1310</v>
+      </c>
+      <c r="E1308" s="53"/>
+      <c r="F1308" s="53"/>
+      <c r="G1308" s="53" t="str">
+        <f t="shared" si="23"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1309" spans="1:7" ht="15">
+      <c r="A1309" t="str">
+        <f>+IFERROR(VLOOKUP(B1309,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1309" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1309" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1309">
+        <v>1311</v>
+      </c>
+      <c r="E1309" s="53"/>
+      <c r="F1309" s="53"/>
+      <c r="G1309" s="53" t="str">
+        <f t="shared" si="23"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1310" spans="1:7" ht="15">
+      <c r="A1310" t="str">
+        <f>+IFERROR(VLOOKUP(B1310,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1310" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1310" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1310">
+        <v>1312</v>
+      </c>
+      <c r="E1310" s="53"/>
+      <c r="F1310" s="53"/>
+      <c r="G1310" s="53" t="str">
+        <f t="shared" si="23"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1311" spans="1:7" ht="15">
+      <c r="A1311" t="str">
+        <f>+IFERROR(VLOOKUP(B1311,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1311" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1311" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1311">
+        <v>1313</v>
+      </c>
+      <c r="E1311" s="53"/>
+      <c r="F1311" s="53"/>
+      <c r="G1311" s="53" t="str">
+        <f t="shared" si="23"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1312" spans="1:7" ht="15">
+      <c r="A1312" t="str">
+        <f>+IFERROR(VLOOKUP(B1312,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1312" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1312" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1312">
+        <v>1314</v>
+      </c>
+      <c r="E1312" s="53"/>
+      <c r="F1312" s="53"/>
+      <c r="G1312" s="53" t="str">
+        <f t="shared" si="23"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1313" spans="1:7" ht="15">
+      <c r="A1313" t="str">
+        <f>+IFERROR(VLOOKUP(B1313,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1313" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1313" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1313">
+        <v>1315</v>
+      </c>
+      <c r="E1313" s="53"/>
+      <c r="F1313" s="53"/>
+      <c r="G1313" s="53" t="str">
+        <f t="shared" si="23"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1314" spans="1:7" ht="15">
+      <c r="A1314" t="str">
+        <f>+IFERROR(VLOOKUP(B1314,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1314" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1314" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1314">
+        <v>1316</v>
+      </c>
+      <c r="E1314" s="53"/>
+      <c r="F1314" s="53"/>
+      <c r="G1314" s="53" t="str">
+        <f t="shared" si="23"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1315" spans="1:7" ht="15">
+      <c r="A1315" t="str">
+        <f>+IFERROR(VLOOKUP(B1315,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1315" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1315" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1315">
+        <v>1317</v>
+      </c>
+      <c r="E1315" s="53"/>
+      <c r="F1315" s="53"/>
+      <c r="G1315" s="53" t="str">
+        <f t="shared" si="23"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1316" spans="1:7" ht="15">
+      <c r="A1316" t="str">
+        <f>+IFERROR(VLOOKUP(B1316,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1316" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1316" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1316">
+        <v>1318</v>
+      </c>
+      <c r="E1316" s="53"/>
+      <c r="F1316" s="53"/>
+      <c r="G1316" s="53" t="str">
+        <f t="shared" si="23"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1317" spans="1:7" ht="15">
+      <c r="A1317" t="str">
+        <f>+IFERROR(VLOOKUP(B1317,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1317" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1317" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1317">
+        <v>1319</v>
+      </c>
+      <c r="E1317" s="53"/>
+      <c r="F1317" s="53"/>
+      <c r="G1317" s="53" t="str">
+        <f t="shared" si="23"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1318" spans="1:7" ht="15">
+      <c r="A1318" t="str">
+        <f>+IFERROR(VLOOKUP(B1318,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1318" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1318" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1318">
+        <v>1320</v>
+      </c>
+      <c r="E1318" s="53"/>
+      <c r="F1318" s="53"/>
+      <c r="G1318" s="53" t="str">
+        <f t="shared" si="23"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1319" spans="1:7" ht="15">
+      <c r="A1319" t="str">
+        <f>+IFERROR(VLOOKUP(B1319,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1319" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1319" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1319">
+        <v>1321</v>
+      </c>
+      <c r="E1319" s="53"/>
+      <c r="F1319" s="53"/>
+      <c r="G1319" s="53" t="str">
+        <f t="shared" si="23"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1320" spans="1:7" ht="15">
+      <c r="A1320" t="str">
+        <f>+IFERROR(VLOOKUP(B1320,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1320" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1320" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1320">
+        <v>1322</v>
+      </c>
+      <c r="E1320" s="53"/>
+      <c r="F1320" s="53"/>
+      <c r="G1320" s="53" t="str">
+        <f t="shared" si="23"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1321" spans="1:7" ht="15">
+      <c r="A1321" t="str">
+        <f>+IFERROR(VLOOKUP(B1321,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1321" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1321" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1321">
+        <v>1323</v>
+      </c>
+      <c r="E1321" s="53"/>
+      <c r="F1321" s="53"/>
+      <c r="G1321" s="53" t="str">
+        <f t="shared" si="23"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1322" spans="1:7" ht="15">
+      <c r="A1322" t="str">
+        <f>+IFERROR(VLOOKUP(B1322,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1322" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1322" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1322">
+        <v>1324</v>
+      </c>
+      <c r="E1322" s="53"/>
+      <c r="F1322" s="53"/>
+      <c r="G1322" s="53" t="str">
+        <f t="shared" si="23"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1323" spans="1:7" ht="15">
+      <c r="A1323" t="str">
+        <f>+IFERROR(VLOOKUP(B1323,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1323" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1323" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1323">
+        <v>1325</v>
+      </c>
+      <c r="E1323" s="53"/>
+      <c r="F1323" s="53"/>
+      <c r="G1323" s="53" t="str">
+        <f t="shared" si="23"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1324" spans="1:7" ht="15">
+      <c r="A1324" t="str">
+        <f>+IFERROR(VLOOKUP(B1324,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1324" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1324" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1324">
+        <v>1326</v>
+      </c>
+      <c r="E1324" s="53"/>
+      <c r="F1324" s="53"/>
+      <c r="G1324" s="53" t="str">
+        <f t="shared" si="23"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1325" spans="1:7" ht="15">
+      <c r="A1325" t="str">
+        <f>+IFERROR(VLOOKUP(B1325,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1325" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1325" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1325">
+        <v>1327</v>
+      </c>
+      <c r="E1325" s="53"/>
+      <c r="F1325" s="53"/>
+      <c r="G1325" s="53" t="str">
+        <f t="shared" si="23"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1326" spans="1:7" ht="15">
+      <c r="A1326" t="str">
+        <f>+IFERROR(VLOOKUP(B1326,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1326" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1326" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1326">
+        <v>1328</v>
+      </c>
+      <c r="E1326" s="53"/>
+      <c r="F1326" s="53"/>
+      <c r="G1326" s="53" t="str">
+        <f t="shared" ref="G1326:G1340" si="24">+IF(E1326=1,"Masculino","Femenino")</f>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1327" spans="1:7" ht="15">
+      <c r="A1327" t="str">
+        <f>+IFERROR(VLOOKUP(B1327,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1327" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1327" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1327">
+        <v>1329</v>
+      </c>
+      <c r="E1327" s="53"/>
+      <c r="F1327" s="53"/>
+      <c r="G1327" s="53" t="str">
+        <f t="shared" si="24"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1328" spans="1:7" ht="15">
+      <c r="A1328" t="str">
+        <f>+IFERROR(VLOOKUP(B1328,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1328" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1328" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1328">
+        <v>1330</v>
+      </c>
+      <c r="E1328" s="53"/>
+      <c r="F1328" s="53"/>
+      <c r="G1328" s="53" t="str">
+        <f t="shared" si="24"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1329" spans="1:7" ht="15">
+      <c r="A1329" t="str">
+        <f>+IFERROR(VLOOKUP(B1329,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1329" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1329" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1329">
+        <v>1331</v>
+      </c>
+      <c r="E1329" s="53"/>
+      <c r="F1329" s="53"/>
+      <c r="G1329" s="53" t="str">
+        <f t="shared" si="24"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1330" spans="1:7" ht="15">
+      <c r="A1330" t="str">
+        <f>+IFERROR(VLOOKUP(B1330,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1330" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1330" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1330">
+        <v>1332</v>
+      </c>
+      <c r="E1330" s="53"/>
+      <c r="F1330" s="53"/>
+      <c r="G1330" s="53" t="str">
+        <f t="shared" si="24"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1331" spans="1:7" ht="15">
+      <c r="A1331" t="str">
+        <f>+IFERROR(VLOOKUP(B1331,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1331" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1331" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1331">
+        <v>1333</v>
+      </c>
+      <c r="E1331" s="53"/>
+      <c r="F1331" s="53"/>
+      <c r="G1331" s="53" t="str">
+        <f t="shared" si="24"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1332" spans="1:7" ht="15">
+      <c r="A1332" t="str">
+        <f>+IFERROR(VLOOKUP(B1332,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1332" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1332" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1332">
+        <v>1334</v>
+      </c>
+      <c r="E1332" s="53"/>
+      <c r="F1332" s="53"/>
+      <c r="G1332" s="53" t="str">
+        <f t="shared" si="24"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1333" spans="1:7" ht="15">
+      <c r="A1333" t="str">
+        <f>+IFERROR(VLOOKUP(B1333,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1333" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1333" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1333">
+        <v>1335</v>
+      </c>
+      <c r="E1333" s="53"/>
+      <c r="F1333" s="53"/>
+      <c r="G1333" s="53" t="str">
+        <f t="shared" si="24"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1334" spans="1:7" ht="15">
+      <c r="A1334" t="str">
+        <f>+IFERROR(VLOOKUP(B1334,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1334" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1334" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1334">
+        <v>1336</v>
+      </c>
+      <c r="E1334" s="53"/>
+      <c r="F1334" s="53"/>
+      <c r="G1334" s="53" t="str">
+        <f t="shared" si="24"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1335" spans="1:7" ht="15">
+      <c r="A1335" t="str">
+        <f>+IFERROR(VLOOKUP(B1335,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1335" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1335" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1335">
+        <v>1337</v>
+      </c>
+      <c r="E1335" s="53"/>
+      <c r="F1335" s="53"/>
+      <c r="G1335" s="53" t="str">
+        <f t="shared" si="24"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1336" spans="1:7" ht="15">
+      <c r="A1336" t="str">
+        <f>+IFERROR(VLOOKUP(B1336,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1336" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1336" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1336">
+        <v>1338</v>
+      </c>
+      <c r="E1336" s="53"/>
+      <c r="F1336" s="53"/>
+      <c r="G1336" s="53" t="str">
+        <f t="shared" si="24"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1337" spans="1:7" ht="15">
+      <c r="A1337" t="str">
+        <f>+IFERROR(VLOOKUP(B1337,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1337" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1337" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1337">
+        <v>1339</v>
+      </c>
+      <c r="E1337" s="53"/>
+      <c r="F1337" s="53"/>
+      <c r="G1337" s="53" t="str">
+        <f t="shared" si="24"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1338" spans="1:7" ht="15">
+      <c r="A1338" t="str">
+        <f>+IFERROR(VLOOKUP(B1338,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1338" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1338" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1338">
+        <v>1340</v>
+      </c>
+      <c r="E1338" s="53"/>
+      <c r="F1338" s="53"/>
+      <c r="G1338" s="53" t="str">
+        <f t="shared" si="24"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1339" spans="1:7" ht="15">
+      <c r="A1339" t="str">
+        <f>+IFERROR(VLOOKUP(B1339,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1339" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1339" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1339">
+        <v>1341</v>
+      </c>
+      <c r="E1339" s="53"/>
+      <c r="F1339" s="53"/>
+      <c r="G1339" s="53" t="str">
+        <f t="shared" si="24"/>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="1340" spans="1:7" ht="15">
+      <c r="A1340" t="str">
+        <f>+IFERROR(VLOOKUP(B1340,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1340" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1340" s="89">
+        <v>43964</v>
+      </c>
+      <c r="D1340">
+        <v>1342</v>
+      </c>
+      <c r="E1340" s="53"/>
+      <c r="F1340" s="53"/>
+      <c r="G1340" s="53" t="str">
+        <f t="shared" si="24"/>
+        <v>Femenino</v>
       </c>
     </row>
   </sheetData>
@@ -39041,7 +42108,7 @@
   </sheetPr>
   <dimension ref="A1:T342"/>
   <sheetViews>
-    <sheetView topLeftCell="E145" workbookViewId="0">
+    <sheetView topLeftCell="G43" workbookViewId="0">
       <selection activeCell="R43" sqref="R43"/>
     </sheetView>
   </sheetViews>
@@ -60617,7 +63684,7 @@
   <dimension ref="B2:H18"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -60892,7 +63959,7 @@
         <v>894</v>
       </c>
       <c r="G15" s="91">
-        <v>43895</v>
+        <v>43954</v>
       </c>
       <c r="H15" s="79" t="s">
         <v>895</v>
@@ -60911,7 +63978,7 @@
         <v>869</v>
       </c>
       <c r="G16" s="91">
-        <v>43895</v>
+        <v>43954</v>
       </c>
       <c r="H16" s="79" t="s">
         <v>897</v>
@@ -60932,7 +63999,7 @@
         <v>899</v>
       </c>
       <c r="G17" s="91">
-        <v>44017</v>
+        <v>43958</v>
       </c>
       <c r="H17" s="79" t="s">
         <v>900</v>
@@ -60953,7 +64020,7 @@
         <v>902</v>
       </c>
       <c r="G18" s="91">
-        <v>44140</v>
+        <v>43962</v>
       </c>
       <c r="H18" s="79" t="s">
         <v>903</v>
@@ -60983,8 +64050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B2:C39"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -61008,7 +64075,7 @@
         <v>33</v>
       </c>
       <c r="C5" s="95">
-        <v>679</v>
+        <v>833</v>
       </c>
     </row>
     <row r="6" spans="2:3">
@@ -61040,7 +64107,7 @@
         <v>96</v>
       </c>
       <c r="C12" s="97">
-        <v>142</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="2:3">
@@ -61074,7 +64141,7 @@
     <row r="19" spans="2:3">
       <c r="B19" s="88"/>
       <c r="C19" s="97">
-        <v>128</v>
+        <v>143</v>
       </c>
     </row>
     <row r="20" spans="2:3">
@@ -61159,7 +64226,7 @@
         <v>190</v>
       </c>
       <c r="C35" s="95">
-        <v>78</v>
+        <v>124</v>
       </c>
     </row>
     <row r="36" spans="2:3">

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-17-2020 07-11-14
</commit_message>
<xml_diff>
--- a/datacovidgt/Casos GT v1.xlsx
+++ b/datacovidgt/Casos GT v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID GT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2878" documentId="8_{9F1230D5-64C1-4EE0-9758-3A2331A06A47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{278C88BE-DF7F-476B-82B2-A1DC26D4D6F0}"/>
+  <xr:revisionPtr revIDLastSave="2960" documentId="8_{9F1230D5-64C1-4EE0-9758-3A2331A06A47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5FBBCBD8-859A-440D-A13D-E96B278D2DFA}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="5" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Nuevos " sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7291" uniqueCount="947">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7411" uniqueCount="947">
   <si>
     <t>DIA</t>
   </si>
@@ -2869,10 +2869,10 @@
     <t>REGION 2</t>
   </si>
   <si>
+    <t>Totonicapan</t>
+  </si>
+  <si>
     <t>REGION 3</t>
-  </si>
-  <si>
-    <t>Totonicapan</t>
   </si>
   <si>
     <t>REGION 4</t>
@@ -3047,7 +3047,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -3420,6 +3420,61 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -3427,7 +3482,7 @@
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -3626,6 +3681,17 @@
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3638,6 +3704,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -4640,8 +4707,8 @@
   </sheetPr>
   <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E50" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="K68" sqref="K68"/>
+    <sheetView showGridLines="0" topLeftCell="A51" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H69" sqref="H69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -8668,10 +8735,10 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:H1642"/>
+  <dimension ref="A1:H1793"/>
   <sheetViews>
-    <sheetView topLeftCell="A1622" workbookViewId="0">
-      <selection activeCell="C1186" sqref="C1186"/>
+    <sheetView tabSelected="1" topLeftCell="A1713" workbookViewId="0">
+      <selection activeCell="H1718" sqref="H1718"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -48696,7 +48763,7 @@
         <v>1</v>
       </c>
       <c r="G1613" s="52" t="str">
-        <f t="shared" ref="G1613:G1641" si="23">+IF(E1613=1,"Masculino","Femenino")</f>
+        <f t="shared" ref="G1613:G1676" si="23">+IF(E1613=1,"Masculino","Femenino")</f>
         <v>Femenino</v>
       </c>
     </row>
@@ -49137,7 +49204,7 @@
         <v>Femenino</v>
       </c>
     </row>
-    <row r="1633" spans="1:7" ht="15">
+    <row r="1633" spans="1:8" ht="15">
       <c r="A1633" t="str">
         <f>+IFERROR(VLOOKUP(B1633,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
@@ -49160,7 +49227,7 @@
         <v>Femenino</v>
       </c>
     </row>
-    <row r="1634" spans="1:7" ht="15">
+    <row r="1634" spans="1:8" ht="15">
       <c r="A1634" t="str">
         <f>+IFERROR(VLOOKUP(B1634,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
@@ -49183,7 +49250,7 @@
         <v>Femenino</v>
       </c>
     </row>
-    <row r="1635" spans="1:7" ht="15">
+    <row r="1635" spans="1:8" ht="15">
       <c r="A1635" t="str">
         <f>+IFERROR(VLOOKUP(B1635,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
@@ -49206,7 +49273,7 @@
         <v>Femenino</v>
       </c>
     </row>
-    <row r="1636" spans="1:7" ht="15">
+    <row r="1636" spans="1:8" ht="15">
       <c r="A1636" t="str">
         <f>+IFERROR(VLOOKUP(B1636,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
@@ -49229,7 +49296,7 @@
         <v>Femenino</v>
       </c>
     </row>
-    <row r="1637" spans="1:7" ht="15">
+    <row r="1637" spans="1:8" ht="15">
       <c r="A1637" t="str">
         <f>+IFERROR(VLOOKUP(B1637,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
@@ -49252,7 +49319,7 @@
         <v>Femenino</v>
       </c>
     </row>
-    <row r="1638" spans="1:7" ht="15">
+    <row r="1638" spans="1:8" ht="15">
       <c r="A1638" t="str">
         <f>+IFERROR(VLOOKUP(B1638,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
@@ -49275,7 +49342,7 @@
         <v>Femenino</v>
       </c>
     </row>
-    <row r="1639" spans="1:7" ht="15">
+    <row r="1639" spans="1:8" ht="15">
       <c r="A1639" t="str">
         <f>+IFERROR(VLOOKUP(B1639,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
@@ -49298,7 +49365,7 @@
         <v>Femenino</v>
       </c>
     </row>
-    <row r="1640" spans="1:7" ht="15">
+    <row r="1640" spans="1:8" ht="15">
       <c r="A1640" t="str">
         <f>+IFERROR(VLOOKUP(B1640,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
@@ -49321,7 +49388,7 @@
         <v>Femenino</v>
       </c>
     </row>
-    <row r="1641" spans="1:7" ht="15">
+    <row r="1641" spans="1:8" ht="15">
       <c r="A1641" t="str">
         <f>+IFERROR(VLOOKUP(B1641,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
         <v>No Informado</v>
@@ -49344,7 +49411,2982 @@
         <v>Femenino</v>
       </c>
     </row>
-    <row r="1642" spans="1:7" ht="15"/>
+    <row r="1642" spans="1:8" ht="15">
+      <c r="A1642" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1642,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1642" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1642,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1642" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1642">
+        <v>1644</v>
+      </c>
+      <c r="E1642">
+        <v>1</v>
+      </c>
+      <c r="G1642" s="94" t="str">
+        <f t="shared" si="23"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1642" s="103"/>
+    </row>
+    <row r="1643" spans="1:8" ht="15">
+      <c r="A1643" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1643,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1643" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1643,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1643" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1643">
+        <v>1645</v>
+      </c>
+      <c r="E1643">
+        <v>1</v>
+      </c>
+      <c r="G1643" s="94" t="str">
+        <f t="shared" si="23"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1643" s="103"/>
+    </row>
+    <row r="1644" spans="1:8" ht="15">
+      <c r="A1644" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1644,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1644" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1644,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1644" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1644">
+        <v>1646</v>
+      </c>
+      <c r="E1644">
+        <v>1</v>
+      </c>
+      <c r="G1644" s="94" t="str">
+        <f t="shared" si="23"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1644" s="103"/>
+    </row>
+    <row r="1645" spans="1:8" ht="15">
+      <c r="A1645" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1645,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1645" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1645,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1645" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1645">
+        <v>1647</v>
+      </c>
+      <c r="E1645">
+        <v>1</v>
+      </c>
+      <c r="G1645" s="94" t="str">
+        <f t="shared" si="23"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1645" s="103"/>
+    </row>
+    <row r="1646" spans="1:8" ht="15">
+      <c r="A1646" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1646,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1646" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1646,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1646" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1646">
+        <v>1648</v>
+      </c>
+      <c r="E1646">
+        <v>1</v>
+      </c>
+      <c r="G1646" s="94" t="str">
+        <f t="shared" si="23"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1646" s="103"/>
+    </row>
+    <row r="1647" spans="1:8" ht="15">
+      <c r="A1647" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1647,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1647" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1647,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1647" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1647">
+        <v>1649</v>
+      </c>
+      <c r="E1647">
+        <v>1</v>
+      </c>
+      <c r="G1647" s="94" t="str">
+        <f t="shared" si="23"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1647" s="103"/>
+    </row>
+    <row r="1648" spans="1:8" ht="15">
+      <c r="A1648" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1648,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1648" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1648,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1648" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1648">
+        <v>1650</v>
+      </c>
+      <c r="E1648">
+        <v>1</v>
+      </c>
+      <c r="G1648" s="94" t="str">
+        <f t="shared" si="23"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1648" s="103"/>
+    </row>
+    <row r="1649" spans="1:8" ht="15">
+      <c r="A1649" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1649,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1649" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1649,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1649" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1649">
+        <v>1651</v>
+      </c>
+      <c r="E1649">
+        <v>1</v>
+      </c>
+      <c r="G1649" s="94" t="str">
+        <f t="shared" si="23"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1649" s="103"/>
+    </row>
+    <row r="1650" spans="1:8" ht="15">
+      <c r="A1650" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1650,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1650" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1650,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1650" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1650">
+        <v>1652</v>
+      </c>
+      <c r="E1650">
+        <v>1</v>
+      </c>
+      <c r="G1650" s="94" t="str">
+        <f t="shared" si="23"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1650" s="103"/>
+    </row>
+    <row r="1651" spans="1:8" ht="15">
+      <c r="A1651" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1651,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1651" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1651,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1651" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1651">
+        <v>1653</v>
+      </c>
+      <c r="E1651">
+        <v>1</v>
+      </c>
+      <c r="G1651" s="94" t="str">
+        <f t="shared" si="23"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1651" s="103"/>
+    </row>
+    <row r="1652" spans="1:8" ht="15">
+      <c r="A1652" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1652,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1652" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1652,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1652" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1652">
+        <v>1654</v>
+      </c>
+      <c r="E1652">
+        <v>1</v>
+      </c>
+      <c r="G1652" s="94" t="str">
+        <f t="shared" si="23"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1652" s="103"/>
+    </row>
+    <row r="1653" spans="1:8" ht="15">
+      <c r="A1653" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1653,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1653" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1653,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1653" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1653">
+        <v>1655</v>
+      </c>
+      <c r="E1653">
+        <v>1</v>
+      </c>
+      <c r="G1653" s="94" t="str">
+        <f t="shared" si="23"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1653" s="103"/>
+    </row>
+    <row r="1654" spans="1:8" ht="15">
+      <c r="A1654" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1654,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1654" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1654,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1654" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1654">
+        <v>1656</v>
+      </c>
+      <c r="E1654">
+        <v>1</v>
+      </c>
+      <c r="G1654" s="94" t="str">
+        <f t="shared" si="23"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1654" s="103"/>
+    </row>
+    <row r="1655" spans="1:8" ht="15">
+      <c r="A1655" s="98" t="str">
+        <f>+IFERROR(VLOOKUP(B1655,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1655" s="98" t="str">
+        <f>+IFERROR(VLOOKUP(C1655,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1655" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1655">
+        <v>1657</v>
+      </c>
+      <c r="E1655">
+        <v>1</v>
+      </c>
+      <c r="G1655" s="94" t="str">
+        <f t="shared" si="23"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1655" s="103"/>
+    </row>
+    <row r="1656" spans="1:8" ht="15">
+      <c r="A1656" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1656,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1656" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1656,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1656" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1656">
+        <v>1658</v>
+      </c>
+      <c r="E1656">
+        <v>1</v>
+      </c>
+      <c r="G1656" s="94" t="str">
+        <f t="shared" si="23"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1656" s="103"/>
+    </row>
+    <row r="1657" spans="1:8" ht="15">
+      <c r="A1657" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1657,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1657" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1657,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1657" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1657">
+        <v>1659</v>
+      </c>
+      <c r="E1657">
+        <v>1</v>
+      </c>
+      <c r="G1657" s="94" t="str">
+        <f t="shared" si="23"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1657" s="103"/>
+    </row>
+    <row r="1658" spans="1:8" ht="15">
+      <c r="A1658" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1658,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1658" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1658,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1658" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1658">
+        <v>1660</v>
+      </c>
+      <c r="E1658">
+        <v>1</v>
+      </c>
+      <c r="G1658" s="94" t="str">
+        <f t="shared" si="23"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1658" s="103"/>
+    </row>
+    <row r="1659" spans="1:8" ht="15">
+      <c r="A1659" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1659,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1659" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1659,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1659" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1659">
+        <v>1661</v>
+      </c>
+      <c r="E1659">
+        <v>1</v>
+      </c>
+      <c r="G1659" s="94" t="str">
+        <f t="shared" si="23"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1659" s="103"/>
+    </row>
+    <row r="1660" spans="1:8" ht="15">
+      <c r="A1660" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1660,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1660" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1660,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1660" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1660">
+        <v>1662</v>
+      </c>
+      <c r="E1660">
+        <v>1</v>
+      </c>
+      <c r="G1660" s="94" t="str">
+        <f t="shared" si="23"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1660" s="103"/>
+    </row>
+    <row r="1661" spans="1:8" ht="15">
+      <c r="A1661" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1661,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1661" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1661,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1661" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1661">
+        <v>1663</v>
+      </c>
+      <c r="E1661">
+        <v>1</v>
+      </c>
+      <c r="G1661" s="94" t="str">
+        <f t="shared" si="23"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1661" s="103"/>
+    </row>
+    <row r="1662" spans="1:8" ht="15">
+      <c r="A1662" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1662,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1662" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1662,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1662" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1662">
+        <v>1664</v>
+      </c>
+      <c r="E1662">
+        <v>1</v>
+      </c>
+      <c r="G1662" s="94" t="str">
+        <f t="shared" si="23"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1662" s="103"/>
+    </row>
+    <row r="1663" spans="1:8" ht="15">
+      <c r="A1663" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1663,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1663" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1663,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1663" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1663">
+        <v>1665</v>
+      </c>
+      <c r="E1663">
+        <v>1</v>
+      </c>
+      <c r="G1663" s="94" t="str">
+        <f t="shared" si="23"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1663" s="103"/>
+    </row>
+    <row r="1664" spans="1:8" ht="15">
+      <c r="A1664" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1664,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1664" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1664,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1664" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1664">
+        <v>1666</v>
+      </c>
+      <c r="E1664">
+        <v>1</v>
+      </c>
+      <c r="G1664" s="94" t="str">
+        <f t="shared" si="23"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1664" s="103"/>
+    </row>
+    <row r="1665" spans="1:8" ht="15">
+      <c r="A1665" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1665,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1665" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1665,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1665" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1665">
+        <v>1667</v>
+      </c>
+      <c r="E1665">
+        <v>1</v>
+      </c>
+      <c r="G1665" s="94" t="str">
+        <f t="shared" si="23"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1665" s="103"/>
+    </row>
+    <row r="1666" spans="1:8" ht="15">
+      <c r="A1666" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1666,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1666" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1666,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1666" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1666">
+        <v>1668</v>
+      </c>
+      <c r="E1666">
+        <v>1</v>
+      </c>
+      <c r="G1666" s="94" t="str">
+        <f t="shared" si="23"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1666" s="103"/>
+    </row>
+    <row r="1667" spans="1:8" ht="15">
+      <c r="A1667" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1667,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1667" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1667,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1667" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1667">
+        <v>1669</v>
+      </c>
+      <c r="E1667">
+        <v>1</v>
+      </c>
+      <c r="G1667" s="94" t="str">
+        <f t="shared" si="23"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1667" s="103"/>
+    </row>
+    <row r="1668" spans="1:8" ht="15">
+      <c r="A1668" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1668,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1668" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1668,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1668" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1668">
+        <v>1670</v>
+      </c>
+      <c r="E1668">
+        <v>1</v>
+      </c>
+      <c r="G1668" s="94" t="str">
+        <f t="shared" si="23"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1668" s="103"/>
+    </row>
+    <row r="1669" spans="1:8" ht="15">
+      <c r="A1669" s="98" t="str">
+        <f>+IFERROR(VLOOKUP(B1669,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1669" s="98" t="str">
+        <f>+IFERROR(VLOOKUP(C1669,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1669" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1669">
+        <v>1671</v>
+      </c>
+      <c r="E1669">
+        <v>1</v>
+      </c>
+      <c r="G1669" s="94" t="str">
+        <f t="shared" si="23"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1669" s="103"/>
+    </row>
+    <row r="1670" spans="1:8" ht="15">
+      <c r="A1670" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1670,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1670" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1670,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1670" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1670">
+        <v>1672</v>
+      </c>
+      <c r="E1670">
+        <v>1</v>
+      </c>
+      <c r="G1670" s="94" t="str">
+        <f t="shared" si="23"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1670" s="103"/>
+    </row>
+    <row r="1671" spans="1:8" ht="15">
+      <c r="A1671" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1671,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1671" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1671,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1671" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1671">
+        <v>1673</v>
+      </c>
+      <c r="E1671">
+        <v>1</v>
+      </c>
+      <c r="G1671" s="94" t="str">
+        <f t="shared" si="23"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1671" s="103"/>
+    </row>
+    <row r="1672" spans="1:8" ht="15">
+      <c r="A1672" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1672,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1672" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1672,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1672" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1672">
+        <v>1674</v>
+      </c>
+      <c r="E1672">
+        <v>1</v>
+      </c>
+      <c r="G1672" s="94" t="str">
+        <f t="shared" si="23"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1672" s="103"/>
+    </row>
+    <row r="1673" spans="1:8" ht="15">
+      <c r="A1673" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1673,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1673" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1673,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1673" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1673">
+        <v>1675</v>
+      </c>
+      <c r="E1673">
+        <v>1</v>
+      </c>
+      <c r="G1673" s="94" t="str">
+        <f t="shared" si="23"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1673" s="103"/>
+    </row>
+    <row r="1674" spans="1:8" ht="15">
+      <c r="A1674" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1674,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1674" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1674,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1674" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1674">
+        <v>1676</v>
+      </c>
+      <c r="E1674">
+        <v>1</v>
+      </c>
+      <c r="G1674" s="94" t="str">
+        <f t="shared" si="23"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1674" s="103"/>
+    </row>
+    <row r="1675" spans="1:8" ht="15">
+      <c r="A1675" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1675,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1675" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1675,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1675" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1675">
+        <v>1677</v>
+      </c>
+      <c r="E1675">
+        <v>1</v>
+      </c>
+      <c r="G1675" s="94" t="str">
+        <f t="shared" si="23"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1675" s="103"/>
+    </row>
+    <row r="1676" spans="1:8" ht="15">
+      <c r="A1676" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1676,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1676" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1676,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1676" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1676">
+        <v>1678</v>
+      </c>
+      <c r="E1676">
+        <v>1</v>
+      </c>
+      <c r="G1676" s="94" t="str">
+        <f t="shared" si="23"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1676" s="103"/>
+    </row>
+    <row r="1677" spans="1:8" ht="15">
+      <c r="A1677" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1677,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1677" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1677,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1677" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1677">
+        <v>1679</v>
+      </c>
+      <c r="E1677">
+        <v>1</v>
+      </c>
+      <c r="G1677" s="94" t="str">
+        <f t="shared" ref="G1677:G1740" si="24">+IF(E1677=1,"Masculino","Femenino")</f>
+        <v>Masculino</v>
+      </c>
+      <c r="H1677" s="103"/>
+    </row>
+    <row r="1678" spans="1:8" ht="15">
+      <c r="A1678" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1678,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1678" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1678,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1678" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1678">
+        <v>1680</v>
+      </c>
+      <c r="E1678">
+        <v>1</v>
+      </c>
+      <c r="G1678" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1678" s="103"/>
+    </row>
+    <row r="1679" spans="1:8" ht="15">
+      <c r="A1679" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1679,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1679" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1679,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1679" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1679">
+        <v>1681</v>
+      </c>
+      <c r="E1679">
+        <v>1</v>
+      </c>
+      <c r="G1679" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1679" s="103"/>
+    </row>
+    <row r="1680" spans="1:8" ht="15">
+      <c r="A1680" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1680,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1680" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1680,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1680" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1680">
+        <v>1682</v>
+      </c>
+      <c r="E1680">
+        <v>1</v>
+      </c>
+      <c r="G1680" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1680" s="103"/>
+    </row>
+    <row r="1681" spans="1:8" ht="15">
+      <c r="A1681" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1681,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1681" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1681,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1681" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1681">
+        <v>1683</v>
+      </c>
+      <c r="E1681">
+        <v>1</v>
+      </c>
+      <c r="G1681" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1681" s="103"/>
+    </row>
+    <row r="1682" spans="1:8" ht="15">
+      <c r="A1682" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1682,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1682" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1682,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1682" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1682">
+        <v>1684</v>
+      </c>
+      <c r="E1682">
+        <v>1</v>
+      </c>
+      <c r="G1682" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1682" s="103"/>
+    </row>
+    <row r="1683" spans="1:8" ht="15">
+      <c r="A1683" s="98" t="str">
+        <f>+IFERROR(VLOOKUP(B1683,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1683" s="98" t="str">
+        <f>+IFERROR(VLOOKUP(C1683,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1683" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1683">
+        <v>1685</v>
+      </c>
+      <c r="E1683">
+        <v>1</v>
+      </c>
+      <c r="G1683" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1683" s="103"/>
+    </row>
+    <row r="1684" spans="1:8" ht="15">
+      <c r="A1684" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1684,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1684" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1684,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1684" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1684">
+        <v>1686</v>
+      </c>
+      <c r="E1684">
+        <v>1</v>
+      </c>
+      <c r="G1684" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1684" s="103"/>
+    </row>
+    <row r="1685" spans="1:8" ht="15">
+      <c r="A1685" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1685,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1685" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1685,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1685" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1685">
+        <v>1687</v>
+      </c>
+      <c r="E1685">
+        <v>1</v>
+      </c>
+      <c r="G1685" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1685" s="103"/>
+    </row>
+    <row r="1686" spans="1:8" ht="15">
+      <c r="A1686" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1686,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1686" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1686,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1686" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1686">
+        <v>1688</v>
+      </c>
+      <c r="E1686">
+        <v>1</v>
+      </c>
+      <c r="G1686" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1686" s="103"/>
+    </row>
+    <row r="1687" spans="1:8" ht="15">
+      <c r="A1687" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1687,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1687" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1687,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1687" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1687">
+        <v>1689</v>
+      </c>
+      <c r="E1687">
+        <v>1</v>
+      </c>
+      <c r="G1687" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1687" s="103"/>
+    </row>
+    <row r="1688" spans="1:8" ht="15">
+      <c r="A1688" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1688,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1688" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1688,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1688" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1688">
+        <v>1690</v>
+      </c>
+      <c r="E1688">
+        <v>1</v>
+      </c>
+      <c r="G1688" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1688" s="103"/>
+    </row>
+    <row r="1689" spans="1:8" ht="15">
+      <c r="A1689" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1689,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1689" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1689,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1689" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1689">
+        <v>1691</v>
+      </c>
+      <c r="E1689">
+        <v>1</v>
+      </c>
+      <c r="G1689" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1689" s="103"/>
+    </row>
+    <row r="1690" spans="1:8" ht="15">
+      <c r="A1690" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1690,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1690" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1690,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1690" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1690">
+        <v>1692</v>
+      </c>
+      <c r="E1690">
+        <v>1</v>
+      </c>
+      <c r="G1690" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1690" s="103"/>
+    </row>
+    <row r="1691" spans="1:8" ht="15">
+      <c r="A1691" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1691,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1691" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1691,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1691" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1691">
+        <v>1693</v>
+      </c>
+      <c r="E1691">
+        <v>1</v>
+      </c>
+      <c r="G1691" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1691" s="103"/>
+    </row>
+    <row r="1692" spans="1:8" ht="15">
+      <c r="A1692" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1692,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1692" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1692,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1692" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1692">
+        <v>1694</v>
+      </c>
+      <c r="E1692">
+        <v>1</v>
+      </c>
+      <c r="G1692" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1692" s="103"/>
+    </row>
+    <row r="1693" spans="1:8" ht="15">
+      <c r="A1693" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1693,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1693" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1693,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1693" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1693">
+        <v>1695</v>
+      </c>
+      <c r="E1693">
+        <v>1</v>
+      </c>
+      <c r="G1693" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1693" s="103"/>
+    </row>
+    <row r="1694" spans="1:8" ht="15">
+      <c r="A1694" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1694,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1694" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1694,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1694" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1694">
+        <v>1696</v>
+      </c>
+      <c r="E1694">
+        <v>1</v>
+      </c>
+      <c r="G1694" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1694" s="103"/>
+    </row>
+    <row r="1695" spans="1:8" ht="15">
+      <c r="A1695" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1695,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1695" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1695,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1695" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1695">
+        <v>1697</v>
+      </c>
+      <c r="E1695">
+        <v>1</v>
+      </c>
+      <c r="G1695" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1695" s="103"/>
+    </row>
+    <row r="1696" spans="1:8" ht="15">
+      <c r="A1696" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1696,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1696" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1696,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1696" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1696">
+        <v>1698</v>
+      </c>
+      <c r="E1696">
+        <v>1</v>
+      </c>
+      <c r="G1696" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1696" s="103"/>
+    </row>
+    <row r="1697" spans="1:8" ht="15">
+      <c r="A1697" s="98" t="str">
+        <f>+IFERROR(VLOOKUP(B1697,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1697" s="98" t="str">
+        <f>+IFERROR(VLOOKUP(C1697,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1697" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1697">
+        <v>1699</v>
+      </c>
+      <c r="E1697">
+        <v>1</v>
+      </c>
+      <c r="G1697" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1697" s="103"/>
+    </row>
+    <row r="1698" spans="1:8" ht="15">
+      <c r="A1698" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1698,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1698" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1698,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1698" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1698">
+        <v>1700</v>
+      </c>
+      <c r="E1698">
+        <v>1</v>
+      </c>
+      <c r="G1698" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1698" s="103"/>
+    </row>
+    <row r="1699" spans="1:8" ht="15">
+      <c r="A1699" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1699,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1699" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1699,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1699" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1699">
+        <v>1701</v>
+      </c>
+      <c r="E1699">
+        <v>1</v>
+      </c>
+      <c r="G1699" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1699" s="103"/>
+    </row>
+    <row r="1700" spans="1:8" ht="15">
+      <c r="A1700" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1700,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1700" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1700,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1700" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1700">
+        <v>1702</v>
+      </c>
+      <c r="E1700">
+        <v>1</v>
+      </c>
+      <c r="G1700" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1700" s="103"/>
+    </row>
+    <row r="1701" spans="1:8" ht="15">
+      <c r="A1701" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1701,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1701" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1701,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1701" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1701">
+        <v>1703</v>
+      </c>
+      <c r="E1701">
+        <v>1</v>
+      </c>
+      <c r="G1701" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1701" s="103"/>
+    </row>
+    <row r="1702" spans="1:8" ht="15">
+      <c r="A1702" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1702,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1702" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1702,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1702" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1702">
+        <v>1704</v>
+      </c>
+      <c r="E1702">
+        <v>1</v>
+      </c>
+      <c r="G1702" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1702" s="103"/>
+    </row>
+    <row r="1703" spans="1:8" ht="15">
+      <c r="A1703" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1703,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1703" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1703,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1703" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1703">
+        <v>1705</v>
+      </c>
+      <c r="E1703">
+        <v>1</v>
+      </c>
+      <c r="G1703" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1703" s="103"/>
+    </row>
+    <row r="1704" spans="1:8" ht="15">
+      <c r="A1704" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1704,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1704" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1704,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1704" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1704">
+        <v>1706</v>
+      </c>
+      <c r="E1704">
+        <v>1</v>
+      </c>
+      <c r="G1704" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1704" s="103"/>
+    </row>
+    <row r="1705" spans="1:8" ht="15">
+      <c r="A1705" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1705,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1705" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1705,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1705" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1705">
+        <v>1707</v>
+      </c>
+      <c r="E1705">
+        <v>1</v>
+      </c>
+      <c r="G1705" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1705" s="103"/>
+    </row>
+    <row r="1706" spans="1:8" ht="15">
+      <c r="A1706" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1706,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1706" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1706,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1706" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1706">
+        <v>1708</v>
+      </c>
+      <c r="E1706">
+        <v>1</v>
+      </c>
+      <c r="G1706" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1706" s="103"/>
+    </row>
+    <row r="1707" spans="1:8" ht="15">
+      <c r="A1707" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1707,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1707" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1707,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1707" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1707">
+        <v>1709</v>
+      </c>
+      <c r="E1707">
+        <v>1</v>
+      </c>
+      <c r="G1707" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1707" s="103"/>
+    </row>
+    <row r="1708" spans="1:8" ht="15">
+      <c r="A1708" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1708,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1708" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1708,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1708" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1708">
+        <v>1710</v>
+      </c>
+      <c r="E1708">
+        <v>1</v>
+      </c>
+      <c r="G1708" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1708" s="103"/>
+    </row>
+    <row r="1709" spans="1:8" ht="15">
+      <c r="A1709" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1709,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1709" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1709,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1709" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1709">
+        <v>1711</v>
+      </c>
+      <c r="E1709">
+        <v>1</v>
+      </c>
+      <c r="G1709" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1709" s="103"/>
+    </row>
+    <row r="1710" spans="1:8" ht="15">
+      <c r="A1710" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1710,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1710" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1710,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1710" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1710">
+        <v>1712</v>
+      </c>
+      <c r="E1710">
+        <v>1</v>
+      </c>
+      <c r="G1710" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1710" s="103"/>
+    </row>
+    <row r="1711" spans="1:8" ht="15">
+      <c r="A1711" s="98" t="str">
+        <f>+IFERROR(VLOOKUP(B1711,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1711" s="98" t="str">
+        <f>+IFERROR(VLOOKUP(C1711,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1711" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1711">
+        <v>1713</v>
+      </c>
+      <c r="E1711">
+        <v>1</v>
+      </c>
+      <c r="G1711" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1711" s="103"/>
+    </row>
+    <row r="1712" spans="1:8" ht="15">
+      <c r="A1712" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1712,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1712" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1712,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1712" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1712">
+        <v>1714</v>
+      </c>
+      <c r="E1712">
+        <v>1</v>
+      </c>
+      <c r="G1712" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1712" s="103"/>
+    </row>
+    <row r="1713" spans="1:8" ht="15">
+      <c r="A1713" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1713,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1713" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1713,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1713" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1713">
+        <v>1715</v>
+      </c>
+      <c r="E1713">
+        <v>1</v>
+      </c>
+      <c r="G1713" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1713" s="103"/>
+    </row>
+    <row r="1714" spans="1:8" ht="15">
+      <c r="A1714" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1714,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1714" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1714,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1714" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1714">
+        <v>1716</v>
+      </c>
+      <c r="E1714">
+        <v>1</v>
+      </c>
+      <c r="G1714" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1714" s="103"/>
+    </row>
+    <row r="1715" spans="1:8" ht="15">
+      <c r="A1715" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1715,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1715" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1715,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1715" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1715">
+        <v>1717</v>
+      </c>
+      <c r="E1715">
+        <v>1</v>
+      </c>
+      <c r="G1715" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1715" s="103"/>
+    </row>
+    <row r="1716" spans="1:8" ht="15">
+      <c r="A1716" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1716,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1716" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1716,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1716" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1716">
+        <v>1718</v>
+      </c>
+      <c r="E1716">
+        <v>1</v>
+      </c>
+      <c r="G1716" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1716" s="103"/>
+    </row>
+    <row r="1717" spans="1:8" ht="15">
+      <c r="A1717" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1717,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1717" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1717,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1717" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1717">
+        <v>1719</v>
+      </c>
+      <c r="E1717">
+        <v>1</v>
+      </c>
+      <c r="G1717" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1717" s="103"/>
+    </row>
+    <row r="1718" spans="1:8" ht="15">
+      <c r="A1718" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1718,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1718" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1718,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1718" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1718">
+        <v>1720</v>
+      </c>
+      <c r="E1718">
+        <v>1</v>
+      </c>
+      <c r="G1718" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1718" s="103"/>
+    </row>
+    <row r="1719" spans="1:8" ht="15">
+      <c r="A1719" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1719,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1719" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1719,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1719" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1719">
+        <v>1721</v>
+      </c>
+      <c r="E1719">
+        <v>1</v>
+      </c>
+      <c r="G1719" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1719" s="103"/>
+    </row>
+    <row r="1720" spans="1:8" ht="15">
+      <c r="A1720" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1720,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1720" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1720,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1720" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1720">
+        <v>1722</v>
+      </c>
+      <c r="E1720">
+        <v>1</v>
+      </c>
+      <c r="G1720" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1720" s="103"/>
+    </row>
+    <row r="1721" spans="1:8" ht="15">
+      <c r="A1721" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1721,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1721" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1721,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1721" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1721">
+        <v>1723</v>
+      </c>
+      <c r="E1721">
+        <v>1</v>
+      </c>
+      <c r="G1721" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1721" s="103"/>
+    </row>
+    <row r="1722" spans="1:8" ht="15">
+      <c r="A1722" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1722,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1722" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1722,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1722" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1722">
+        <v>1724</v>
+      </c>
+      <c r="E1722">
+        <v>1</v>
+      </c>
+      <c r="G1722" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1722" s="103"/>
+    </row>
+    <row r="1723" spans="1:8" ht="15">
+      <c r="A1723" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1723,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1723" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1723,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1723" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1723">
+        <v>1725</v>
+      </c>
+      <c r="E1723">
+        <v>1</v>
+      </c>
+      <c r="G1723" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1723" s="103"/>
+    </row>
+    <row r="1724" spans="1:8" ht="15">
+      <c r="A1724" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1724,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1724" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1724,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1724" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1724">
+        <v>1726</v>
+      </c>
+      <c r="E1724">
+        <v>1</v>
+      </c>
+      <c r="G1724" s="94" t="str">
+        <f t="shared" si="24"/>
+        <v>Masculino</v>
+      </c>
+      <c r="H1724" s="103"/>
+    </row>
+    <row r="1725" spans="1:8" ht="15">
+      <c r="A1725" s="98" t="str">
+        <f>+IFERROR(VLOOKUP(B1725,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1725" s="98" t="str">
+        <f>+IFERROR(VLOOKUP(C1725,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1725" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1725">
+        <v>1727</v>
+      </c>
+      <c r="F1725">
+        <v>1</v>
+      </c>
+      <c r="G1725" s="95" t="str">
+        <f t="shared" si="24"/>
+        <v>Femenino</v>
+      </c>
+      <c r="H1725" s="103"/>
+    </row>
+    <row r="1726" spans="1:8" ht="15">
+      <c r="A1726" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1726,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1726" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1726,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1726" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1726">
+        <v>1728</v>
+      </c>
+      <c r="F1726">
+        <v>1</v>
+      </c>
+      <c r="G1726" s="95" t="str">
+        <f t="shared" si="24"/>
+        <v>Femenino</v>
+      </c>
+      <c r="H1726" s="103"/>
+    </row>
+    <row r="1727" spans="1:8" ht="15">
+      <c r="A1727" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1727,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1727" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1727,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1727" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1727">
+        <v>1729</v>
+      </c>
+      <c r="F1727">
+        <v>1</v>
+      </c>
+      <c r="G1727" s="95" t="str">
+        <f t="shared" si="24"/>
+        <v>Femenino</v>
+      </c>
+      <c r="H1727" s="103"/>
+    </row>
+    <row r="1728" spans="1:8" ht="15">
+      <c r="A1728" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1728,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1728" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1728,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1728" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1728">
+        <v>1730</v>
+      </c>
+      <c r="F1728">
+        <v>1</v>
+      </c>
+      <c r="G1728" s="95" t="str">
+        <f t="shared" si="24"/>
+        <v>Femenino</v>
+      </c>
+      <c r="H1728" s="103"/>
+    </row>
+    <row r="1729" spans="1:8" ht="15">
+      <c r="A1729" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1729,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1729" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1729,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1729" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1729">
+        <v>1731</v>
+      </c>
+      <c r="F1729">
+        <v>1</v>
+      </c>
+      <c r="G1729" s="95" t="str">
+        <f t="shared" si="24"/>
+        <v>Femenino</v>
+      </c>
+      <c r="H1729" s="103"/>
+    </row>
+    <row r="1730" spans="1:8" ht="15">
+      <c r="A1730" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1730,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1730" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1730,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1730" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1730">
+        <v>1732</v>
+      </c>
+      <c r="F1730">
+        <v>1</v>
+      </c>
+      <c r="G1730" s="95" t="str">
+        <f t="shared" si="24"/>
+        <v>Femenino</v>
+      </c>
+      <c r="H1730" s="103"/>
+    </row>
+    <row r="1731" spans="1:8" ht="15">
+      <c r="A1731" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1731,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1731" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1731,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1731" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1731">
+        <v>1733</v>
+      </c>
+      <c r="F1731">
+        <v>1</v>
+      </c>
+      <c r="G1731" s="95" t="str">
+        <f t="shared" si="24"/>
+        <v>Femenino</v>
+      </c>
+      <c r="H1731" s="103"/>
+    </row>
+    <row r="1732" spans="1:8" ht="15">
+      <c r="A1732" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1732,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1732" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1732,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1732" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1732">
+        <v>1734</v>
+      </c>
+      <c r="F1732">
+        <v>1</v>
+      </c>
+      <c r="G1732" s="95" t="str">
+        <f t="shared" si="24"/>
+        <v>Femenino</v>
+      </c>
+      <c r="H1732" s="103"/>
+    </row>
+    <row r="1733" spans="1:8" ht="15">
+      <c r="A1733" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1733,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1733" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1733,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1733" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1733">
+        <v>1735</v>
+      </c>
+      <c r="F1733">
+        <v>1</v>
+      </c>
+      <c r="G1733" s="95" t="str">
+        <f t="shared" si="24"/>
+        <v>Femenino</v>
+      </c>
+      <c r="H1733" s="103"/>
+    </row>
+    <row r="1734" spans="1:8" ht="15">
+      <c r="A1734" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1734,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1734" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1734,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1734" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1734">
+        <v>1736</v>
+      </c>
+      <c r="F1734">
+        <v>1</v>
+      </c>
+      <c r="G1734" s="95" t="str">
+        <f t="shared" si="24"/>
+        <v>Femenino</v>
+      </c>
+      <c r="H1734" s="103"/>
+    </row>
+    <row r="1735" spans="1:8" ht="15">
+      <c r="A1735" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1735,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1735" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1735,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1735" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1735">
+        <v>1737</v>
+      </c>
+      <c r="F1735">
+        <v>1</v>
+      </c>
+      <c r="G1735" s="95" t="str">
+        <f t="shared" si="24"/>
+        <v>Femenino</v>
+      </c>
+      <c r="H1735" s="103"/>
+    </row>
+    <row r="1736" spans="1:8" ht="15">
+      <c r="A1736" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1736,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1736" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1736,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1736" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1736">
+        <v>1738</v>
+      </c>
+      <c r="F1736">
+        <v>1</v>
+      </c>
+      <c r="G1736" s="95" t="str">
+        <f t="shared" si="24"/>
+        <v>Femenino</v>
+      </c>
+      <c r="H1736" s="103"/>
+    </row>
+    <row r="1737" spans="1:8" ht="15">
+      <c r="A1737" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1737,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1737" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1737,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1737" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1737">
+        <v>1739</v>
+      </c>
+      <c r="F1737">
+        <v>1</v>
+      </c>
+      <c r="G1737" s="95" t="str">
+        <f t="shared" si="24"/>
+        <v>Femenino</v>
+      </c>
+      <c r="H1737" s="103"/>
+    </row>
+    <row r="1738" spans="1:8" ht="15">
+      <c r="A1738" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1738,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1738" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1738,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1738" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1738">
+        <v>1740</v>
+      </c>
+      <c r="F1738">
+        <v>1</v>
+      </c>
+      <c r="G1738" s="95" t="str">
+        <f t="shared" si="24"/>
+        <v>Femenino</v>
+      </c>
+      <c r="H1738" s="103"/>
+    </row>
+    <row r="1739" spans="1:8" ht="15">
+      <c r="A1739" s="98" t="str">
+        <f>+IFERROR(VLOOKUP(B1739,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1739" s="98" t="str">
+        <f>+IFERROR(VLOOKUP(C1739,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1739" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1739">
+        <v>1741</v>
+      </c>
+      <c r="F1739">
+        <v>1</v>
+      </c>
+      <c r="G1739" s="95" t="str">
+        <f t="shared" si="24"/>
+        <v>Femenino</v>
+      </c>
+      <c r="H1739" s="103"/>
+    </row>
+    <row r="1740" spans="1:8" ht="15">
+      <c r="A1740" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1740,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1740" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1740,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1740" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1740">
+        <v>1742</v>
+      </c>
+      <c r="F1740">
+        <v>1</v>
+      </c>
+      <c r="G1740" s="95" t="str">
+        <f t="shared" si="24"/>
+        <v>Femenino</v>
+      </c>
+      <c r="H1740" s="103"/>
+    </row>
+    <row r="1741" spans="1:8" ht="15">
+      <c r="A1741" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1741,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1741" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1741,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1741" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1741">
+        <v>1743</v>
+      </c>
+      <c r="F1741">
+        <v>1</v>
+      </c>
+      <c r="G1741" s="95" t="str">
+        <f t="shared" ref="G1741:G1761" si="25">+IF(E1741=1,"Masculino","Femenino")</f>
+        <v>Femenino</v>
+      </c>
+      <c r="H1741" s="103"/>
+    </row>
+    <row r="1742" spans="1:8" ht="15">
+      <c r="A1742" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1742,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1742" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1742,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1742" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1742">
+        <v>1744</v>
+      </c>
+      <c r="F1742">
+        <v>1</v>
+      </c>
+      <c r="G1742" s="95" t="str">
+        <f t="shared" si="25"/>
+        <v>Femenino</v>
+      </c>
+      <c r="H1742" s="103"/>
+    </row>
+    <row r="1743" spans="1:8" ht="15">
+      <c r="A1743" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1743,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1743" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1743,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1743" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1743">
+        <v>1745</v>
+      </c>
+      <c r="F1743">
+        <v>1</v>
+      </c>
+      <c r="G1743" s="95" t="str">
+        <f t="shared" si="25"/>
+        <v>Femenino</v>
+      </c>
+      <c r="H1743" s="103"/>
+    </row>
+    <row r="1744" spans="1:8" ht="15">
+      <c r="A1744" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1744,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1744" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1744,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1744" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1744">
+        <v>1746</v>
+      </c>
+      <c r="F1744">
+        <v>1</v>
+      </c>
+      <c r="G1744" s="95" t="str">
+        <f t="shared" si="25"/>
+        <v>Femenino</v>
+      </c>
+      <c r="H1744" s="103"/>
+    </row>
+    <row r="1745" spans="1:8" ht="15">
+      <c r="A1745" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1745,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1745" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1745,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1745" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1745">
+        <v>1747</v>
+      </c>
+      <c r="F1745">
+        <v>1</v>
+      </c>
+      <c r="G1745" s="95" t="str">
+        <f t="shared" si="25"/>
+        <v>Femenino</v>
+      </c>
+      <c r="H1745" s="103"/>
+    </row>
+    <row r="1746" spans="1:8" ht="15">
+      <c r="A1746" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1746,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1746" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1746,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1746" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1746">
+        <v>1748</v>
+      </c>
+      <c r="F1746">
+        <v>1</v>
+      </c>
+      <c r="G1746" s="95" t="str">
+        <f t="shared" si="25"/>
+        <v>Femenino</v>
+      </c>
+      <c r="H1746" s="103"/>
+    </row>
+    <row r="1747" spans="1:8" ht="15">
+      <c r="A1747" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1747,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1747" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1747,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1747" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1747">
+        <v>1749</v>
+      </c>
+      <c r="F1747">
+        <v>1</v>
+      </c>
+      <c r="G1747" s="95" t="str">
+        <f t="shared" si="25"/>
+        <v>Femenino</v>
+      </c>
+      <c r="H1747" s="103"/>
+    </row>
+    <row r="1748" spans="1:8" ht="15">
+      <c r="A1748" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1748,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1748" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1748,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1748" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1748">
+        <v>1750</v>
+      </c>
+      <c r="F1748">
+        <v>1</v>
+      </c>
+      <c r="G1748" s="95" t="str">
+        <f t="shared" si="25"/>
+        <v>Femenino</v>
+      </c>
+      <c r="H1748" s="103"/>
+    </row>
+    <row r="1749" spans="1:8" ht="15">
+      <c r="A1749" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1749,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1749" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1749,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1749" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1749">
+        <v>1751</v>
+      </c>
+      <c r="F1749">
+        <v>1</v>
+      </c>
+      <c r="G1749" s="95" t="str">
+        <f t="shared" si="25"/>
+        <v>Femenino</v>
+      </c>
+      <c r="H1749" s="103"/>
+    </row>
+    <row r="1750" spans="1:8" ht="15">
+      <c r="A1750" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1750,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1750" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1750,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1750" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1750">
+        <v>1752</v>
+      </c>
+      <c r="F1750">
+        <v>1</v>
+      </c>
+      <c r="G1750" s="95" t="str">
+        <f t="shared" si="25"/>
+        <v>Femenino</v>
+      </c>
+      <c r="H1750" s="103"/>
+    </row>
+    <row r="1751" spans="1:8" ht="15">
+      <c r="A1751" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1751,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1751" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1751,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1751" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1751">
+        <v>1753</v>
+      </c>
+      <c r="F1751">
+        <v>1</v>
+      </c>
+      <c r="G1751" s="95" t="str">
+        <f t="shared" si="25"/>
+        <v>Femenino</v>
+      </c>
+      <c r="H1751" s="103"/>
+    </row>
+    <row r="1752" spans="1:8" ht="15">
+      <c r="A1752" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1752,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1752" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1752,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1752" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1752">
+        <v>1754</v>
+      </c>
+      <c r="F1752">
+        <v>1</v>
+      </c>
+      <c r="G1752" s="95" t="str">
+        <f t="shared" si="25"/>
+        <v>Femenino</v>
+      </c>
+      <c r="H1752" s="103"/>
+    </row>
+    <row r="1753" spans="1:8" ht="15">
+      <c r="A1753" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1753,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1753" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1753,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1753" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1753">
+        <v>1755</v>
+      </c>
+      <c r="F1753">
+        <v>1</v>
+      </c>
+      <c r="G1753" s="95" t="str">
+        <f t="shared" si="25"/>
+        <v>Femenino</v>
+      </c>
+      <c r="H1753" s="103"/>
+    </row>
+    <row r="1754" spans="1:8" ht="15">
+      <c r="A1754" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1754,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1754" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1754,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1754" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1754">
+        <v>1756</v>
+      </c>
+      <c r="F1754">
+        <v>1</v>
+      </c>
+      <c r="G1754" s="95" t="str">
+        <f t="shared" si="25"/>
+        <v>Femenino</v>
+      </c>
+      <c r="H1754" s="103"/>
+    </row>
+    <row r="1755" spans="1:8" ht="15">
+      <c r="A1755" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1755,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1755" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1755,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1755" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1755">
+        <v>1757</v>
+      </c>
+      <c r="F1755">
+        <v>1</v>
+      </c>
+      <c r="G1755" s="95" t="str">
+        <f t="shared" si="25"/>
+        <v>Femenino</v>
+      </c>
+      <c r="H1755" s="103"/>
+    </row>
+    <row r="1756" spans="1:8" ht="15">
+      <c r="A1756" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1756,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1756" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1756,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1756" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1756">
+        <v>1758</v>
+      </c>
+      <c r="F1756">
+        <v>1</v>
+      </c>
+      <c r="G1756" s="95" t="str">
+        <f t="shared" si="25"/>
+        <v>Femenino</v>
+      </c>
+      <c r="H1756" s="103"/>
+    </row>
+    <row r="1757" spans="1:8" ht="15">
+      <c r="A1757" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1757,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1757" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1757,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1757" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1757">
+        <v>1759</v>
+      </c>
+      <c r="F1757">
+        <v>1</v>
+      </c>
+      <c r="G1757" s="95" t="str">
+        <f t="shared" si="25"/>
+        <v>Femenino</v>
+      </c>
+      <c r="H1757" s="103"/>
+    </row>
+    <row r="1758" spans="1:8" ht="15">
+      <c r="A1758" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1758,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1758" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1758,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1758" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1758">
+        <v>1760</v>
+      </c>
+      <c r="F1758">
+        <v>1</v>
+      </c>
+      <c r="G1758" s="95" t="str">
+        <f t="shared" si="25"/>
+        <v>Femenino</v>
+      </c>
+      <c r="H1758" s="103"/>
+    </row>
+    <row r="1759" spans="1:8" ht="15">
+      <c r="A1759" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1759,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1759" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1759,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1759" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1759">
+        <v>1761</v>
+      </c>
+      <c r="F1759">
+        <v>1</v>
+      </c>
+      <c r="G1759" s="95" t="str">
+        <f t="shared" si="25"/>
+        <v>Femenino</v>
+      </c>
+      <c r="H1759" s="103"/>
+    </row>
+    <row r="1760" spans="1:8" ht="15">
+      <c r="A1760" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(B1760,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1760" s="97" t="str">
+        <f>+IFERROR(VLOOKUP(C1760,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1760" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1760">
+        <v>1762</v>
+      </c>
+      <c r="F1760">
+        <v>1</v>
+      </c>
+      <c r="G1760" s="95" t="str">
+        <f t="shared" si="25"/>
+        <v>Femenino</v>
+      </c>
+      <c r="H1760" s="103"/>
+    </row>
+    <row r="1761" spans="1:8" ht="15">
+      <c r="A1761" s="98" t="str">
+        <f>+IFERROR(VLOOKUP(B1761,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="B1761" s="98" t="str">
+        <f>+IFERROR(VLOOKUP(C1761,LOCALIZACION[[Departamento]:[Región COVID]],4,0),"No Informado")</f>
+        <v>No Informado</v>
+      </c>
+      <c r="C1761" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1761">
+        <v>1763</v>
+      </c>
+      <c r="F1761">
+        <v>1</v>
+      </c>
+      <c r="G1761" s="95" t="str">
+        <f t="shared" si="25"/>
+        <v>Femenino</v>
+      </c>
+      <c r="H1761" s="103"/>
+    </row>
+    <row r="1762" spans="1:8">
+      <c r="H1762" s="103"/>
+    </row>
+    <row r="1763" spans="1:8">
+      <c r="H1763" s="103"/>
+    </row>
+    <row r="1764" spans="1:8">
+      <c r="H1764" s="103"/>
+    </row>
+    <row r="1765" spans="1:8">
+      <c r="H1765" s="103"/>
+    </row>
+    <row r="1766" spans="1:8">
+      <c r="H1766" s="103"/>
+    </row>
+    <row r="1767" spans="1:8">
+      <c r="H1767" s="103"/>
+    </row>
+    <row r="1768" spans="1:8">
+      <c r="H1768" s="103"/>
+    </row>
+    <row r="1769" spans="1:8">
+      <c r="H1769" s="103"/>
+    </row>
+    <row r="1770" spans="1:8">
+      <c r="H1770" s="103"/>
+    </row>
+    <row r="1771" spans="1:8">
+      <c r="H1771" s="103"/>
+    </row>
+    <row r="1772" spans="1:8">
+      <c r="H1772" s="103"/>
+    </row>
+    <row r="1773" spans="1:8">
+      <c r="H1773" s="103"/>
+    </row>
+    <row r="1774" spans="1:8">
+      <c r="H1774" s="103"/>
+    </row>
+    <row r="1775" spans="1:8">
+      <c r="H1775" s="103"/>
+    </row>
+    <row r="1776" spans="1:8">
+      <c r="H1776" s="103"/>
+    </row>
+    <row r="1777" spans="8:8">
+      <c r="H1777" s="103"/>
+    </row>
+    <row r="1778" spans="8:8">
+      <c r="H1778" s="103"/>
+    </row>
+    <row r="1779" spans="8:8">
+      <c r="H1779" s="103"/>
+    </row>
+    <row r="1780" spans="8:8">
+      <c r="H1780" s="103"/>
+    </row>
+    <row r="1781" spans="8:8">
+      <c r="H1781" s="103"/>
+    </row>
+    <row r="1782" spans="8:8">
+      <c r="H1782" s="103"/>
+    </row>
+    <row r="1783" spans="8:8">
+      <c r="H1783" s="103"/>
+    </row>
+    <row r="1784" spans="8:8">
+      <c r="H1784" s="103"/>
+    </row>
+    <row r="1785" spans="8:8">
+      <c r="H1785" s="103"/>
+    </row>
+    <row r="1786" spans="8:8">
+      <c r="H1786" s="103"/>
+    </row>
+    <row r="1787" spans="8:8">
+      <c r="H1787" s="103"/>
+    </row>
+    <row r="1788" spans="8:8">
+      <c r="H1788" s="103"/>
+    </row>
+    <row r="1789" spans="8:8">
+      <c r="H1789" s="103"/>
+    </row>
+    <row r="1790" spans="8:8">
+      <c r="H1790" s="103"/>
+    </row>
+    <row r="1791" spans="8:8">
+      <c r="H1791" s="103"/>
+    </row>
+    <row r="1792" spans="8:8">
+      <c r="H1792" s="103"/>
+    </row>
+    <row r="1793" spans="8:8">
+      <c r="H1793" s="103"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -71303,7 +74345,7 @@
   <dimension ref="B2:C39"/>
   <sheetViews>
     <sheetView topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -71326,21 +74368,21 @@
       <c r="B5" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="94">
-        <v>1066</v>
+      <c r="C5" s="99">
+        <v>1152</v>
       </c>
     </row>
     <row r="6" spans="2:3">
       <c r="B6" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C6" s="94"/>
+      <c r="C6" s="99"/>
     </row>
     <row r="7" spans="2:3" ht="15" thickBot="1">
       <c r="B7" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="95"/>
+      <c r="C7" s="100"/>
     </row>
     <row r="10" spans="2:3">
       <c r="B10" s="82" t="s">
@@ -71349,40 +74391,38 @@
       <c r="C10" s="83"/>
     </row>
     <row r="11" spans="2:3">
-      <c r="B11" s="84" t="s">
-        <v>814</v>
-      </c>
+      <c r="B11" s="84"/>
       <c r="C11" s="85"/>
     </row>
     <row r="12" spans="2:3">
       <c r="B12" s="84" t="s">
-        <v>138</v>
-      </c>
-      <c r="C12" s="96">
-        <v>184</v>
+        <v>548</v>
+      </c>
+      <c r="C12" s="101">
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="2:3">
       <c r="B13" s="84" t="s">
-        <v>70</v>
-      </c>
-      <c r="C13" s="96"/>
+        <v>72</v>
+      </c>
+      <c r="C13" s="101"/>
     </row>
     <row r="14" spans="2:3">
       <c r="B14" s="84" t="s">
-        <v>845</v>
-      </c>
-      <c r="C14" s="96"/>
+        <v>491</v>
+      </c>
+      <c r="C14" s="101"/>
     </row>
     <row r="15" spans="2:3">
       <c r="B15" s="86" t="s">
-        <v>787</v>
-      </c>
-      <c r="C15" s="97"/>
+        <v>943</v>
+      </c>
+      <c r="C15" s="102"/>
     </row>
     <row r="17" spans="2:3">
       <c r="B17" s="82" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="C17" s="83"/>
     </row>
@@ -71391,34 +74431,36 @@
       <c r="C18" s="85"/>
     </row>
     <row r="19" spans="2:3">
-      <c r="B19" s="87"/>
-      <c r="C19" s="96">
-        <v>166</v>
+      <c r="B19" s="87" t="s">
+        <v>814</v>
+      </c>
+      <c r="C19" s="101">
+        <v>173</v>
       </c>
     </row>
     <row r="20" spans="2:3">
       <c r="B20" s="84" t="s">
-        <v>548</v>
-      </c>
-      <c r="C20" s="96"/>
+        <v>138</v>
+      </c>
+      <c r="C20" s="101"/>
     </row>
     <row r="21" spans="2:3">
       <c r="B21" s="84" t="s">
-        <v>72</v>
-      </c>
-      <c r="C21" s="96"/>
+        <v>70</v>
+      </c>
+      <c r="C21" s="101"/>
     </row>
     <row r="22" spans="2:3">
       <c r="B22" s="84" t="s">
-        <v>491</v>
-      </c>
-      <c r="C22" s="96"/>
+        <v>845</v>
+      </c>
+      <c r="C22" s="101"/>
     </row>
     <row r="23" spans="2:3">
       <c r="B23" s="86" t="s">
-        <v>944</v>
-      </c>
-      <c r="C23" s="97"/>
+        <v>787</v>
+      </c>
+      <c r="C23" s="102"/>
     </row>
     <row r="25" spans="2:3">
       <c r="B25" s="6" t="s">
@@ -71432,35 +74474,35 @@
     </row>
     <row r="27" spans="2:3">
       <c r="B27" s="3" t="s">
-        <v>696</v>
-      </c>
-      <c r="C27" s="94">
-        <v>91</v>
+        <v>232</v>
+      </c>
+      <c r="C27" s="99">
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="2:3">
       <c r="B28" s="3" t="s">
-        <v>674</v>
-      </c>
-      <c r="C28" s="94"/>
+        <v>861</v>
+      </c>
+      <c r="C28" s="99"/>
     </row>
     <row r="29" spans="2:3">
       <c r="B29" s="3" t="s">
-        <v>742</v>
-      </c>
-      <c r="C29" s="94"/>
+        <v>69</v>
+      </c>
+      <c r="C29" s="99"/>
     </row>
     <row r="30" spans="2:3">
       <c r="B30" s="3" t="s">
-        <v>622</v>
-      </c>
-      <c r="C30" s="94"/>
+        <v>73</v>
+      </c>
+      <c r="C30" s="99"/>
     </row>
     <row r="31" spans="2:3" ht="15" thickBot="1">
       <c r="B31" s="5" t="s">
-        <v>300</v>
-      </c>
-      <c r="C31" s="95"/>
+        <v>470</v>
+      </c>
+      <c r="C31" s="100"/>
     </row>
     <row r="32" spans="2:3" ht="15" thickBot="1"/>
     <row r="33" spans="2:3">
@@ -71475,35 +74517,35 @@
     </row>
     <row r="35" spans="2:3">
       <c r="B35" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="C35" s="94">
-        <v>136</v>
+        <v>696</v>
+      </c>
+      <c r="C35" s="99">
+        <v>148</v>
       </c>
     </row>
     <row r="36" spans="2:3">
       <c r="B36" s="3" t="s">
-        <v>861</v>
-      </c>
-      <c r="C36" s="94"/>
+        <v>674</v>
+      </c>
+      <c r="C36" s="99"/>
     </row>
     <row r="37" spans="2:3">
       <c r="B37" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C37" s="94"/>
+        <v>742</v>
+      </c>
+      <c r="C37" s="99"/>
     </row>
     <row r="38" spans="2:3">
       <c r="B38" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C38" s="94"/>
+        <v>622</v>
+      </c>
+      <c r="C38" s="99"/>
     </row>
     <row r="39" spans="2:3" ht="15" thickBot="1">
       <c r="B39" s="5" t="s">
-        <v>470</v>
-      </c>
-      <c r="C39" s="95"/>
+        <v>300</v>
+      </c>
+      <c r="C39" s="100"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-18-2020 16-01-26
</commit_message>
<xml_diff>
--- a/datacovidgt/Casos GT v1.xlsx
+++ b/datacovidgt/Casos GT v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID GT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3077" documentId="8_{9F1230D5-64C1-4EE0-9758-3A2331A06A47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DC5FC7FB-95C3-4A3D-AEBB-5FE366D03D02}"/>
+  <xr:revisionPtr revIDLastSave="3086" documentId="8_{9F1230D5-64C1-4EE0-9758-3A2331A06A47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{14E543EE-702F-4DC9-9050-DD357AEA76BD}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4667,8 +4667,9 @@
   </sheetPr>
   <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A46" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7367,7 +7368,10 @@
   </sheetPr>
   <dimension ref="A1:C131"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -8833,8 +8837,9 @@
   </sheetPr>
   <dimension ref="A1:H1910"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1892" workbookViewId="0">
-      <selection activeCell="C1909" sqref="C1909"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A518" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C537" sqref="C537"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10805,7 +10810,7 @@
         <v>72</v>
       </c>
       <c r="C76" s="89">
-        <v>44016</v>
+        <v>43928</v>
       </c>
       <c r="D76">
         <v>75</v>
@@ -10830,8 +10835,8 @@
       <c r="B77" t="s">
         <v>67</v>
       </c>
-      <c r="C77" s="89">
-        <v>44016</v>
+      <c r="C77" s="90">
+        <v>43928</v>
       </c>
       <c r="D77">
         <v>76</v>
@@ -10856,8 +10861,8 @@
       <c r="B78" t="s">
         <v>66</v>
       </c>
-      <c r="C78" s="89">
-        <v>44016</v>
+      <c r="C78" s="90">
+        <v>43928</v>
       </c>
       <c r="D78">
         <v>77</v>
@@ -10882,8 +10887,8 @@
       <c r="B79" t="s">
         <v>71</v>
       </c>
-      <c r="C79" s="89">
-        <v>44016</v>
+      <c r="C79" s="90">
+        <v>43928</v>
       </c>
       <c r="D79">
         <v>78</v>
@@ -10908,8 +10913,8 @@
       <c r="B80" t="s">
         <v>66</v>
       </c>
-      <c r="C80" s="89">
-        <v>44016</v>
+      <c r="C80" s="90">
+        <v>43928</v>
       </c>
       <c r="D80">
         <v>79</v>
@@ -10934,8 +10939,8 @@
       <c r="B81" t="s">
         <v>69</v>
       </c>
-      <c r="C81" s="89">
-        <v>44016</v>
+      <c r="C81" s="90">
+        <v>43928</v>
       </c>
       <c r="D81">
         <v>80</v>
@@ -10961,7 +10966,7 @@
         <v>74</v>
       </c>
       <c r="C82" s="89">
-        <v>44047</v>
+        <v>43929</v>
       </c>
       <c r="D82">
         <v>81</v>
@@ -10986,8 +10991,8 @@
       <c r="B83" t="s">
         <v>74</v>
       </c>
-      <c r="C83" s="89">
-        <v>44047</v>
+      <c r="C83" s="90">
+        <v>43929</v>
       </c>
       <c r="D83">
         <v>82</v>
@@ -11012,8 +11017,8 @@
       <c r="B84" t="s">
         <v>74</v>
       </c>
-      <c r="C84" s="89">
-        <v>44047</v>
+      <c r="C84" s="90">
+        <v>43929</v>
       </c>
       <c r="D84">
         <v>83</v>
@@ -11038,8 +11043,8 @@
       <c r="B85" t="s">
         <v>74</v>
       </c>
-      <c r="C85" s="89">
-        <v>44047</v>
+      <c r="C85" s="90">
+        <v>43929</v>
       </c>
       <c r="D85">
         <v>84</v>
@@ -11064,8 +11069,8 @@
       <c r="B86" t="s">
         <v>74</v>
       </c>
-      <c r="C86" s="89">
-        <v>44047</v>
+      <c r="C86" s="90">
+        <v>43929</v>
       </c>
       <c r="D86">
         <v>85</v>
@@ -11090,8 +11095,8 @@
       <c r="B87" t="s">
         <v>74</v>
       </c>
-      <c r="C87" s="89">
-        <v>44047</v>
+      <c r="C87" s="90">
+        <v>43929</v>
       </c>
       <c r="D87">
         <v>86</v>
@@ -11116,8 +11121,8 @@
       <c r="B88" t="s">
         <v>74</v>
       </c>
-      <c r="C88" s="89">
-        <v>44047</v>
+      <c r="C88" s="90">
+        <v>43929</v>
       </c>
       <c r="D88">
         <v>87</v>
@@ -11142,8 +11147,8 @@
       <c r="B89" t="s">
         <v>74</v>
       </c>
-      <c r="C89" s="89">
-        <v>44078</v>
+      <c r="C89" s="90">
+        <v>43930</v>
       </c>
       <c r="D89">
         <v>88</v>
@@ -11168,8 +11173,8 @@
       <c r="B90" t="s">
         <v>74</v>
       </c>
-      <c r="C90" s="89">
-        <v>44078</v>
+      <c r="C90" s="90">
+        <v>43930</v>
       </c>
       <c r="D90">
         <v>89</v>
@@ -11194,8 +11199,8 @@
       <c r="B91" t="s">
         <v>74</v>
       </c>
-      <c r="C91" s="89">
-        <v>44078</v>
+      <c r="C91" s="90">
+        <v>43930</v>
       </c>
       <c r="D91">
         <v>90</v>
@@ -11220,8 +11225,8 @@
       <c r="B92" t="s">
         <v>74</v>
       </c>
-      <c r="C92" s="89">
-        <v>44078</v>
+      <c r="C92" s="90">
+        <v>43930</v>
       </c>
       <c r="D92">
         <v>91</v>
@@ -11246,8 +11251,8 @@
       <c r="B93" t="s">
         <v>74</v>
       </c>
-      <c r="C93" s="89">
-        <v>44078</v>
+      <c r="C93" s="90">
+        <v>43930</v>
       </c>
       <c r="D93">
         <v>92</v>
@@ -11272,8 +11277,8 @@
       <c r="B94" t="s">
         <v>74</v>
       </c>
-      <c r="C94" s="89">
-        <v>44078</v>
+      <c r="C94" s="90">
+        <v>43930</v>
       </c>
       <c r="D94">
         <v>93</v>
@@ -11298,8 +11303,8 @@
       <c r="B95" t="s">
         <v>74</v>
       </c>
-      <c r="C95" s="89">
-        <v>44078</v>
+      <c r="C95" s="90">
+        <v>43930</v>
       </c>
       <c r="D95">
         <v>94</v>
@@ -11324,8 +11329,8 @@
       <c r="B96" t="s">
         <v>74</v>
       </c>
-      <c r="C96" s="89">
-        <v>44078</v>
+      <c r="C96" s="90">
+        <v>43930</v>
       </c>
       <c r="D96">
         <v>95</v>
@@ -11350,8 +11355,8 @@
       <c r="B97" t="s">
         <v>74</v>
       </c>
-      <c r="C97" s="89">
-        <v>44078</v>
+      <c r="C97" s="90">
+        <v>43930</v>
       </c>
       <c r="D97">
         <v>96</v>
@@ -11376,8 +11381,8 @@
       <c r="B98" t="s">
         <v>74</v>
       </c>
-      <c r="C98" s="89">
-        <v>44078</v>
+      <c r="C98" s="90">
+        <v>43930</v>
       </c>
       <c r="D98">
         <v>97</v>
@@ -11402,8 +11407,8 @@
       <c r="B99" t="s">
         <v>74</v>
       </c>
-      <c r="C99" s="89">
-        <v>44078</v>
+      <c r="C99" s="90">
+        <v>43930</v>
       </c>
       <c r="D99">
         <v>98</v>
@@ -11428,8 +11433,8 @@
       <c r="B100" t="s">
         <v>74</v>
       </c>
-      <c r="C100" s="89">
-        <v>44078</v>
+      <c r="C100" s="90">
+        <v>43930</v>
       </c>
       <c r="D100">
         <v>99</v>
@@ -11454,8 +11459,8 @@
       <c r="B101" t="s">
         <v>74</v>
       </c>
-      <c r="C101" s="89">
-        <v>44078</v>
+      <c r="C101" s="90">
+        <v>43930</v>
       </c>
       <c r="D101">
         <v>100</v>
@@ -11480,8 +11485,8 @@
       <c r="B102" t="s">
         <v>74</v>
       </c>
-      <c r="C102" s="89">
-        <v>44078</v>
+      <c r="C102" s="90">
+        <v>43930</v>
       </c>
       <c r="D102">
         <v>101</v>
@@ -11506,8 +11511,8 @@
       <c r="B103" t="s">
         <v>74</v>
       </c>
-      <c r="C103" s="89">
-        <v>44078</v>
+      <c r="C103" s="90">
+        <v>43930</v>
       </c>
       <c r="D103">
         <v>102</v>
@@ -11532,8 +11537,8 @@
       <c r="B104" t="s">
         <v>74</v>
       </c>
-      <c r="C104" s="89">
-        <v>44078</v>
+      <c r="C104" s="90">
+        <v>43930</v>
       </c>
       <c r="D104">
         <v>103</v>
@@ -11558,8 +11563,8 @@
       <c r="B105" t="s">
         <v>74</v>
       </c>
-      <c r="C105" s="89">
-        <v>44078</v>
+      <c r="C105" s="90">
+        <v>43930</v>
       </c>
       <c r="D105">
         <v>104</v>
@@ -11584,8 +11589,8 @@
       <c r="B106" t="s">
         <v>74</v>
       </c>
-      <c r="C106" s="89">
-        <v>44078</v>
+      <c r="C106" s="90">
+        <v>43930</v>
       </c>
       <c r="D106">
         <v>105</v>
@@ -11610,8 +11615,8 @@
       <c r="B107" t="s">
         <v>74</v>
       </c>
-      <c r="C107" s="89">
-        <v>44078</v>
+      <c r="C107" s="90">
+        <v>43930</v>
       </c>
       <c r="D107">
         <v>106</v>
@@ -11636,8 +11641,8 @@
       <c r="B108" t="s">
         <v>74</v>
       </c>
-      <c r="C108" s="89">
-        <v>44078</v>
+      <c r="C108" s="90">
+        <v>43930</v>
       </c>
       <c r="D108">
         <v>107</v>
@@ -11662,8 +11667,8 @@
       <c r="B109" t="s">
         <v>74</v>
       </c>
-      <c r="C109" s="89">
-        <v>44078</v>
+      <c r="C109" s="90">
+        <v>43930</v>
       </c>
       <c r="D109">
         <v>108</v>
@@ -11688,8 +11693,8 @@
       <c r="B110" t="s">
         <v>74</v>
       </c>
-      <c r="C110" s="89">
-        <v>44078</v>
+      <c r="C110" s="90">
+        <v>43930</v>
       </c>
       <c r="D110">
         <v>109</v>
@@ -11714,8 +11719,8 @@
       <c r="B111" t="s">
         <v>74</v>
       </c>
-      <c r="C111" s="89">
-        <v>44078</v>
+      <c r="C111" s="90">
+        <v>43930</v>
       </c>
       <c r="D111">
         <v>110</v>
@@ -11740,8 +11745,8 @@
       <c r="B112" t="s">
         <v>74</v>
       </c>
-      <c r="C112" s="89">
-        <v>44078</v>
+      <c r="C112" s="90">
+        <v>43930</v>
       </c>
       <c r="D112">
         <v>111</v>
@@ -11766,8 +11771,8 @@
       <c r="B113" t="s">
         <v>74</v>
       </c>
-      <c r="C113" s="89">
-        <v>44078</v>
+      <c r="C113" s="90">
+        <v>43930</v>
       </c>
       <c r="D113">
         <v>112</v>
@@ -11792,8 +11797,8 @@
       <c r="B114" t="s">
         <v>74</v>
       </c>
-      <c r="C114" s="89">
-        <v>44078</v>
+      <c r="C114" s="90">
+        <v>43930</v>
       </c>
       <c r="D114">
         <v>113</v>
@@ -11818,8 +11823,8 @@
       <c r="B115" t="s">
         <v>74</v>
       </c>
-      <c r="C115" s="89">
-        <v>44078</v>
+      <c r="C115" s="90">
+        <v>43930</v>
       </c>
       <c r="D115">
         <v>114</v>
@@ -11844,8 +11849,8 @@
       <c r="B116" t="s">
         <v>74</v>
       </c>
-      <c r="C116" s="89">
-        <v>44078</v>
+      <c r="C116" s="90">
+        <v>43930</v>
       </c>
       <c r="D116">
         <v>115</v>
@@ -11870,8 +11875,8 @@
       <c r="B117" t="s">
         <v>74</v>
       </c>
-      <c r="C117" s="89">
-        <v>44078</v>
+      <c r="C117" s="90">
+        <v>43930</v>
       </c>
       <c r="D117">
         <v>116</v>
@@ -11896,8 +11901,8 @@
       <c r="B118" t="s">
         <v>74</v>
       </c>
-      <c r="C118" s="89">
-        <v>44078</v>
+      <c r="C118" s="90">
+        <v>43930</v>
       </c>
       <c r="D118">
         <v>117</v>
@@ -11922,8 +11927,8 @@
       <c r="B119" t="s">
         <v>74</v>
       </c>
-      <c r="C119" s="89">
-        <v>44078</v>
+      <c r="C119" s="90">
+        <v>43930</v>
       </c>
       <c r="D119">
         <v>118</v>
@@ -11948,8 +11953,8 @@
       <c r="B120" t="s">
         <v>74</v>
       </c>
-      <c r="C120" s="89">
-        <v>44078</v>
+      <c r="C120" s="90">
+        <v>43930</v>
       </c>
       <c r="D120">
         <v>119</v>
@@ -11974,8 +11979,8 @@
       <c r="B121" t="s">
         <v>74</v>
       </c>
-      <c r="C121" s="89">
-        <v>44078</v>
+      <c r="C121" s="90">
+        <v>43930</v>
       </c>
       <c r="D121">
         <v>120</v>
@@ -12000,8 +12005,8 @@
       <c r="B122" t="s">
         <v>74</v>
       </c>
-      <c r="C122" s="89">
-        <v>44078</v>
+      <c r="C122" s="90">
+        <v>43930</v>
       </c>
       <c r="D122">
         <v>121</v>
@@ -12026,8 +12031,8 @@
       <c r="B123" t="s">
         <v>74</v>
       </c>
-      <c r="C123" s="89">
-        <v>44078</v>
+      <c r="C123" s="90">
+        <v>43930</v>
       </c>
       <c r="D123">
         <v>122</v>
@@ -12052,8 +12057,8 @@
       <c r="B124" t="s">
         <v>74</v>
       </c>
-      <c r="C124" s="89">
-        <v>44078</v>
+      <c r="C124" s="90">
+        <v>43930</v>
       </c>
       <c r="D124">
         <v>123</v>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-19-2020 19-18-37
</commit_message>
<xml_diff>
--- a/datacovidgt/Casos GT v1.xlsx
+++ b/datacovidgt/Casos GT v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID GT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3499" documentId="8_{9F1230D5-64C1-4EE0-9758-3A2331A06A47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BFB97090-A3D7-45AC-B9B6-48B8786C081F}"/>
+  <xr:revisionPtr revIDLastSave="3500" documentId="8_{9F1230D5-64C1-4EE0-9758-3A2331A06A47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7BA53ECE-3057-4851-98F7-C9339495E360}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos Region" sheetId="11" r:id="rId1"/>
@@ -6203,9 +6203,9 @@
   </sheetPr>
   <dimension ref="A1:H2000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A1986" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1993" sqref="C1993"/>
+      <selection pane="bottomLeft" activeCell="D2003" sqref="D2003"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -56411,9 +56411,9 @@
   </sheetPr>
   <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B68" sqref="B68"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G70" sqref="G70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -59038,7 +59038,7 @@
         <v>139</v>
       </c>
       <c r="G68" s="64">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H68" s="60">
         <f>+F68-F67</f>
@@ -59046,7 +59046,7 @@
       </c>
       <c r="I68" s="65">
         <f>+G68-G67</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J68" s="66">
         <v>1824</v>

</xml_diff>